<commit_message>
NOAK numbers for HTSE
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/synfuels_model_numbers.xlsx
+++ b/use_cases/2022_05/data/synfuels_model_numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garrm\projects\FORCE\use_cases\2022_05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CD661BE0-C8C8-48AA-9A51-A25FB46B4D01}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180F1DF0-74D4-440F-A5C7-B0673DB4F99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" firstSheet="1" activeTab="3" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" firstSheet="1" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -40,7 +40,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="199" uniqueCount="98">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
   <si>
     <t>Source</t>
   </si>
@@ -327,20 +327,23 @@
     <t xml:space="preserve"> </t>
   </si>
   <si>
-    <t>kWh/h</t>
-  </si>
-  <si>
-    <t>kWh/day</t>
-  </si>
-  <si>
-    <t>Should be a fixed amount!</t>
+    <t>Fixed no matter production level</t>
+  </si>
+  <si>
+    <t>Modeled as separate electricity consuming component</t>
+  </si>
+  <si>
+    <t>Using NOAK values</t>
+  </si>
+  <si>
+    <t>kg-H2/kWh-e</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="1" x14ac:knownFonts="1">
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -348,13 +351,40 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color rgb="FF006100"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1" tint="0.499984740745262"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="3">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFC6EFCE"/>
+      </patternFill>
     </fill>
   </fills>
   <borders count="1">
@@ -366,18 +396,25 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="4">
+  <cellXfs count="9">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Good" xfId="1" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -847,16 +884,17 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0215393-90AE-4217-9780-C6903F6FBFD3}">
-  <dimension ref="A1:C13"/>
+  <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="A13" sqref="A13"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="27.90625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:3" x14ac:dyDescent="0.35">
@@ -882,7 +920,7 @@
       <c r="A3" t="s">
         <v>25</v>
       </c>
-      <c r="B3">
+      <c r="B3" s="8">
         <v>36.799999999999997</v>
       </c>
       <c r="C3" t="s">
@@ -890,33 +928,31 @@
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>30</v>
-      </c>
-      <c r="B4">
-        <v>6.4</v>
+      <c r="B4" s="8">
+        <f>1/B3</f>
+        <v>2.7173913043478264E-2</v>
       </c>
       <c r="C4" t="s">
-        <v>31</v>
+        <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>36</v>
+        <v>30</v>
       </c>
       <c r="B5">
-        <v>590</v>
+        <v>6.4</v>
       </c>
       <c r="C5" t="s">
-        <v>33</v>
+        <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B6">
-        <v>763</v>
+        <v>590</v>
       </c>
       <c r="C6" t="s">
         <v>33</v>
@@ -924,10 +960,10 @@
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
-        <v>32</v>
+        <v>37</v>
       </c>
       <c r="B7">
-        <v>544</v>
+        <v>763</v>
       </c>
       <c r="C7" t="s">
         <v>33</v>
@@ -935,10 +971,10 @@
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B8">
-        <v>703</v>
+        <v>544</v>
       </c>
       <c r="C8" t="s">
         <v>33</v>
@@ -946,57 +982,73 @@
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
-        <v>38</v>
-      </c>
-      <c r="B9">
-        <v>20</v>
+        <v>35</v>
+      </c>
+      <c r="B9" s="8">
+        <v>703</v>
       </c>
       <c r="C9" t="s">
-        <v>39</v>
+        <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="B10">
-        <v>32.64</v>
+        <v>20</v>
       </c>
       <c r="C10" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
-        <v>42</v>
-      </c>
-      <c r="B11">
-        <v>3.41</v>
+        <v>40</v>
+      </c>
+      <c r="B11" s="8">
+        <v>32.64</v>
       </c>
       <c r="C11" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
-        <v>44</v>
-      </c>
-      <c r="B12">
-        <v>10</v>
+        <v>42</v>
+      </c>
+      <c r="B12" s="8">
+        <v>3.41</v>
       </c>
       <c r="C12" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
+        <v>44</v>
+      </c>
+      <c r="B13">
+        <v>10</v>
+      </c>
+      <c r="C13" t="s">
+        <v>45</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>46</v>
       </c>
-      <c r="B13">
+      <c r="B14" s="8">
         <v>20</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C14" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A16" s="8" t="s">
+        <v>97</v>
       </c>
     </row>
   </sheetData>
@@ -1009,7 +1061,7 @@
   <dimension ref="A1:C11"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+      <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1112,8 +1164,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
   <dimension ref="A1:H15"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="H6" sqref="H6"/>
+    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1122,9 +1174,15 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" t="s">
+      <c r="A1" s="3" t="s">
         <v>61</v>
       </c>
+      <c r="B1" s="3"/>
+      <c r="C1" s="3"/>
+      <c r="D1" s="3"/>
+      <c r="E1" s="3"/>
+      <c r="F1" s="3"/>
+      <c r="G1" s="3"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A2" s="3" t="s">
@@ -1147,14 +1205,14 @@
       <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="2">
+      <c r="D3" s="4">
         <f>B3*1000/(24*3600)</f>
         <v>18.287037037037038</v>
       </c>
-      <c r="E3" t="s">
+      <c r="E3" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="2">
+      <c r="F3" s="6">
         <f>B3*1000/24</f>
         <v>65833.333333333328</v>
       </c>
@@ -1172,14 +1230,14 @@
       <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="2">
+      <c r="D4" s="4">
         <f>B4*1000/(24*3600)</f>
         <v>2.9513888888888888</v>
       </c>
-      <c r="E4" t="s">
+      <c r="E4" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="2">
+      <c r="F4" s="6">
         <f>B4*1000/24</f>
         <v>10625</v>
       </c>
@@ -1197,21 +1255,14 @@
       <c r="C5" t="s">
         <v>66</v>
       </c>
-      <c r="D5" s="2">
-        <v>357600</v>
+      <c r="D5" s="2" t="s">
+        <v>95</v>
       </c>
       <c r="E5" t="s">
         <v>96</v>
       </c>
-      <c r="F5" s="2">
-        <v>14900</v>
-      </c>
-      <c r="G5" t="s">
-        <v>95</v>
-      </c>
-      <c r="H5" s="2" t="s">
-        <v>97</v>
-      </c>
+      <c r="F5" s="2"/>
+      <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="3" t="s">
@@ -1234,14 +1285,14 @@
       <c r="C7" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="2">
+      <c r="D7" s="4">
         <f>B7*1000/(24*3600)</f>
         <v>2.0370370370370372</v>
       </c>
-      <c r="E7" t="s">
+      <c r="E7" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="2">
+      <c r="F7" s="6">
         <f>B7*1000/24</f>
         <v>7333.333333333333</v>
       </c>
@@ -1259,14 +1310,14 @@
       <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="2">
+      <c r="D8" s="4">
         <f t="shared" ref="D8:D9" si="0">B8*1000/(24*3600)</f>
         <v>2.4652777777777777</v>
       </c>
-      <c r="E8" t="s">
+      <c r="E8" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="2">
+      <c r="F8" s="6">
         <f t="shared" ref="F8:F9" si="1">B8*1000/24</f>
         <v>8875</v>
       </c>
@@ -1284,14 +1335,14 @@
       <c r="C9" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="2">
+      <c r="D9" s="4">
         <f t="shared" si="0"/>
         <v>1.3657407407407407</v>
       </c>
-      <c r="E9" t="s">
+      <c r="E9" s="5" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="2">
+      <c r="F9" s="6">
         <f t="shared" si="1"/>
         <v>4916.666666666667</v>
       </c>
@@ -1300,9 +1351,15 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="3" t="s">
         <v>17</v>
       </c>
+      <c r="B11" s="3"/>
+      <c r="C11" s="3"/>
+      <c r="D11" s="3"/>
+      <c r="E11" s="3"/>
+      <c r="F11" s="3"/>
+      <c r="G11" s="3"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A12" s="3" t="s">
@@ -1333,7 +1390,7 @@
       <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="B15">
+      <c r="B15" s="7">
         <f>1/B13</f>
         <v>2.5125628140703519E-2</v>
       </c>
@@ -1342,11 +1399,13 @@
       </c>
     </row>
   </sheetData>
-  <mergeCells count="4">
+  <mergeCells count="6">
     <mergeCell ref="A12:C12"/>
     <mergeCell ref="A14:C14"/>
     <mergeCell ref="A2:G2"/>
     <mergeCell ref="A6:G6"/>
+    <mergeCell ref="A1:G1"/>
+    <mergeCell ref="A11:G11"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>

</xml_diff>

<commit_message>
Add capex, FOM, VOM numbers for FT to spreadsheet
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/synfuels_model_numbers.xlsx
+++ b/use_cases/2022_05/data/synfuels_model_numbers.xlsx
@@ -8,17 +8,18 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garrm\projects\FORCE\use_cases\2022_05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{180F1DF0-74D4-440F-A5C7-B0673DB4F99A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28E3A76-F76C-45B3-BAE9-51FEA71F48D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" firstSheet="1" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="2" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
     <sheet name="HTSE" sheetId="2" r:id="rId2"/>
-    <sheet name="Capacity_Market" sheetId="3" r:id="rId3"/>
-    <sheet name="Transfer_rates" sheetId="4" r:id="rId4"/>
-    <sheet name="grid_sellall_test" sheetId="5" r:id="rId5"/>
-    <sheet name="grid_sellnothing_test" sheetId="6" r:id="rId6"/>
+    <sheet name="FT" sheetId="7" r:id="rId3"/>
+    <sheet name="Capacity_Market" sheetId="3" r:id="rId4"/>
+    <sheet name="Transfer_rates" sheetId="4" r:id="rId5"/>
+    <sheet name="grid_sellall_test" sheetId="5" r:id="rId6"/>
+    <sheet name="grid_sellnothing_test" sheetId="6" r:id="rId7"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -40,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="200" uniqueCount="99">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
   <si>
     <t>Source</t>
   </si>
@@ -337,6 +338,87 @@
   </si>
   <si>
     <t>kg-H2/kWh-e</t>
+  </si>
+  <si>
+    <t>Performance and cost analysis of liquid fuel production form H2 and CO2 based on the FT process</t>
+  </si>
+  <si>
+    <t>Description</t>
+  </si>
+  <si>
+    <t>Total Direct Capital Costs, sum of equipment installed costs</t>
+  </si>
+  <si>
+    <t>TDCC</t>
+  </si>
+  <si>
+    <t>Depreciable Capital Costs</t>
+  </si>
+  <si>
+    <t>Non-depreciable Capital Costs</t>
+  </si>
+  <si>
+    <t>Land</t>
+  </si>
+  <si>
+    <t>$USD (2016)</t>
+  </si>
+  <si>
+    <t>Project contingency</t>
+  </si>
+  <si>
+    <t>Upfront permitting costs</t>
+  </si>
+  <si>
+    <t>Eng and design</t>
+  </si>
+  <si>
+    <t>Total Capital Investment</t>
+  </si>
+  <si>
+    <t>Site preparation</t>
+  </si>
+  <si>
+    <t>TCI</t>
+  </si>
+  <si>
+    <t>Total depreciable capital costs</t>
+  </si>
+  <si>
+    <t>Catalyst first fill fee</t>
+  </si>
+  <si>
+    <t>LC</t>
+  </si>
+  <si>
+    <t>Labor Cost</t>
+  </si>
+  <si>
+    <t>$USD (2016)/year</t>
+  </si>
+  <si>
+    <t>Gen and admin</t>
+  </si>
+  <si>
+    <t>Property taxes and insurance</t>
+  </si>
+  <si>
+    <t>2% TCI</t>
+  </si>
+  <si>
+    <t>20% LC</t>
+  </si>
+  <si>
+    <t>Materials costs for maintenance</t>
+  </si>
+  <si>
+    <t>Total Fixed Operating Costs</t>
+  </si>
+  <si>
+    <t>None Energy material and utilities costs</t>
+  </si>
+  <si>
+    <t>Total Variable Operating Costs (excl. feedstock and elec)</t>
   </si>
 </sst>
 </file>
@@ -387,7 +469,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="1">
+  <borders count="15">
     <border>
       <left/>
       <right/>
@@ -395,12 +477,160 @@
       <bottom/>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="thin">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="thin">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top/>
+      <bottom style="medium">
+        <color indexed="64"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="9">
+  <cellXfs count="36">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -412,6 +642,43 @@
     <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="6" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="7" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="2">
     <cellStyle name="Good" xfId="1" builtinId="26"/>
@@ -886,8 +1153,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0215393-90AE-4217-9780-C6903F6FBFD3}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H14" sqref="H14"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1057,6 +1324,266 @@
 </file>
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E35C99A-39AC-4C72-B859-1A7DCC98EEE1}">
+  <dimension ref="A1:D18"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I10" sqref="I10"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.81640625" customWidth="1"/>
+    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="9" t="s">
+        <v>99</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" s="19" t="s">
+        <v>26</v>
+      </c>
+      <c r="B2" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="C2" s="20" t="s">
+        <v>27</v>
+      </c>
+      <c r="D2" s="21" t="s">
+        <v>28</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+      <c r="A3" s="22" t="s">
+        <v>102</v>
+      </c>
+      <c r="B3" s="10" t="s">
+        <v>101</v>
+      </c>
+      <c r="C3" s="11">
+        <v>257800644</v>
+      </c>
+      <c r="D3" s="23" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" s="24" t="s">
+        <v>103</v>
+      </c>
+      <c r="B4" s="12" t="s">
+        <v>111</v>
+      </c>
+      <c r="C4" s="13">
+        <f>0.02*C3</f>
+        <v>5156012.88</v>
+      </c>
+      <c r="D4" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" s="24"/>
+      <c r="B5" s="12" t="s">
+        <v>109</v>
+      </c>
+      <c r="C5" s="13">
+        <f>0.1*C3</f>
+        <v>25780064.400000002</v>
+      </c>
+      <c r="D5" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" s="24"/>
+      <c r="B6" s="12" t="s">
+        <v>107</v>
+      </c>
+      <c r="C6" s="13">
+        <f>0.15*C3</f>
+        <v>38670096.600000001</v>
+      </c>
+      <c r="D6" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A7" s="24"/>
+      <c r="B7" s="12" t="s">
+        <v>114</v>
+      </c>
+      <c r="C7" s="13">
+        <v>12251143</v>
+      </c>
+      <c r="D7" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A8" s="24"/>
+      <c r="B8" s="12" t="s">
+        <v>108</v>
+      </c>
+      <c r="C8" s="13">
+        <f>0.15*C3</f>
+        <v>38670096.600000001</v>
+      </c>
+      <c r="D8" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A9" s="24" t="s">
+        <v>113</v>
+      </c>
+      <c r="B9" s="12"/>
+      <c r="C9" s="13">
+        <f>SUM(C4:C8)</f>
+        <v>120527413.47999999</v>
+      </c>
+      <c r="D9" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A10" s="24" t="s">
+        <v>104</v>
+      </c>
+      <c r="B10" s="12" t="s">
+        <v>105</v>
+      </c>
+      <c r="C10" s="13">
+        <f>10*55036</f>
+        <v>550360</v>
+      </c>
+      <c r="D10" s="25" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A11" s="26" t="s">
+        <v>112</v>
+      </c>
+      <c r="B11" s="14" t="s">
+        <v>110</v>
+      </c>
+      <c r="C11" s="15">
+        <f>SUM(C3,C9,C10)</f>
+        <v>378878417.48000002</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A12" s="28" t="s">
+        <v>115</v>
+      </c>
+      <c r="B12" s="17" t="s">
+        <v>116</v>
+      </c>
+      <c r="C12" s="11">
+        <v>9607972</v>
+      </c>
+      <c r="D12" s="29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A13" s="30" t="s">
+        <v>118</v>
+      </c>
+      <c r="B13" s="16" t="s">
+        <v>121</v>
+      </c>
+      <c r="C13" s="13">
+        <f>0.2*C12</f>
+        <v>1921594.4000000001</v>
+      </c>
+      <c r="D13" s="31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A14" s="30" t="s">
+        <v>119</v>
+      </c>
+      <c r="B14" s="16" t="s">
+        <v>120</v>
+      </c>
+      <c r="C14" s="13">
+        <f>0.02*C11</f>
+        <v>7577568.3496000003</v>
+      </c>
+      <c r="D14" s="31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A15" s="30" t="s">
+        <v>122</v>
+      </c>
+      <c r="B15" s="13"/>
+      <c r="C15" s="13">
+        <v>1049006</v>
+      </c>
+      <c r="D15" s="31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A16" s="30" t="s">
+        <v>123</v>
+      </c>
+      <c r="B16" s="13"/>
+      <c r="C16" s="18">
+        <f>SUM(C12:C15)</f>
+        <v>20156140.749600001</v>
+      </c>
+      <c r="D16" s="31" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A17" s="28" t="s">
+        <v>124</v>
+      </c>
+      <c r="B17" s="11"/>
+      <c r="C17" s="11">
+        <v>7085933</v>
+      </c>
+      <c r="D17" s="29" t="s">
+        <v>117</v>
+      </c>
+    </row>
+    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A18" s="32" t="s">
+        <v>125</v>
+      </c>
+      <c r="B18" s="33"/>
+      <c r="C18" s="34">
+        <f>C17</f>
+        <v>7085933</v>
+      </c>
+      <c r="D18" s="35" t="s">
+        <v>117</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -1160,7 +1687,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -1412,7 +1939,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD4092A-9167-4B1E-A144-D4BB7A88B529}">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -1666,7 +2193,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8827ECA-5F74-4389-B5A8-A15818A92C9F}">
   <dimension ref="A1:E42"/>
   <sheetViews>

</xml_diff>

<commit_message>
Add depreciation schedule for FT and HTSE
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/synfuels_model_numbers.xlsx
+++ b/use_cases/2022_05/data/synfuels_model_numbers.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garrm\projects\FORCE\use_cases\2022_05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{F28E3A76-F76C-45B3-BAE9-51FEA71F48D3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC2EA4E-FAE5-4BCB-8E98-01E8FFAE956A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="2" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="245" uniqueCount="126">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="127">
   <si>
     <t>Source</t>
   </si>
@@ -419,13 +419,26 @@
   </si>
   <si>
     <t>Total Variable Operating Costs (excl. feedstock and elec)</t>
+  </si>
+  <si>
+    <t>Depreciation schedule</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="4" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="5" x14ac:knownFonts="1">
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -626,22 +639,23 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="2">
+  <cellStyleXfs count="3">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="36">
+  <cellXfs count="43">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="11" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
@@ -654,14 +668,13 @@
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="2" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="2" xfId="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="1" xfId="0" applyNumberFormat="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="0" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="0" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
@@ -677,11 +690,20 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="13" xfId="0" applyBorder="1"/>
-    <xf numFmtId="0" fontId="1" fillId="2" borderId="13" xfId="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="13" xfId="2" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="1" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="0" fillId="0" borderId="0" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="44" fontId="2" fillId="2" borderId="0" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="10" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="2">
-    <cellStyle name="Good" xfId="1" builtinId="26"/>
+  <cellStyles count="3">
+    <cellStyle name="Currency" xfId="1" builtinId="4"/>
+    <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -1153,8 +1175,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0215393-90AE-4217-9780-C6903F6FBFD3}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C2"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="F9" sqref="F9"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1164,7 +1186,7 @@
     <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -1173,143 +1195,144 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
+      <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C2" s="20" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
+      <c r="A3" s="23" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="8">
+      <c r="B3" s="17">
         <v>36.799999999999997</v>
       </c>
-      <c r="C3" t="s">
+      <c r="C3" s="24" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="B4" s="8">
+      <c r="A4" s="23"/>
+      <c r="B4" s="17">
         <f>1/B3</f>
         <v>2.7173913043478264E-2</v>
       </c>
-      <c r="C4" t="s">
+      <c r="C4" s="24" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
+      <c r="A5" s="23" t="s">
         <v>30</v>
       </c>
-      <c r="B5">
+      <c r="B5" s="13">
         <v>6.4</v>
       </c>
-      <c r="C5" t="s">
+      <c r="C5" s="24" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
+      <c r="A6" s="23" t="s">
         <v>36</v>
       </c>
-      <c r="B6">
+      <c r="B6" s="13">
         <v>590</v>
       </c>
-      <c r="C6" t="s">
+      <c r="C6" s="24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
+      <c r="A7" s="23" t="s">
         <v>37</v>
       </c>
-      <c r="B7">
+      <c r="B7" s="13">
         <v>763</v>
       </c>
-      <c r="C7" t="s">
+      <c r="C7" s="24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
+      <c r="A8" s="23" t="s">
         <v>32</v>
       </c>
-      <c r="B8">
+      <c r="B8" s="13">
         <v>544</v>
       </c>
-      <c r="C8" t="s">
+      <c r="C8" s="24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
+      <c r="A9" s="23" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="8">
+      <c r="B9" s="17">
         <v>703</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C9" s="24" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
+      <c r="A10" s="23" t="s">
         <v>38</v>
       </c>
-      <c r="B10">
+      <c r="B10" s="13">
         <v>20</v>
       </c>
-      <c r="C10" t="s">
+      <c r="C10" s="24" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
+      <c r="A11" s="23" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="8">
+      <c r="B11" s="17">
         <v>32.64</v>
       </c>
-      <c r="C11" t="s">
+      <c r="C11" s="24" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
+      <c r="A12" s="23" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="8">
+      <c r="B12" s="17">
         <v>3.41</v>
       </c>
-      <c r="C12" t="s">
+      <c r="C12" s="24" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
+      <c r="A13" s="23" t="s">
         <v>44</v>
       </c>
-      <c r="B13">
+      <c r="B13" s="13">
         <v>10</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C13" s="24" t="s">
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A14" s="41" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="8">
+      <c r="B14" s="33">
         <v>20</v>
       </c>
-      <c r="C14" t="s">
+      <c r="C14" s="42" t="s">
         <v>39</v>
       </c>
     </row>
@@ -1325,17 +1348,17 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E35C99A-39AC-4C72-B859-1A7DCC98EEE1}">
-  <dimension ref="A1:D18"/>
+  <dimension ref="A1:D19"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="I10" sqref="I10"/>
+    <sheetView topLeftCell="A2" workbookViewId="0">
+      <selection activeCell="H13" sqref="H13"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="34.81640625" customWidth="1"/>
-    <col min="3" max="3" width="11.81640625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1348,234 +1371,248 @@
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="19" t="s">
+      <c r="A2" s="18" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="20" t="s">
+      <c r="B2" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="21" t="s">
+      <c r="D2" s="20" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="22" t="s">
+      <c r="A3" s="21" t="s">
         <v>102</v>
       </c>
       <c r="B3" s="10" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="11">
+      <c r="C3" s="35">
         <v>257800644</v>
       </c>
-      <c r="D3" s="23" t="s">
+      <c r="D3" s="22" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="24" t="s">
+      <c r="A4" s="23" t="s">
         <v>103</v>
       </c>
       <c r="B4" s="12" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="13">
+      <c r="C4" s="36">
         <f>0.02*C3</f>
         <v>5156012.88</v>
       </c>
-      <c r="D4" s="25" t="s">
+      <c r="D4" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="24"/>
+      <c r="A5" s="23"/>
       <c r="B5" s="12" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="13">
+      <c r="C5" s="36">
         <f>0.1*C3</f>
         <v>25780064.400000002</v>
       </c>
-      <c r="D5" s="25" t="s">
+      <c r="D5" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="24"/>
+      <c r="A6" s="23"/>
       <c r="B6" s="12" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="13">
+      <c r="C6" s="36">
         <f>0.15*C3</f>
         <v>38670096.600000001</v>
       </c>
-      <c r="D6" s="25" t="s">
+      <c r="D6" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="24"/>
+      <c r="A7" s="23"/>
       <c r="B7" s="12" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="13">
+      <c r="C7" s="36">
         <v>12251143</v>
       </c>
-      <c r="D7" s="25" t="s">
+      <c r="D7" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="24"/>
+      <c r="A8" s="23"/>
       <c r="B8" s="12" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="13">
+      <c r="C8" s="36">
         <f>0.15*C3</f>
         <v>38670096.600000001</v>
       </c>
-      <c r="D8" s="25" t="s">
+      <c r="D8" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="24" t="s">
+      <c r="A9" s="23" t="s">
         <v>113</v>
       </c>
       <c r="B9" s="12"/>
-      <c r="C9" s="13">
+      <c r="C9" s="36">
         <f>SUM(C4:C8)</f>
         <v>120527413.47999999</v>
       </c>
-      <c r="D9" s="25" t="s">
+      <c r="D9" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="24" t="s">
+      <c r="A10" s="23" t="s">
         <v>104</v>
       </c>
       <c r="B10" s="12" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="13">
+      <c r="C10" s="36">
         <f>10*55036</f>
         <v>550360</v>
       </c>
-      <c r="D10" s="25" t="s">
+      <c r="D10" s="24" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="26" t="s">
+      <c r="A11" s="25" t="s">
         <v>112</v>
       </c>
       <c r="B11" s="14" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="15">
+      <c r="C11" s="37">
         <f>SUM(C3,C9,C10)</f>
         <v>378878417.48000002</v>
       </c>
-      <c r="D11" s="27" t="s">
+      <c r="D11" s="26" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="28" t="s">
+      <c r="A12" s="27" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="17" t="s">
+      <c r="B12" s="16" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="11">
+      <c r="C12" s="35">
         <v>9607972</v>
       </c>
-      <c r="D12" s="29" t="s">
+      <c r="D12" s="28" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="30" t="s">
+      <c r="A13" s="29" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="16" t="s">
+      <c r="B13" s="15" t="s">
         <v>121</v>
       </c>
-      <c r="C13" s="13">
+      <c r="C13" s="36">
         <f>0.2*C12</f>
         <v>1921594.4000000001</v>
       </c>
-      <c r="D13" s="31" t="s">
+      <c r="D13" s="30" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="30" t="s">
+      <c r="A14" s="29" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="16" t="s">
+      <c r="B14" s="15" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="13">
+      <c r="C14" s="36">
         <f>0.02*C11</f>
         <v>7577568.3496000003</v>
       </c>
-      <c r="D14" s="31" t="s">
+      <c r="D14" s="30" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="30" t="s">
+      <c r="A15" s="29" t="s">
         <v>122</v>
       </c>
       <c r="B15" s="13"/>
-      <c r="C15" s="13">
+      <c r="C15" s="36">
         <v>1049006</v>
       </c>
-      <c r="D15" s="31" t="s">
+      <c r="D15" s="30" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="30" t="s">
+      <c r="A16" s="29" t="s">
         <v>123</v>
       </c>
       <c r="B16" s="13"/>
-      <c r="C16" s="18">
+      <c r="C16" s="38">
         <f>SUM(C12:C15)</f>
         <v>20156140.749600001</v>
       </c>
-      <c r="D16" s="31" t="s">
+      <c r="D16" s="30" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="28" t="s">
+      <c r="A17" s="27" t="s">
         <v>124</v>
       </c>
       <c r="B17" s="11"/>
-      <c r="C17" s="11">
+      <c r="C17" s="35">
         <v>7085933</v>
       </c>
-      <c r="D17" s="29" t="s">
+      <c r="D17" s="28" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A18" s="32" t="s">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A18" s="39" t="s">
         <v>125</v>
       </c>
-      <c r="B18" s="33"/>
-      <c r="C18" s="34">
+      <c r="B18" s="14"/>
+      <c r="C18" s="37">
         <f>C17</f>
         <v>7085933</v>
       </c>
-      <c r="D18" s="35" t="s">
+      <c r="D18" s="40" t="s">
         <v>117</v>
+      </c>
+    </row>
+    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="31" t="s">
+        <v>126</v>
+      </c>
+      <c r="B19" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="C19" s="32">
+        <v>20</v>
+      </c>
+      <c r="D19" s="34" t="s">
+        <v>39</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Regression for FT process scaling factor
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/synfuels_model_numbers.xlsx
+++ b/use_cases/2022_05/data/synfuels_model_numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25128"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garrm\projects\FORCE\use_cases\2022_05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FDC2EA4E-FAE5-4BCB-8E98-01E8FFAE956A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B42934-EE9E-48B8-91F4-EA5B7DB854D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="1" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="2" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -41,7 +41,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="248" uniqueCount="127">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="171">
   <si>
     <t>Source</t>
   </si>
@@ -422,14 +422,147 @@
   </si>
   <si>
     <t>Depreciation schedule</t>
+  </si>
+  <si>
+    <t>Equipment Installed costs</t>
+  </si>
+  <si>
+    <t>Equipment</t>
+  </si>
+  <si>
+    <t>Base cost</t>
+  </si>
+  <si>
+    <t>Installation factor</t>
+  </si>
+  <si>
+    <t>Scaling exponent</t>
+  </si>
+  <si>
+    <t>Source: Performance and Cost Analysis of Liquid Fuel Production from H2 and CO2 Based on the Fischer-Tropsch Process</t>
+  </si>
+  <si>
+    <t>CO2 compressor 1</t>
+  </si>
+  <si>
+    <t>CO2 compressor 2</t>
+  </si>
+  <si>
+    <t>H2 compressor</t>
+  </si>
+  <si>
+    <t>RWGS reactor</t>
+  </si>
+  <si>
+    <t>Syngas preheater</t>
+  </si>
+  <si>
+    <t>CO2 separator</t>
+  </si>
+  <si>
+    <t>Syngas cooler</t>
+  </si>
+  <si>
+    <t>Flash separator</t>
+  </si>
+  <si>
+    <t>Syngas compressor</t>
+  </si>
+  <si>
+    <t>FT synthesis reactor</t>
+  </si>
+  <si>
+    <t>Wax separator</t>
+  </si>
+  <si>
+    <t>Gas/liquid separator</t>
+  </si>
+  <si>
+    <t>Flue gas heat exchanger</t>
+  </si>
+  <si>
+    <t>Flue gas cooler</t>
+  </si>
+  <si>
+    <t>Dryer FT-synthesis</t>
+  </si>
+  <si>
+    <t>Dryer RWGS</t>
+  </si>
+  <si>
+    <t>Flue gas compressor</t>
+  </si>
+  <si>
+    <t>PSA H2 separator</t>
+  </si>
+  <si>
+    <t>Wax preheater</t>
+  </si>
+  <si>
+    <t>Wax cooler</t>
+  </si>
+  <si>
+    <t>Wax dryer</t>
+  </si>
+  <si>
+    <t>Liquid cooler and dryer</t>
+  </si>
+  <si>
+    <t>Wax hydrocracking</t>
+  </si>
+  <si>
+    <t>Gas separator</t>
+  </si>
+  <si>
+    <t>Naphta distillation</t>
+  </si>
+  <si>
+    <t>Jet fuel distillation</t>
+  </si>
+  <si>
+    <t>Naphta dryer and cooler</t>
+  </si>
+  <si>
+    <t>Boiler steam generator</t>
+  </si>
+  <si>
+    <t>Steam turbine</t>
+  </si>
+  <si>
+    <t>Boiler auxiliary device</t>
+  </si>
+  <si>
+    <t>Cooling tower</t>
+  </si>
+  <si>
+    <t>Fuel storage</t>
+  </si>
+  <si>
+    <t>Wastewater treatment</t>
+  </si>
+  <si>
+    <t>Diesel distillation</t>
+  </si>
+  <si>
+    <t>Assumption: Every component size increases in the same way as the whole process</t>
+  </si>
+  <si>
+    <t>Size factor</t>
+  </si>
+  <si>
+    <t>Log TCI</t>
+  </si>
+  <si>
+    <t>Log size factor</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="1">
+  <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -644,13 +777,10 @@
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="43">
+  <cellXfs count="46">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="11" fontId="4" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="11" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
@@ -700,6 +830,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -717,6 +853,1172 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/charts/chart1.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:rich>
+          <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:r>
+              <a:rPr lang="en-US"/>
+              <a:t>TCI logarithmic</a:t>
+            </a:r>
+            <a:r>
+              <a:rPr lang="en-US" baseline="0"/>
+              <a:t> regression</a:t>
+            </a:r>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:rich>
+      </c:tx>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>FT!$D$63</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Log TCI</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:trendline>
+            <c:spPr>
+              <a:ln w="19050" cap="rnd">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+                <a:prstDash val="sysDot"/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+            <c:trendlineType val="linear"/>
+            <c:dispRSqr val="1"/>
+            <c:dispEq val="1"/>
+            <c:trendlineLbl>
+              <c:numFmt formatCode="General" sourceLinked="0"/>
+              <c:spPr>
+                <a:noFill/>
+                <a:ln>
+                  <a:noFill/>
+                </a:ln>
+                <a:effectLst/>
+              </c:spPr>
+              <c:txPr>
+                <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+                <a:lstStyle/>
+                <a:p>
+                  <a:pPr>
+                    <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                      <a:solidFill>
+                        <a:schemeClr val="tx1">
+                          <a:lumMod val="65000"/>
+                          <a:lumOff val="35000"/>
+                        </a:schemeClr>
+                      </a:solidFill>
+                      <a:latin typeface="+mn-lt"/>
+                      <a:ea typeface="+mn-ea"/>
+                      <a:cs typeface="+mn-cs"/>
+                    </a:defRPr>
+                  </a:pPr>
+                  <a:endParaRPr lang="en-US"/>
+                </a:p>
+              </c:txPr>
+            </c:trendlineLbl>
+          </c:trendline>
+          <c:xVal>
+            <c:numRef>
+              <c:f>FT!$E$62:$M$62</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>-0.6020599913279624</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>-0.3010299956639812</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>9.691001300805642E-2</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>0.17609125905568124</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>0.3010299956639812</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>0.6020599913279624</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>0.69897000433601886</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>1</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>FT!$E$63:$M$63</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="9"/>
+                <c:pt idx="0">
+                  <c:v>8.0156193531831796</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>8.2128604602155431</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>8.411284001279153</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>8.4754249287508117</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>8.5279296264238802</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>8.6109577543918885</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>8.8119472733677942</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>8.8769417662830747</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>9.0797652001107316</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-2470-4815-83E6-4DB2285777F3}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="837646064"/>
+        <c:axId val="837647312"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="837646064"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log(Size factor)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="837647312"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="837647312"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:minorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="5000"/>
+                  <a:lumOff val="95000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:minorGridlines>
+        <c:title>
+          <c:tx>
+            <c:rich>
+              <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+              <a:lstStyle/>
+              <a:p>
+                <a:pPr>
+                  <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                    <a:solidFill>
+                      <a:schemeClr val="tx1">
+                        <a:lumMod val="65000"/>
+                        <a:lumOff val="35000"/>
+                      </a:schemeClr>
+                    </a:solidFill>
+                    <a:latin typeface="+mn-lt"/>
+                    <a:ea typeface="+mn-ea"/>
+                    <a:cs typeface="+mn-cs"/>
+                  </a:defRPr>
+                </a:pPr>
+                <a:r>
+                  <a:rPr lang="en-US"/>
+                  <a:t>log(TCI)</a:t>
+                </a:r>
+              </a:p>
+            </c:rich>
+          </c:tx>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1">
+                      <a:lumMod val="65000"/>
+                      <a:lumOff val="35000"/>
+                    </a:schemeClr>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="out"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="837646064"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/drawings/drawing1.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>4</xdr:col>
+      <xdr:colOff>779462</xdr:colOff>
+      <xdr:row>63</xdr:row>
+      <xdr:rowOff>160336</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>457200</xdr:colOff>
+      <xdr:row>92</xdr:row>
+      <xdr:rowOff>104775</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="3" name="Chart 2">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{3E656C37-AFFE-1C1C-5B7A-E46941F34BB3}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -1040,10 +2342,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="42" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="3"/>
+      <c r="B2" s="42"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -1175,8 +2477,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{D0215393-90AE-4217-9780-C6903F6FBFD3}">
   <dimension ref="A1:C16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="F9" sqref="F9"/>
+    <sheetView workbookViewId="0">
+      <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1195,149 +2497,149 @@
       </c>
     </row>
     <row r="2" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="C2" s="20" t="s">
+      <c r="C2" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A3" s="23" t="s">
+      <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
-      <c r="B3" s="17">
+      <c r="B3" s="16">
         <v>36.799999999999997</v>
       </c>
-      <c r="C3" s="24" t="s">
+      <c r="C3" s="23" t="s">
         <v>29</v>
       </c>
     </row>
     <row r="4" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A4" s="23"/>
-      <c r="B4" s="17">
+      <c r="A4" s="22"/>
+      <c r="B4" s="16">
         <f>1/B3</f>
         <v>2.7173913043478264E-2</v>
       </c>
-      <c r="C4" s="24" t="s">
+      <c r="C4" s="23" t="s">
         <v>98</v>
       </c>
     </row>
     <row r="5" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A5" s="23" t="s">
+      <c r="A5" s="22" t="s">
         <v>30</v>
       </c>
-      <c r="B5" s="13">
+      <c r="B5" s="12">
         <v>6.4</v>
       </c>
-      <c r="C5" s="24" t="s">
+      <c r="C5" s="23" t="s">
         <v>31</v>
       </c>
     </row>
     <row r="6" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A6" s="23" t="s">
+      <c r="A6" s="22" t="s">
         <v>36</v>
       </c>
-      <c r="B6" s="13">
+      <c r="B6" s="12">
         <v>590</v>
       </c>
-      <c r="C6" s="24" t="s">
+      <c r="C6" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="7" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A7" s="23" t="s">
+      <c r="A7" s="22" t="s">
         <v>37</v>
       </c>
-      <c r="B7" s="13">
+      <c r="B7" s="12">
         <v>763</v>
       </c>
-      <c r="C7" s="24" t="s">
+      <c r="C7" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="8" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A8" s="23" t="s">
+      <c r="A8" s="22" t="s">
         <v>32</v>
       </c>
-      <c r="B8" s="13">
+      <c r="B8" s="12">
         <v>544</v>
       </c>
-      <c r="C8" s="24" t="s">
+      <c r="C8" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="9" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>35</v>
       </c>
-      <c r="B9" s="17">
+      <c r="B9" s="16">
         <v>703</v>
       </c>
-      <c r="C9" s="24" t="s">
+      <c r="C9" s="23" t="s">
         <v>33</v>
       </c>
     </row>
     <row r="10" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>38</v>
       </c>
-      <c r="B10" s="13">
+      <c r="B10" s="12">
         <v>20</v>
       </c>
-      <c r="C10" s="24" t="s">
+      <c r="C10" s="23" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="11" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A11" s="23" t="s">
+      <c r="A11" s="22" t="s">
         <v>40</v>
       </c>
-      <c r="B11" s="17">
+      <c r="B11" s="16">
         <v>32.64</v>
       </c>
-      <c r="C11" s="24" t="s">
+      <c r="C11" s="23" t="s">
         <v>41</v>
       </c>
     </row>
     <row r="12" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A12" s="23" t="s">
+      <c r="A12" s="22" t="s">
         <v>42</v>
       </c>
-      <c r="B12" s="17">
+      <c r="B12" s="16">
         <v>3.41</v>
       </c>
-      <c r="C12" s="24" t="s">
+      <c r="C12" s="23" t="s">
         <v>43</v>
       </c>
     </row>
     <row r="13" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A13" s="23" t="s">
+      <c r="A13" s="22" t="s">
         <v>44</v>
       </c>
-      <c r="B13" s="13">
+      <c r="B13" s="12">
         <v>10</v>
       </c>
-      <c r="C13" s="24" t="s">
+      <c r="C13" s="23" t="s">
         <v>45</v>
       </c>
     </row>
     <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A14" s="41" t="s">
+      <c r="A14" s="40" t="s">
         <v>46</v>
       </c>
-      <c r="B14" s="33">
+      <c r="B14" s="32">
         <v>20</v>
       </c>
-      <c r="C14" s="42" t="s">
+      <c r="C14" s="41" t="s">
         <v>39</v>
       </c>
     </row>
     <row r="16" spans="1:3" x14ac:dyDescent="0.35">
-      <c r="A16" s="8" t="s">
+      <c r="A16" s="7" t="s">
         <v>97</v>
       </c>
     </row>
@@ -1348,10 +2650,10 @@
 
 <file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E35C99A-39AC-4C72-B859-1A7DCC98EEE1}">
-  <dimension ref="A1:D19"/>
+  <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="A2" workbookViewId="0">
-      <selection activeCell="H13" sqref="H13"/>
+    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
+      <selection activeCell="T68" sqref="T68"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -1360,263 +2662,2188 @@
     <col min="2" max="2" width="34.81640625" customWidth="1"/>
     <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="13.08984375" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="9" t="s">
+      <c r="B1" s="8" t="s">
         <v>99</v>
       </c>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A2" s="18" t="s">
+      <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
-      <c r="B2" s="19" t="s">
+      <c r="B2" s="18" t="s">
         <v>100</v>
       </c>
-      <c r="C2" s="19" t="s">
+      <c r="C2" s="18" t="s">
         <v>27</v>
       </c>
-      <c r="D2" s="20" t="s">
+      <c r="D2" s="19" t="s">
         <v>28</v>
       </c>
     </row>
     <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
-      <c r="A3" s="21" t="s">
+      <c r="A3" s="20" t="s">
         <v>102</v>
       </c>
-      <c r="B3" s="10" t="s">
+      <c r="B3" s="9" t="s">
         <v>101</v>
       </c>
-      <c r="C3" s="35">
+      <c r="C3" s="34">
         <v>257800644</v>
       </c>
-      <c r="D3" s="22" t="s">
+      <c r="D3" s="21" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="4" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A4" s="23" t="s">
+      <c r="A4" s="22" t="s">
         <v>103</v>
       </c>
-      <c r="B4" s="12" t="s">
+      <c r="B4" s="11" t="s">
         <v>111</v>
       </c>
-      <c r="C4" s="36">
+      <c r="C4" s="35">
         <f>0.02*C3</f>
         <v>5156012.88</v>
       </c>
-      <c r="D4" s="24" t="s">
+      <c r="D4" s="23" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="5" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A5" s="23"/>
-      <c r="B5" s="12" t="s">
+      <c r="A5" s="22"/>
+      <c r="B5" s="11" t="s">
         <v>109</v>
       </c>
-      <c r="C5" s="36">
+      <c r="C5" s="35">
         <f>0.1*C3</f>
         <v>25780064.400000002</v>
       </c>
-      <c r="D5" s="24" t="s">
+      <c r="D5" s="23" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="6" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A6" s="23"/>
-      <c r="B6" s="12" t="s">
+      <c r="A6" s="22"/>
+      <c r="B6" s="11" t="s">
         <v>107</v>
       </c>
-      <c r="C6" s="36">
+      <c r="C6" s="35">
         <f>0.15*C3</f>
         <v>38670096.600000001</v>
       </c>
-      <c r="D6" s="24" t="s">
+      <c r="D6" s="23" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="7" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A7" s="23"/>
-      <c r="B7" s="12" t="s">
+      <c r="A7" s="22"/>
+      <c r="B7" s="11" t="s">
         <v>114</v>
       </c>
-      <c r="C7" s="36">
+      <c r="C7" s="35">
         <v>12251143</v>
       </c>
-      <c r="D7" s="24" t="s">
+      <c r="D7" s="23" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="8" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A8" s="23"/>
-      <c r="B8" s="12" t="s">
+      <c r="A8" s="22"/>
+      <c r="B8" s="11" t="s">
         <v>108</v>
       </c>
-      <c r="C8" s="36">
+      <c r="C8" s="35">
         <f>0.15*C3</f>
         <v>38670096.600000001</v>
       </c>
-      <c r="D8" s="24" t="s">
+      <c r="D8" s="23" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="9" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A9" s="23" t="s">
+      <c r="A9" s="22" t="s">
         <v>113</v>
       </c>
-      <c r="B9" s="12"/>
-      <c r="C9" s="36">
+      <c r="B9" s="11"/>
+      <c r="C9" s="35">
         <f>SUM(C4:C8)</f>
         <v>120527413.47999999</v>
       </c>
-      <c r="D9" s="24" t="s">
+      <c r="D9" s="23" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="10" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A10" s="23" t="s">
+      <c r="A10" s="22" t="s">
         <v>104</v>
       </c>
-      <c r="B10" s="12" t="s">
+      <c r="B10" s="11" t="s">
         <v>105</v>
       </c>
-      <c r="C10" s="36">
+      <c r="C10" s="35">
         <f>10*55036</f>
         <v>550360</v>
       </c>
-      <c r="D10" s="24" t="s">
+      <c r="D10" s="23" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="11" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A11" s="25" t="s">
+      <c r="A11" s="24" t="s">
         <v>112</v>
       </c>
-      <c r="B11" s="14" t="s">
+      <c r="B11" s="13" t="s">
         <v>110</v>
       </c>
-      <c r="C11" s="37">
+      <c r="C11" s="36">
         <f>SUM(C3,C9,C10)</f>
         <v>378878417.48000002</v>
       </c>
-      <c r="D11" s="26" t="s">
+      <c r="D11" s="25" t="s">
         <v>106</v>
       </c>
     </row>
     <row r="12" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A12" s="27" t="s">
+      <c r="A12" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B12" s="16" t="s">
+      <c r="B12" s="15" t="s">
         <v>116</v>
       </c>
-      <c r="C12" s="35">
+      <c r="C12" s="34">
         <v>9607972</v>
       </c>
-      <c r="D12" s="28" t="s">
+      <c r="D12" s="27" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="13" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A13" s="29" t="s">
+      <c r="A13" s="28" t="s">
         <v>118</v>
       </c>
-      <c r="B13" s="15" t="s">
+      <c r="B13" s="14" t="s">
         <v>121</v>
       </c>
-      <c r="C13" s="36">
+      <c r="C13" s="35">
         <f>0.2*C12</f>
         <v>1921594.4000000001</v>
       </c>
-      <c r="D13" s="30" t="s">
+      <c r="D13" s="29" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="14" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A14" s="29" t="s">
+      <c r="A14" s="28" t="s">
         <v>119</v>
       </c>
-      <c r="B14" s="15" t="s">
+      <c r="B14" s="14" t="s">
         <v>120</v>
       </c>
-      <c r="C14" s="36">
+      <c r="C14" s="35">
         <f>0.02*C11</f>
         <v>7577568.3496000003</v>
       </c>
-      <c r="D14" s="30" t="s">
+      <c r="D14" s="29" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="15" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A15" s="29" t="s">
+      <c r="A15" s="28" t="s">
         <v>122</v>
       </c>
-      <c r="B15" s="13"/>
-      <c r="C15" s="36">
+      <c r="B15" s="12"/>
+      <c r="C15" s="35">
         <v>1049006</v>
       </c>
-      <c r="D15" s="30" t="s">
+      <c r="D15" s="29" t="s">
         <v>117</v>
       </c>
     </row>
     <row r="16" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A16" s="29" t="s">
+      <c r="A16" s="28" t="s">
         <v>123</v>
       </c>
-      <c r="B16" s="13"/>
-      <c r="C16" s="38">
+      <c r="B16" s="12"/>
+      <c r="C16" s="37">
         <f>SUM(C12:C15)</f>
         <v>20156140.749600001</v>
       </c>
-      <c r="D16" s="30" t="s">
+      <c r="D16" s="29" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A17" s="27" t="s">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A17" s="26" t="s">
         <v>124</v>
       </c>
-      <c r="B17" s="11"/>
-      <c r="C17" s="35">
+      <c r="B17" s="10"/>
+      <c r="C17" s="34">
         <v>7085933</v>
       </c>
-      <c r="D17" s="28" t="s">
+      <c r="D17" s="27" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
-      <c r="A18" s="39" t="s">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A18" s="38" t="s">
         <v>125</v>
       </c>
-      <c r="B18" s="14"/>
-      <c r="C18" s="37">
+      <c r="B18" s="13"/>
+      <c r="C18" s="36">
         <f>C17</f>
         <v>7085933</v>
       </c>
-      <c r="D18" s="40" t="s">
+      <c r="D18" s="39" t="s">
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:4" ht="15" thickBot="1" x14ac:dyDescent="0.4">
-      <c r="A19" s="31" t="s">
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A19" s="30" t="s">
         <v>126</v>
       </c>
-      <c r="B19" s="32" t="s">
+      <c r="B19" s="31" t="s">
         <v>4</v>
       </c>
-      <c r="C19" s="32">
+      <c r="C19" s="31">
         <v>20</v>
       </c>
-      <c r="D19" s="34" t="s">
+      <c r="D19" s="33" t="s">
         <v>39</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A22" t="s">
+        <v>127</v>
+      </c>
+      <c r="B22" t="s">
+        <v>132</v>
+      </c>
+      <c r="C22" t="s">
+        <v>167</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="E23" t="s">
+        <v>168</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A24" t="s">
+        <v>128</v>
+      </c>
+      <c r="B24" t="s">
+        <v>129</v>
+      </c>
+      <c r="C24" t="s">
+        <v>130</v>
+      </c>
+      <c r="D24" t="s">
+        <v>131</v>
+      </c>
+      <c r="E24">
+        <v>0.25</v>
+      </c>
+      <c r="F24">
+        <v>0.5</v>
+      </c>
+      <c r="G24">
+        <v>1</v>
+      </c>
+      <c r="H24">
+        <v>1.25</v>
+      </c>
+      <c r="I24">
+        <v>1.5</v>
+      </c>
+      <c r="J24">
+        <v>2</v>
+      </c>
+      <c r="K24">
+        <v>4</v>
+      </c>
+      <c r="L24">
+        <v>5</v>
+      </c>
+      <c r="M24">
+        <v>10</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A25" t="s">
+        <v>133</v>
+      </c>
+      <c r="B25" s="43">
+        <v>11807922</v>
+      </c>
+      <c r="C25">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D25">
+        <v>0.65</v>
+      </c>
+      <c r="E25" s="44">
+        <f>$B25*POWER(E$24,$D25)</f>
+        <v>4795506.4702437567</v>
+      </c>
+      <c r="F25" s="44">
+        <f>$B25*POWER(F$24,$D25)</f>
+        <v>7524956.2358284583</v>
+      </c>
+      <c r="G25" s="44">
+        <f t="shared" ref="F25:M40" si="0">$B25*POWER(G$24,$D25)</f>
+        <v>11807922</v>
+      </c>
+      <c r="H25" s="44">
+        <f t="shared" si="0"/>
+        <v>13651016.264884572</v>
+      </c>
+      <c r="I25" s="44">
+        <f t="shared" si="0"/>
+        <v>15368546.448911712</v>
+      </c>
+      <c r="J25" s="44">
+        <f t="shared" si="0"/>
+        <v>18528615.660810392</v>
+      </c>
+      <c r="K25" s="44">
+        <f t="shared" si="0"/>
+        <v>29074514.407025062</v>
+      </c>
+      <c r="L25" s="44">
+        <f t="shared" si="0"/>
+        <v>33612744.821986459</v>
+      </c>
+      <c r="M25" s="44">
+        <f t="shared" si="0"/>
+        <v>52744050.147983856</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A26" t="s">
+        <v>134</v>
+      </c>
+      <c r="B26" s="43">
+        <v>17388504</v>
+      </c>
+      <c r="C26">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D26">
+        <v>0.8</v>
+      </c>
+      <c r="E26" s="44">
+        <f t="shared" ref="E26:M58" si="1">$B26*POWER(E$24,$D26)</f>
+        <v>5736067.1461265292</v>
+      </c>
+      <c r="F26" s="44">
+        <f t="shared" si="0"/>
+        <v>9987072.9703296833</v>
+      </c>
+      <c r="G26" s="44">
+        <f t="shared" si="0"/>
+        <v>17388504</v>
+      </c>
+      <c r="H26" s="44">
+        <f t="shared" si="0"/>
+        <v>20786924.085011322</v>
+      </c>
+      <c r="I26" s="44">
+        <f t="shared" si="0"/>
+        <v>24051115.660847504</v>
+      </c>
+      <c r="J26" s="44">
+        <f t="shared" si="0"/>
+        <v>30275143.904153816</v>
+      </c>
+      <c r="K26" s="44">
+        <f t="shared" si="0"/>
+        <v>52712087.159264646</v>
+      </c>
+      <c r="L26" s="44">
+        <f t="shared" si="0"/>
+        <v>63014170.40489132</v>
+      </c>
+      <c r="M26" s="44">
+        <f t="shared" si="0"/>
+        <v>109714043.08323221</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A27" t="s">
+        <v>135</v>
+      </c>
+      <c r="B27" s="43">
+        <v>2547995</v>
+      </c>
+      <c r="C27">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D27">
+        <v>0.6</v>
+      </c>
+      <c r="E27" s="44">
+        <f t="shared" si="1"/>
+        <v>1109079.2412628538</v>
+      </c>
+      <c r="F27" s="44">
+        <f t="shared" si="0"/>
+        <v>1681049.7795548902</v>
+      </c>
+      <c r="G27" s="44">
+        <f t="shared" si="0"/>
+        <v>2547995</v>
+      </c>
+      <c r="H27" s="44">
+        <f t="shared" si="0"/>
+        <v>2913027.4644639199</v>
+      </c>
+      <c r="I27" s="44">
+        <f t="shared" si="0"/>
+        <v>3249775.2504720115</v>
+      </c>
+      <c r="J27" s="44">
+        <f t="shared" si="0"/>
+        <v>3862038.2328856615</v>
+      </c>
+      <c r="K27" s="44">
+        <f t="shared" si="0"/>
+        <v>5853755.3300813409</v>
+      </c>
+      <c r="L27" s="44">
+        <f t="shared" si="0"/>
+        <v>6692379.7129817763</v>
+      </c>
+      <c r="M27" s="44">
+        <f t="shared" si="0"/>
+        <v>10143750.800344583</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A28" t="s">
+        <v>136</v>
+      </c>
+      <c r="B28" s="43">
+        <v>22972192</v>
+      </c>
+      <c r="C28">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D28">
+        <v>0.6</v>
+      </c>
+      <c r="E28" s="44">
+        <f t="shared" si="1"/>
+        <v>9999227.3428733572</v>
+      </c>
+      <c r="F28" s="44">
+        <f t="shared" si="0"/>
+        <v>15155994.535896897</v>
+      </c>
+      <c r="G28" s="44">
+        <f t="shared" si="0"/>
+        <v>22972192</v>
+      </c>
+      <c r="H28" s="44">
+        <f t="shared" si="0"/>
+        <v>26263248.638611279</v>
+      </c>
+      <c r="I28" s="44">
+        <f t="shared" si="0"/>
+        <v>29299296.509879783</v>
+      </c>
+      <c r="J28" s="44">
+        <f t="shared" si="0"/>
+        <v>34819331.983457632</v>
+      </c>
+      <c r="K28" s="44">
+        <f t="shared" si="0"/>
+        <v>52776238.322152101</v>
+      </c>
+      <c r="L28" s="44">
+        <f t="shared" si="0"/>
+        <v>60337101.016101778</v>
+      </c>
+      <c r="M28" s="44">
+        <f t="shared" si="0"/>
+        <v>91453943.585316852</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A29" t="s">
+        <v>137</v>
+      </c>
+      <c r="B29" s="43">
+        <v>6248204</v>
+      </c>
+      <c r="C29">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D29">
+        <v>0.6</v>
+      </c>
+      <c r="E29" s="44">
+        <f t="shared" si="1"/>
+        <v>2719688.7558945478</v>
+      </c>
+      <c r="F29" s="44">
+        <f t="shared" si="0"/>
+        <v>4122277.3030614201</v>
+      </c>
+      <c r="G29" s="44">
+        <f t="shared" si="0"/>
+        <v>6248204</v>
+      </c>
+      <c r="H29" s="44">
+        <f t="shared" si="0"/>
+        <v>7143338.1366813211</v>
+      </c>
+      <c r="I29" s="44">
+        <f t="shared" si="0"/>
+        <v>7969112.4665080681</v>
+      </c>
+      <c r="J29" s="44">
+        <f t="shared" si="0"/>
+        <v>9470506.3137365356</v>
+      </c>
+      <c r="K29" s="44">
+        <f t="shared" si="0"/>
+        <v>14354603.312971789</v>
+      </c>
+      <c r="L29" s="44">
+        <f t="shared" si="0"/>
+        <v>16411081.533586834</v>
+      </c>
+      <c r="M29" s="44">
+        <f t="shared" si="0"/>
+        <v>24874548.15481044</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A30" t="s">
+        <v>138</v>
+      </c>
+      <c r="B30" s="43">
+        <v>32995221</v>
+      </c>
+      <c r="C30">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D30">
+        <v>0.6</v>
+      </c>
+      <c r="E30" s="44">
+        <f t="shared" si="1"/>
+        <v>14362004.113815052</v>
+      </c>
+      <c r="F30" s="44">
+        <f t="shared" si="0"/>
+        <v>21768727.563599963</v>
+      </c>
+      <c r="G30" s="44">
+        <f t="shared" si="0"/>
+        <v>32995221</v>
+      </c>
+      <c r="H30" s="44">
+        <f t="shared" si="0"/>
+        <v>37722203.131896526</v>
+      </c>
+      <c r="I30" s="44">
+        <f t="shared" si="0"/>
+        <v>42082913.266962603</v>
+      </c>
+      <c r="J30" s="44">
+        <f t="shared" si="0"/>
+        <v>50011403.085371777</v>
+      </c>
+      <c r="K30" s="44">
+        <f t="shared" si="0"/>
+        <v>75803112.170927256</v>
+      </c>
+      <c r="L30" s="44">
+        <f t="shared" si="0"/>
+        <v>86662865.368947059</v>
+      </c>
+      <c r="M30" s="44">
+        <f t="shared" si="0"/>
+        <v>131356340.74097335</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A31" t="s">
+        <v>139</v>
+      </c>
+      <c r="B31" s="43">
+        <v>4186906</v>
+      </c>
+      <c r="C31">
+        <v>3.23</v>
+      </c>
+      <c r="D31">
+        <v>0.7</v>
+      </c>
+      <c r="E31" s="44">
+        <f t="shared" si="1"/>
+        <v>1586540.6966554464</v>
+      </c>
+      <c r="F31" s="44">
+        <f t="shared" si="0"/>
+        <v>2577342.9655501549</v>
+      </c>
+      <c r="G31" s="44">
+        <f t="shared" si="0"/>
+        <v>4186906</v>
+      </c>
+      <c r="H31" s="44">
+        <f t="shared" si="0"/>
+        <v>4894746.672099025</v>
+      </c>
+      <c r="I31" s="44">
+        <f t="shared" si="0"/>
+        <v>5561053.740726185</v>
+      </c>
+      <c r="J31" s="44">
+        <f t="shared" si="0"/>
+        <v>6801648.8636366008</v>
+      </c>
+      <c r="K31" s="44">
+        <f t="shared" si="0"/>
+        <v>11049311.17732499</v>
+      </c>
+      <c r="L31" s="44">
+        <f t="shared" si="0"/>
+        <v>12917313.910127921</v>
+      </c>
+      <c r="M31" s="44">
+        <f t="shared" si="0"/>
+        <v>20984238.355974279</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A32" t="s">
+        <v>140</v>
+      </c>
+      <c r="B32" s="43">
+        <v>807728</v>
+      </c>
+      <c r="C32">
+        <v>1.82</v>
+      </c>
+      <c r="D32">
+        <v>0.7</v>
+      </c>
+      <c r="E32" s="44">
+        <f t="shared" si="1"/>
+        <v>306071.67770857771</v>
+      </c>
+      <c r="F32" s="44">
+        <f t="shared" si="0"/>
+        <v>497214.90735113126</v>
+      </c>
+      <c r="G32" s="44">
+        <f t="shared" si="0"/>
+        <v>807728</v>
+      </c>
+      <c r="H32" s="44">
+        <f t="shared" si="0"/>
+        <v>944282.94782858784</v>
+      </c>
+      <c r="I32" s="44">
+        <f t="shared" si="0"/>
+        <v>1072825.3311369494</v>
+      </c>
+      <c r="J32" s="44">
+        <f t="shared" si="0"/>
+        <v>1312158.0072080588</v>
+      </c>
+      <c r="K32" s="44">
+        <f t="shared" si="0"/>
+        <v>2131606.9715055367</v>
+      </c>
+      <c r="L32" s="44">
+        <f t="shared" si="0"/>
+        <v>2491977.6393355392</v>
+      </c>
+      <c r="M32" s="44">
+        <f t="shared" si="0"/>
+        <v>4048229.6184328939</v>
+      </c>
+    </row>
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A33" t="s">
+        <v>148</v>
+      </c>
+      <c r="B33" s="43">
+        <v>75501</v>
+      </c>
+      <c r="C33">
+        <v>2</v>
+      </c>
+      <c r="D33">
+        <v>0.7</v>
+      </c>
+      <c r="E33" s="44">
+        <f t="shared" si="1"/>
+        <v>28609.529122025393</v>
+      </c>
+      <c r="F33" s="44">
+        <f t="shared" si="0"/>
+        <v>46476.317175977267</v>
+      </c>
+      <c r="G33" s="44">
+        <f t="shared" si="0"/>
+        <v>75501</v>
+      </c>
+      <c r="H33" s="44">
+        <f t="shared" si="0"/>
+        <v>88265.24132381966</v>
+      </c>
+      <c r="I33" s="44">
+        <f t="shared" si="0"/>
+        <v>100280.52181696167</v>
+      </c>
+      <c r="J33" s="44">
+        <f t="shared" si="0"/>
+        <v>122651.73635458427</v>
+      </c>
+      <c r="K33" s="44">
+        <f t="shared" si="0"/>
+        <v>199248.33354252856</v>
+      </c>
+      <c r="L33" s="44">
+        <f t="shared" si="0"/>
+        <v>232933.3683461172</v>
+      </c>
+      <c r="M33" s="44">
+        <f t="shared" si="0"/>
+        <v>378401.37326092686</v>
+      </c>
+    </row>
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A34" t="s">
+        <v>141</v>
+      </c>
+      <c r="B34" s="43">
+        <v>11461600</v>
+      </c>
+      <c r="C34">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D34">
+        <v>0.65</v>
+      </c>
+      <c r="E34" s="44">
+        <f t="shared" si="1"/>
+        <v>4654856.0330383144</v>
+      </c>
+      <c r="F34" s="44">
+        <f t="shared" si="0"/>
+        <v>7304252.0430412283</v>
+      </c>
+      <c r="G34" s="44">
+        <f t="shared" si="0"/>
+        <v>11461600</v>
+      </c>
+      <c r="H34" s="44">
+        <f t="shared" si="0"/>
+        <v>13250636.989438193</v>
+      </c>
+      <c r="I34" s="44">
+        <f t="shared" si="0"/>
+        <v>14917792.646229072</v>
+      </c>
+      <c r="J34" s="44">
+        <f t="shared" si="0"/>
+        <v>17985178.192906797</v>
+      </c>
+      <c r="K34" s="44">
+        <f t="shared" si="0"/>
+        <v>28221769.615988184</v>
+      </c>
+      <c r="L34" s="44">
+        <f t="shared" si="0"/>
+        <v>32626895.405616667</v>
+      </c>
+      <c r="M34" s="44">
+        <f t="shared" si="0"/>
+        <v>51197086.5979748</v>
+      </c>
+    </row>
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A35" t="s">
+        <v>142</v>
+      </c>
+      <c r="B35" s="43">
+        <v>36681585</v>
+      </c>
+      <c r="C35">
+        <v>2.75</v>
+      </c>
+      <c r="D35">
+        <v>0.8</v>
+      </c>
+      <c r="E35" s="44">
+        <f t="shared" si="1"/>
+        <v>12100410.396797085</v>
+      </c>
+      <c r="F35" s="44">
+        <f t="shared" si="0"/>
+        <v>21068038.174091958</v>
+      </c>
+      <c r="G35" s="44">
+        <f t="shared" si="0"/>
+        <v>36681585</v>
+      </c>
+      <c r="H35" s="44">
+        <f t="shared" si="0"/>
+        <v>43850656.888763405</v>
+      </c>
+      <c r="I35" s="44">
+        <f t="shared" si="0"/>
+        <v>50736569.601284206</v>
+      </c>
+      <c r="J35" s="44">
+        <f t="shared" si="0"/>
+        <v>63866348.968689315</v>
+      </c>
+      <c r="K35" s="44">
+        <f t="shared" si="0"/>
+        <v>111197772.14071864</v>
+      </c>
+      <c r="L35" s="44">
+        <f t="shared" si="0"/>
+        <v>132930334.19732401</v>
+      </c>
+      <c r="M35" s="44">
+        <f t="shared" si="0"/>
+        <v>231445154.62924495</v>
+      </c>
+    </row>
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A36" t="s">
+        <v>143</v>
+      </c>
+      <c r="B36" s="43">
+        <v>144155</v>
+      </c>
+      <c r="C36">
+        <v>3.02</v>
+      </c>
+      <c r="D36">
+        <v>0.6</v>
+      </c>
+      <c r="E36" s="44">
+        <f t="shared" si="1"/>
+        <v>62747.108225976386</v>
+      </c>
+      <c r="F36" s="44">
+        <f t="shared" si="0"/>
+        <v>95106.831438733279</v>
+      </c>
+      <c r="G36" s="44">
+        <f t="shared" si="0"/>
+        <v>144155</v>
+      </c>
+      <c r="H36" s="44">
+        <f t="shared" si="0"/>
+        <v>164807.02440145935</v>
+      </c>
+      <c r="I36" s="44">
+        <f t="shared" si="0"/>
+        <v>183858.81888771086</v>
+      </c>
+      <c r="J36" s="44">
+        <f t="shared" si="0"/>
+        <v>218498.12164530641</v>
+      </c>
+      <c r="K36" s="44">
+        <f t="shared" si="0"/>
+        <v>331181.2227291952</v>
+      </c>
+      <c r="L36" s="44">
+        <f t="shared" si="0"/>
+        <v>378627.11564382503</v>
+      </c>
+      <c r="M36" s="44">
+        <f t="shared" si="0"/>
+        <v>573891.39171139395</v>
+      </c>
+    </row>
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A37" t="s">
+        <v>144</v>
+      </c>
+      <c r="B37" s="43">
+        <v>6595713</v>
+      </c>
+      <c r="C37">
+        <v>1.69</v>
+      </c>
+      <c r="D37">
+        <v>0.7</v>
+      </c>
+      <c r="E37" s="44">
+        <f t="shared" si="1"/>
+        <v>2499307.8655119995</v>
+      </c>
+      <c r="F37" s="44">
+        <f t="shared" si="0"/>
+        <v>4060137.6059882189</v>
+      </c>
+      <c r="G37" s="44">
+        <f t="shared" si="0"/>
+        <v>6595713</v>
+      </c>
+      <c r="H37" s="44">
+        <f t="shared" si="0"/>
+        <v>7710787.9319168562</v>
+      </c>
+      <c r="I37" s="44">
+        <f t="shared" si="0"/>
+        <v>8760434.1849103682</v>
+      </c>
+      <c r="J37" s="44">
+        <f t="shared" si="0"/>
+        <v>10714767.379855949</v>
+      </c>
+      <c r="K37" s="44">
+        <f t="shared" si="0"/>
+        <v>17406190.961375237</v>
+      </c>
+      <c r="L37" s="44">
+        <f t="shared" si="0"/>
+        <v>20348891.348912913</v>
+      </c>
+      <c r="M37" s="44">
+        <f t="shared" si="0"/>
+        <v>33056871.522694372</v>
+      </c>
+    </row>
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A38" t="s">
+        <v>145</v>
+      </c>
+      <c r="B38" s="43">
+        <v>1626125</v>
+      </c>
+      <c r="C38">
+        <v>1.52</v>
+      </c>
+      <c r="D38">
+        <v>0.7</v>
+      </c>
+      <c r="E38" s="44">
+        <f t="shared" si="1"/>
+        <v>616186.15042918036</v>
+      </c>
+      <c r="F38" s="44">
+        <f t="shared" si="0"/>
+        <v>1000997.354575251</v>
+      </c>
+      <c r="G38" s="44">
+        <f t="shared" si="0"/>
+        <v>1626125</v>
+      </c>
+      <c r="H38" s="44">
+        <f t="shared" si="0"/>
+        <v>1901038.6027694501</v>
+      </c>
+      <c r="I38" s="44">
+        <f t="shared" si="0"/>
+        <v>2159821.2413028539</v>
+      </c>
+      <c r="J38" s="44">
+        <f t="shared" si="0"/>
+        <v>2641647.856049567</v>
+      </c>
+      <c r="K38" s="44">
+        <f t="shared" si="0"/>
+        <v>4291369.6028111456</v>
+      </c>
+      <c r="L38" s="44">
+        <f t="shared" si="0"/>
+        <v>5016870.9500778774</v>
+      </c>
+      <c r="M38" s="44">
+        <f t="shared" si="0"/>
+        <v>8149930.9028214812</v>
+      </c>
+    </row>
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A39" t="s">
+        <v>146</v>
+      </c>
+      <c r="B39" s="43">
+        <v>980551</v>
+      </c>
+      <c r="C39">
+        <v>2.0299999999999998</v>
+      </c>
+      <c r="D39">
+        <v>0.7</v>
+      </c>
+      <c r="E39" s="44">
+        <f t="shared" si="1"/>
+        <v>371559.34875208436</v>
+      </c>
+      <c r="F39" s="44">
+        <f t="shared" si="0"/>
+        <v>603599.94282488548</v>
+      </c>
+      <c r="G39" s="44">
+        <f t="shared" si="0"/>
+        <v>980551</v>
+      </c>
+      <c r="H39" s="44">
+        <f t="shared" si="0"/>
+        <v>1146323.5009511488</v>
+      </c>
+      <c r="I39" s="44">
+        <f t="shared" si="0"/>
+        <v>1302369.0540276761</v>
+      </c>
+      <c r="J39" s="44">
+        <f t="shared" si="0"/>
+        <v>1592909.7989990062</v>
+      </c>
+      <c r="K39" s="44">
+        <f t="shared" si="0"/>
+        <v>2587689.6028325441</v>
+      </c>
+      <c r="L39" s="44">
+        <f t="shared" si="0"/>
+        <v>3025165.8556198403</v>
+      </c>
+      <c r="M39" s="44">
+        <f t="shared" si="0"/>
+        <v>4914396.4312045546</v>
+      </c>
+    </row>
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A40" t="s">
+        <v>147</v>
+      </c>
+      <c r="B40" s="43">
+        <v>123670</v>
+      </c>
+      <c r="C40">
+        <v>3.02</v>
+      </c>
+      <c r="D40">
+        <v>0.6</v>
+      </c>
+      <c r="E40" s="44">
+        <f t="shared" si="1"/>
+        <v>53830.494081415833</v>
+      </c>
+      <c r="F40" s="44">
+        <f t="shared" si="0"/>
+        <v>81591.771662641913</v>
+      </c>
+      <c r="G40" s="44">
+        <f t="shared" si="0"/>
+        <v>123670</v>
+      </c>
+      <c r="H40" s="44">
+        <f t="shared" si="0"/>
+        <v>141387.28942963114</v>
+      </c>
+      <c r="I40" s="44">
+        <f t="shared" si="0"/>
+        <v>157731.74799239152</v>
+      </c>
+      <c r="J40" s="44">
+        <f t="shared" si="0"/>
+        <v>187448.66778034091</v>
+      </c>
+      <c r="K40" s="44">
+        <f t="shared" si="0"/>
+        <v>284119.05112496665</v>
+      </c>
+      <c r="L40" s="44">
+        <f t="shared" si="0"/>
+        <v>324822.69357061386</v>
+      </c>
+      <c r="M40" s="44">
+        <f t="shared" si="0"/>
+        <v>492339.1378235101</v>
+      </c>
+    </row>
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A41" t="s">
+        <v>149</v>
+      </c>
+      <c r="B41" s="43">
+        <v>718300</v>
+      </c>
+      <c r="C41">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D41">
+        <v>0.8</v>
+      </c>
+      <c r="E41" s="44">
+        <f t="shared" si="1"/>
+        <v>236950.63307704253</v>
+      </c>
+      <c r="F41" s="44">
+        <f t="shared" si="1"/>
+        <v>412555.01419718517</v>
+      </c>
+      <c r="G41" s="44">
+        <f t="shared" si="1"/>
+        <v>718300</v>
+      </c>
+      <c r="H41" s="44">
+        <f t="shared" si="1"/>
+        <v>858685.00074897939</v>
+      </c>
+      <c r="I41" s="44">
+        <f t="shared" si="1"/>
+        <v>993525.16922598751</v>
+      </c>
+      <c r="J41" s="44">
+        <f t="shared" si="1"/>
+        <v>1250632.939231212</v>
+      </c>
+      <c r="K41" s="44">
+        <f t="shared" si="1"/>
+        <v>2177478.4194488376</v>
+      </c>
+      <c r="L41" s="44">
+        <f t="shared" si="1"/>
+        <v>2603046.1620984436</v>
+      </c>
+      <c r="M41" s="44">
+        <f t="shared" si="1"/>
+        <v>4532166.6054012291</v>
+      </c>
+    </row>
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A42" t="s">
+        <v>150</v>
+      </c>
+      <c r="B42" s="43">
+        <v>7495642</v>
+      </c>
+      <c r="C42">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D42">
+        <v>0.6</v>
+      </c>
+      <c r="E42" s="44">
+        <f t="shared" si="1"/>
+        <v>3262667.6826830432</v>
+      </c>
+      <c r="F42" s="44">
+        <f t="shared" si="1"/>
+        <v>4945279.4576607794</v>
+      </c>
+      <c r="G42" s="44">
+        <f t="shared" si="1"/>
+        <v>7495642</v>
+      </c>
+      <c r="H42" s="44">
+        <f t="shared" si="1"/>
+        <v>8569487.3850966208</v>
+      </c>
+      <c r="I42" s="44">
+        <f t="shared" si="1"/>
+        <v>9560125.4547197036</v>
+      </c>
+      <c r="J42" s="44">
+        <f t="shared" si="1"/>
+        <v>11361268.756031133</v>
+      </c>
+      <c r="K42" s="44">
+        <f t="shared" si="1"/>
+        <v>17220463.270093374</v>
+      </c>
+      <c r="L42" s="44">
+        <f t="shared" si="1"/>
+        <v>19687512.124856662</v>
+      </c>
+      <c r="M42" s="44">
+        <f t="shared" si="1"/>
+        <v>29840688.281019572</v>
+      </c>
+    </row>
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A43" t="s">
+        <v>151</v>
+      </c>
+      <c r="B43" s="43">
+        <v>969104</v>
+      </c>
+      <c r="C43">
+        <v>1.52</v>
+      </c>
+      <c r="D43">
+        <v>0.7</v>
+      </c>
+      <c r="E43" s="44">
+        <f t="shared" si="1"/>
+        <v>367221.74686787324</v>
+      </c>
+      <c r="F43" s="44">
+        <f t="shared" si="1"/>
+        <v>596553.48777510587</v>
+      </c>
+      <c r="G43" s="44">
+        <f t="shared" si="1"/>
+        <v>969104</v>
+      </c>
+      <c r="H43" s="44">
+        <f t="shared" si="1"/>
+        <v>1132941.2647233671</v>
+      </c>
+      <c r="I43" s="44">
+        <f t="shared" si="1"/>
+        <v>1287165.1344340448</v>
+      </c>
+      <c r="J43" s="44">
+        <f t="shared" si="1"/>
+        <v>1574314.0926368264</v>
+      </c>
+      <c r="K43" s="44">
+        <f t="shared" si="1"/>
+        <v>2557480.7887233095</v>
+      </c>
+      <c r="L43" s="44">
+        <f t="shared" si="1"/>
+        <v>2989849.9224870605</v>
+      </c>
+      <c r="M43" s="44">
+        <f t="shared" si="1"/>
+        <v>4857025.5285712406</v>
+      </c>
+    </row>
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A44" t="s">
+        <v>152</v>
+      </c>
+      <c r="B44" s="43">
+        <v>29456</v>
+      </c>
+      <c r="C44">
+        <v>2.33</v>
+      </c>
+      <c r="D44">
+        <v>0.7</v>
+      </c>
+      <c r="E44" s="44">
+        <f t="shared" si="1"/>
+        <v>11161.736795782572</v>
+      </c>
+      <c r="F44" s="44">
+        <f t="shared" si="1"/>
+        <v>18132.294919743927</v>
+      </c>
+      <c r="G44" s="44">
+        <f t="shared" si="1"/>
+        <v>29456</v>
+      </c>
+      <c r="H44" s="44">
+        <f t="shared" si="1"/>
+        <v>34435.847848828918</v>
+      </c>
+      <c r="I44" s="44">
+        <f t="shared" si="1"/>
+        <v>39123.495723770851</v>
+      </c>
+      <c r="J44" s="44">
+        <f t="shared" si="1"/>
+        <v>47851.413174138543</v>
+      </c>
+      <c r="K44" s="44">
+        <f t="shared" si="1"/>
+        <v>77734.850039452736</v>
+      </c>
+      <c r="L44" s="44">
+        <f t="shared" si="1"/>
+        <v>90876.747301403011</v>
+      </c>
+      <c r="M44" s="44">
+        <f t="shared" si="1"/>
+        <v>147629.71153724933</v>
+      </c>
+    </row>
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A45" t="s">
+        <v>153</v>
+      </c>
+      <c r="B45" s="43">
+        <v>21715</v>
+      </c>
+      <c r="C45">
+        <v>3.02</v>
+      </c>
+      <c r="D45">
+        <v>0.6</v>
+      </c>
+      <c r="E45" s="44">
+        <f t="shared" si="1"/>
+        <v>9452.0027409876675</v>
+      </c>
+      <c r="F45" s="44">
+        <f t="shared" si="1"/>
+        <v>14326.557141216699</v>
+      </c>
+      <c r="G45" s="44">
+        <f t="shared" si="1"/>
+        <v>21715</v>
+      </c>
+      <c r="H45" s="44">
+        <f t="shared" si="1"/>
+        <v>24825.948006504732</v>
+      </c>
+      <c r="I45" s="44">
+        <f t="shared" si="1"/>
+        <v>27695.843031089047</v>
+      </c>
+      <c r="J45" s="44">
+        <f t="shared" si="1"/>
+        <v>32913.785241773294</v>
+      </c>
+      <c r="K45" s="44">
+        <f t="shared" si="1"/>
+        <v>49887.969557521232</v>
+      </c>
+      <c r="L45" s="44">
+        <f t="shared" si="1"/>
+        <v>57035.051272627803</v>
+      </c>
+      <c r="M45" s="44">
+        <f t="shared" si="1"/>
+        <v>86448.97208569193</v>
+      </c>
+    </row>
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A46" t="s">
+        <v>154</v>
+      </c>
+      <c r="B46" s="43">
+        <v>50244</v>
+      </c>
+      <c r="C46">
+        <v>1.52</v>
+      </c>
+      <c r="D46">
+        <v>0.7</v>
+      </c>
+      <c r="E46" s="44">
+        <f t="shared" si="1"/>
+        <v>19038.915791937114</v>
+      </c>
+      <c r="F46" s="44">
+        <f t="shared" si="1"/>
+        <v>30928.809952050986</v>
+      </c>
+      <c r="G46" s="44">
+        <f t="shared" si="1"/>
+        <v>50244</v>
+      </c>
+      <c r="H46" s="44">
+        <f t="shared" si="1"/>
+        <v>58738.27876549973</v>
+      </c>
+      <c r="I46" s="44">
+        <f t="shared" si="1"/>
+        <v>66734.143099712877</v>
+      </c>
+      <c r="J46" s="44">
+        <f t="shared" si="1"/>
+        <v>81621.618805045393</v>
+      </c>
+      <c r="K46" s="44">
+        <f t="shared" si="1"/>
+        <v>132594.7109377466</v>
+      </c>
+      <c r="L46" s="44">
+        <f t="shared" si="1"/>
+        <v>155011.24699252081</v>
+      </c>
+      <c r="M46" s="44">
+        <f t="shared" si="1"/>
+        <v>251816.5136636867</v>
+      </c>
+    </row>
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A47" t="s">
+        <v>155</v>
+      </c>
+      <c r="B47" s="43">
+        <v>33067253</v>
+      </c>
+      <c r="C47">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D47">
+        <v>0.65</v>
+      </c>
+      <c r="E47" s="44">
+        <f t="shared" si="1"/>
+        <v>13429477.745083958</v>
+      </c>
+      <c r="F47" s="44">
+        <f t="shared" si="1"/>
+        <v>21073109.363702379</v>
+      </c>
+      <c r="G47" s="44">
+        <f t="shared" si="1"/>
+        <v>33067253</v>
+      </c>
+      <c r="H47" s="44">
+        <f t="shared" si="1"/>
+        <v>38228708.534664541</v>
+      </c>
+      <c r="I47" s="44">
+        <f t="shared" si="1"/>
+        <v>43038530.714245498</v>
+      </c>
+      <c r="J47" s="44">
+        <f t="shared" si="1"/>
+        <v>51888081.729857251</v>
+      </c>
+      <c r="K47" s="44">
+        <f t="shared" si="1"/>
+        <v>81421127.591225848</v>
+      </c>
+      <c r="L47" s="44">
+        <f t="shared" si="1"/>
+        <v>94130121.883686736</v>
+      </c>
+      <c r="M47" s="44">
+        <f t="shared" si="1"/>
+        <v>147705993.52604714</v>
+      </c>
+    </row>
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A48" t="s">
+        <v>156</v>
+      </c>
+      <c r="B48" s="43">
+        <v>411911</v>
+      </c>
+      <c r="C48">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D48">
+        <v>0.65</v>
+      </c>
+      <c r="E48" s="44">
+        <f t="shared" si="1"/>
+        <v>167287.84841774666</v>
+      </c>
+      <c r="F48" s="44">
+        <f t="shared" si="1"/>
+        <v>262502.77127985231</v>
+      </c>
+      <c r="G48" s="44">
+        <f t="shared" si="1"/>
+        <v>411911</v>
+      </c>
+      <c r="H48" s="44">
+        <f t="shared" si="1"/>
+        <v>476206.03868190094</v>
+      </c>
+      <c r="I48" s="44">
+        <f t="shared" si="1"/>
+        <v>536120.86329141329</v>
+      </c>
+      <c r="J48" s="44">
+        <f t="shared" si="1"/>
+        <v>646357.64069749706</v>
+      </c>
+      <c r="K48" s="44">
+        <f t="shared" si="1"/>
+        <v>1014243.8528906356</v>
+      </c>
+      <c r="L48" s="44">
+        <f t="shared" si="1"/>
+        <v>1172556.808248671</v>
+      </c>
+      <c r="M48" s="44">
+        <f t="shared" si="1"/>
+        <v>1839938.8512649538</v>
+      </c>
+    </row>
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A49" t="s">
+        <v>157</v>
+      </c>
+      <c r="B49" s="43">
+        <v>585966</v>
+      </c>
+      <c r="C49">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D49">
+        <v>0.65</v>
+      </c>
+      <c r="E49" s="44">
+        <f t="shared" si="1"/>
+        <v>237976.14384163893</v>
+      </c>
+      <c r="F49" s="44">
+        <f t="shared" si="1"/>
+        <v>373424.5962738794</v>
+      </c>
+      <c r="G49" s="44">
+        <f t="shared" si="1"/>
+        <v>585966</v>
+      </c>
+      <c r="H49" s="44">
+        <f t="shared" si="1"/>
+        <v>677429.22054103622</v>
+      </c>
+      <c r="I49" s="44">
+        <f t="shared" si="1"/>
+        <v>762661.34621172119</v>
+      </c>
+      <c r="J49" s="44">
+        <f t="shared" si="1"/>
+        <v>919479.21101633494</v>
+      </c>
+      <c r="K49" s="44">
+        <f t="shared" si="1"/>
+        <v>1442817.5346201344</v>
+      </c>
+      <c r="L49" s="44">
+        <f t="shared" si="1"/>
+        <v>1668026.4006113959</v>
+      </c>
+      <c r="M49" s="44">
+        <f t="shared" si="1"/>
+        <v>2617413.9775833129</v>
+      </c>
+    </row>
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A50" t="s">
+        <v>158</v>
+      </c>
+      <c r="B50" s="43">
+        <v>326304</v>
+      </c>
+      <c r="C50">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D50">
+        <v>0.65</v>
+      </c>
+      <c r="E50" s="44">
+        <f t="shared" si="1"/>
+        <v>132520.60297031252</v>
+      </c>
+      <c r="F50" s="44">
+        <f t="shared" si="1"/>
+        <v>207947.11546839227</v>
+      </c>
+      <c r="G50" s="44">
+        <f t="shared" si="1"/>
+        <v>326304</v>
+      </c>
+      <c r="H50" s="44">
+        <f t="shared" si="1"/>
+        <v>377236.67308243527</v>
+      </c>
+      <c r="I50" s="44">
+        <f t="shared" si="1"/>
+        <v>424699.46705827554</v>
+      </c>
+      <c r="J50" s="44">
+        <f t="shared" si="1"/>
+        <v>512025.85896020272</v>
+      </c>
+      <c r="K50" s="44">
+        <f t="shared" si="1"/>
+        <v>803454.69330419914</v>
+      </c>
+      <c r="L50" s="44">
+        <f t="shared" si="1"/>
+        <v>928865.6451485256</v>
+      </c>
+      <c r="M50" s="44">
+        <f t="shared" si="1"/>
+        <v>1457546.4285322789</v>
+      </c>
+    </row>
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A51" t="s">
+        <v>166</v>
+      </c>
+      <c r="B51" s="43">
+        <v>178050</v>
+      </c>
+      <c r="C51">
+        <v>2.4700000000000002</v>
+      </c>
+      <c r="D51">
+        <v>0.65</v>
+      </c>
+      <c r="E51" s="44">
+        <f t="shared" si="1"/>
+        <v>72310.76958561386</v>
+      </c>
+      <c r="F51" s="44">
+        <f t="shared" si="1"/>
+        <v>113467.75984709732</v>
+      </c>
+      <c r="G51" s="44">
+        <f t="shared" si="1"/>
+        <v>178050</v>
+      </c>
+      <c r="H51" s="44">
+        <f t="shared" si="1"/>
+        <v>205841.75996104124</v>
+      </c>
+      <c r="I51" s="44">
+        <f t="shared" si="1"/>
+        <v>231740.15675482361</v>
+      </c>
+      <c r="J51" s="44">
+        <f t="shared" si="1"/>
+        <v>279390.39726103295</v>
+      </c>
+      <c r="K51" s="44">
+        <f t="shared" si="1"/>
+        <v>438410.52559212467</v>
+      </c>
+      <c r="L51" s="44">
+        <f t="shared" si="1"/>
+        <v>506841.86561824247</v>
+      </c>
+      <c r="M51" s="44">
+        <f t="shared" si="1"/>
+        <v>795320.13582478999</v>
+      </c>
+    </row>
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A52" t="s">
+        <v>159</v>
+      </c>
+      <c r="B52" s="43">
+        <v>223100</v>
+      </c>
+      <c r="C52">
+        <v>4.99</v>
+      </c>
+      <c r="D52">
+        <v>0.7</v>
+      </c>
+      <c r="E52" s="44">
+        <f t="shared" si="1"/>
+        <v>84539.091497117464</v>
+      </c>
+      <c r="F52" s="44">
+        <f t="shared" si="1"/>
+        <v>137334.15930862541</v>
+      </c>
+      <c r="G52" s="44">
+        <f t="shared" si="1"/>
+        <v>223100</v>
+      </c>
+      <c r="H52" s="44">
+        <f t="shared" si="1"/>
+        <v>260817.4108865335</v>
+      </c>
+      <c r="I52" s="44">
+        <f t="shared" si="1"/>
+        <v>296321.69663135783</v>
+      </c>
+      <c r="J52" s="44">
+        <f t="shared" si="1"/>
+        <v>362427.01925415226</v>
+      </c>
+      <c r="K52" s="44">
+        <f t="shared" si="1"/>
+        <v>588764.42978686537</v>
+      </c>
+      <c r="L52" s="44">
+        <f t="shared" si="1"/>
+        <v>688301.27386417065</v>
+      </c>
+      <c r="M52" s="44">
+        <f t="shared" si="1"/>
+        <v>1118148.7182224444</v>
+      </c>
+    </row>
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A53" t="s">
+        <v>160</v>
+      </c>
+      <c r="B53" s="43">
+        <v>27883640</v>
+      </c>
+      <c r="C53">
+        <v>1.8</v>
+      </c>
+      <c r="D53">
+        <v>0.6</v>
+      </c>
+      <c r="E53" s="44">
+        <f t="shared" si="1"/>
+        <v>12137059.254373169</v>
+      </c>
+      <c r="F53" s="44">
+        <f t="shared" si="1"/>
+        <v>18396341.780571751</v>
+      </c>
+      <c r="G53" s="44">
+        <f t="shared" si="1"/>
+        <v>27883640</v>
+      </c>
+      <c r="H53" s="44">
+        <f t="shared" si="1"/>
+        <v>31878323.595307186</v>
+      </c>
+      <c r="I53" s="44">
+        <f t="shared" si="1"/>
+        <v>35563477.622629322</v>
+      </c>
+      <c r="J53" s="44">
+        <f t="shared" si="1"/>
+        <v>42263695.082611993</v>
+      </c>
+      <c r="K53" s="44">
+        <f t="shared" si="1"/>
+        <v>64059782.798659056</v>
+      </c>
+      <c r="L53" s="44">
+        <f t="shared" si="1"/>
+        <v>73237155.74798505</v>
+      </c>
+      <c r="M53" s="44">
+        <f t="shared" si="1"/>
+        <v>111006770.25132319</v>
+      </c>
+    </row>
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A54" t="s">
+        <v>161</v>
+      </c>
+      <c r="B54" s="43">
+        <v>11065762</v>
+      </c>
+      <c r="C54">
+        <v>1.8</v>
+      </c>
+      <c r="D54">
+        <v>0.6</v>
+      </c>
+      <c r="E54" s="44">
+        <f t="shared" si="1"/>
+        <v>4816652.6712004226</v>
+      </c>
+      <c r="F54" s="44">
+        <f t="shared" si="1"/>
+        <v>7300680.2488650419</v>
+      </c>
+      <c r="G54" s="44">
+        <f t="shared" si="1"/>
+        <v>11065762</v>
+      </c>
+      <c r="H54" s="44">
+        <f t="shared" si="1"/>
+        <v>12651072.165063588</v>
+      </c>
+      <c r="I54" s="44">
+        <f t="shared" si="1"/>
+        <v>14113543.972893851</v>
+      </c>
+      <c r="J54" s="44">
+        <f t="shared" si="1"/>
+        <v>16772558.784461234</v>
+      </c>
+      <c r="K54" s="44">
+        <f t="shared" si="1"/>
+        <v>25422445.212377403</v>
+      </c>
+      <c r="L54" s="44">
+        <f t="shared" si="1"/>
+        <v>29064531.569914639</v>
+      </c>
+      <c r="M54" s="44">
+        <f t="shared" si="1"/>
+        <v>44053591.998384088</v>
+      </c>
+    </row>
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A55" t="s">
+        <v>162</v>
+      </c>
+      <c r="B55" s="43">
+        <v>6015366</v>
+      </c>
+      <c r="C55">
+        <v>1.8</v>
+      </c>
+      <c r="D55">
+        <v>0.6</v>
+      </c>
+      <c r="E55" s="44">
+        <f t="shared" si="1"/>
+        <v>2618340.1298661763</v>
+      </c>
+      <c r="F55" s="44">
+        <f t="shared" si="1"/>
+        <v>3968661.5115971509</v>
+      </c>
+      <c r="G55" s="44">
+        <f t="shared" si="1"/>
+        <v>6015366</v>
+      </c>
+      <c r="H55" s="44">
+        <f t="shared" si="1"/>
+        <v>6877143.152479684</v>
+      </c>
+      <c r="I55" s="44">
+        <f t="shared" si="1"/>
+        <v>7672145.1766313603</v>
+      </c>
+      <c r="J55" s="44">
+        <f t="shared" si="1"/>
+        <v>9117589.8998233862</v>
+      </c>
+      <c r="K55" s="44">
+        <f t="shared" si="1"/>
+        <v>13819682.057810189</v>
+      </c>
+      <c r="L55" s="44">
+        <f t="shared" si="1"/>
+        <v>15799526.05266507</v>
+      </c>
+      <c r="M55" s="44">
+        <f t="shared" si="1"/>
+        <v>23947603.381037086</v>
+      </c>
+    </row>
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A56" t="s">
+        <v>165</v>
+      </c>
+      <c r="B56" s="43">
+        <v>1779507</v>
+      </c>
+      <c r="C56">
+        <v>1.41</v>
+      </c>
+      <c r="D56">
+        <v>0.6</v>
+      </c>
+      <c r="E56" s="44">
+        <f t="shared" si="1"/>
+        <v>774575.410619698</v>
+      </c>
+      <c r="F56" s="44">
+        <f t="shared" si="1"/>
+        <v>1174036.7818878703</v>
+      </c>
+      <c r="G56" s="44">
+        <f t="shared" si="1"/>
+        <v>1779507</v>
+      </c>
+      <c r="H56" s="44">
+        <f t="shared" si="1"/>
+        <v>2034443.8526001018</v>
+      </c>
+      <c r="I56" s="44">
+        <f t="shared" si="1"/>
+        <v>2269626.8268350991</v>
+      </c>
+      <c r="J56" s="44">
+        <f t="shared" si="1"/>
+        <v>2697228.2401212188</v>
+      </c>
+      <c r="K56" s="44">
+        <f t="shared" si="1"/>
+        <v>4088233.5272114179</v>
+      </c>
+      <c r="L56" s="44">
+        <f t="shared" si="1"/>
+        <v>4673924.6136311339</v>
+      </c>
+      <c r="M56" s="44">
+        <f t="shared" si="1"/>
+        <v>7084344.9675014224</v>
+      </c>
+    </row>
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A57" t="s">
+        <v>163</v>
+      </c>
+      <c r="B57" s="43">
+        <v>2929758</v>
+      </c>
+      <c r="C57">
+        <v>1.5</v>
+      </c>
+      <c r="D57">
+        <v>0.6</v>
+      </c>
+      <c r="E57" s="44">
+        <f t="shared" si="1"/>
+        <v>1275251.238610663</v>
+      </c>
+      <c r="F57" s="44">
+        <f t="shared" si="1"/>
+        <v>1932919.4288250864</v>
+      </c>
+      <c r="G57" s="44">
+        <f t="shared" si="1"/>
+        <v>2929758</v>
+      </c>
+      <c r="H57" s="44">
+        <f t="shared" si="1"/>
+        <v>3349482.8358112499</v>
+      </c>
+      <c r="I57" s="44">
+        <f t="shared" si="1"/>
+        <v>3736685.1341044153</v>
+      </c>
+      <c r="J57" s="44">
+        <f t="shared" si="1"/>
+        <v>4440682.7364663705</v>
+      </c>
+      <c r="K57" s="44">
+        <f t="shared" si="1"/>
+        <v>6730816.3902788069</v>
+      </c>
+      <c r="L57" s="44">
+        <f t="shared" si="1"/>
+        <v>7695090.8471743716</v>
+      </c>
+      <c r="M57" s="44">
+        <f t="shared" si="1"/>
+        <v>11663576.67786473</v>
+      </c>
+    </row>
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A58" t="s">
+        <v>164</v>
+      </c>
+      <c r="B58" s="43">
+        <v>7405996</v>
+      </c>
+      <c r="C58">
+        <v>3.02</v>
+      </c>
+      <c r="D58">
+        <v>0.65</v>
+      </c>
+      <c r="E58" s="44">
+        <f t="shared" si="1"/>
+        <v>3007768.9992023474</v>
+      </c>
+      <c r="F58" s="44">
+        <f t="shared" si="1"/>
+        <v>4719695.4538419731</v>
+      </c>
+      <c r="G58" s="44">
+        <f t="shared" si="1"/>
+        <v>7405996</v>
+      </c>
+      <c r="H58" s="44">
+        <f t="shared" si="1"/>
+        <v>8561995.2311397456</v>
+      </c>
+      <c r="I58" s="44">
+        <f t="shared" si="1"/>
+        <v>9639239.9548755772</v>
+      </c>
+      <c r="J58" s="44">
+        <f t="shared" si="1"/>
+        <v>11621253.38137389</v>
+      </c>
+      <c r="K58" s="44">
+        <f t="shared" si="1"/>
+        <v>18235701.201309595</v>
+      </c>
+      <c r="L58" s="44">
+        <f t="shared" si="1"/>
+        <v>21082105.191807028</v>
+      </c>
+      <c r="M58" s="44">
+        <f t="shared" si="1"/>
+        <v>33081368.967356648</v>
+      </c>
+    </row>
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D60" t="s">
+        <v>168</v>
+      </c>
+      <c r="E60" s="45">
+        <f>E24</f>
+        <v>0.25</v>
+      </c>
+      <c r="F60" s="45">
+        <f t="shared" ref="F60:M60" si="2">F24</f>
+        <v>0.5</v>
+      </c>
+      <c r="G60" s="45">
+        <f t="shared" si="2"/>
+        <v>1</v>
+      </c>
+      <c r="H60" s="45">
+        <f t="shared" si="2"/>
+        <v>1.25</v>
+      </c>
+      <c r="I60" s="45">
+        <f t="shared" si="2"/>
+        <v>1.5</v>
+      </c>
+      <c r="J60" s="45">
+        <f t="shared" si="2"/>
+        <v>2</v>
+      </c>
+      <c r="K60" s="45">
+        <f t="shared" si="2"/>
+        <v>4</v>
+      </c>
+      <c r="L60" s="45">
+        <f t="shared" si="2"/>
+        <v>5</v>
+      </c>
+      <c r="M60" s="45">
+        <f t="shared" si="2"/>
+        <v>10</v>
+      </c>
+    </row>
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D61" t="s">
+        <v>112</v>
+      </c>
+      <c r="E61" s="44">
+        <f>SUM(E25:E58)</f>
+        <v>103661944.99376373</v>
+      </c>
+      <c r="F61" s="44">
+        <f t="shared" ref="F61:M61" si="3">SUM(F25:F58)</f>
+        <v>163252732.89508671</v>
+      </c>
+      <c r="G61" s="44">
+        <f t="shared" si="3"/>
+        <v>257800646</v>
+      </c>
+      <c r="H61" s="44">
+        <f t="shared" si="3"/>
+        <v>298830505.00587934</v>
+      </c>
+      <c r="I61" s="44">
+        <f t="shared" si="3"/>
+        <v>337232658.66429305</v>
+      </c>
+      <c r="J61" s="44">
+        <f t="shared" si="3"/>
+        <v>408279669.36056608</v>
+      </c>
+      <c r="K61" s="44">
+        <f t="shared" si="3"/>
+        <v>648555689.20624173</v>
+      </c>
+      <c r="L61" s="44">
+        <f t="shared" si="3"/>
+        <v>753254554.49843431</v>
+      </c>
+      <c r="M61" s="44">
+        <f t="shared" si="3"/>
+        <v>1201614609.967025</v>
+      </c>
+    </row>
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D62" t="s">
+        <v>170</v>
+      </c>
+      <c r="E62" s="45">
+        <f>LOG(E60)</f>
+        <v>-0.6020599913279624</v>
+      </c>
+      <c r="F62" s="45">
+        <f t="shared" ref="F62:M62" si="4">LOG(F60)</f>
+        <v>-0.3010299956639812</v>
+      </c>
+      <c r="G62" s="45">
+        <f t="shared" si="4"/>
+        <v>0</v>
+      </c>
+      <c r="H62" s="45">
+        <f t="shared" si="4"/>
+        <v>9.691001300805642E-2</v>
+      </c>
+      <c r="I62" s="45">
+        <f t="shared" si="4"/>
+        <v>0.17609125905568124</v>
+      </c>
+      <c r="J62" s="45">
+        <f t="shared" si="4"/>
+        <v>0.3010299956639812</v>
+      </c>
+      <c r="K62" s="45">
+        <f t="shared" si="4"/>
+        <v>0.6020599913279624</v>
+      </c>
+      <c r="L62" s="45">
+        <f t="shared" si="4"/>
+        <v>0.69897000433601886</v>
+      </c>
+      <c r="M62" s="45">
+        <f t="shared" si="4"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="D63" t="s">
+        <v>169</v>
+      </c>
+      <c r="E63">
+        <f>LOG(E61)</f>
+        <v>8.0156193531831796</v>
+      </c>
+      <c r="F63">
+        <f t="shared" ref="F63:M63" si="5">LOG(F61)</f>
+        <v>8.2128604602155431</v>
+      </c>
+      <c r="G63">
+        <f t="shared" si="5"/>
+        <v>8.411284001279153</v>
+      </c>
+      <c r="H63">
+        <f t="shared" si="5"/>
+        <v>8.4754249287508117</v>
+      </c>
+      <c r="I63">
+        <f t="shared" si="5"/>
+        <v>8.5279296264238802</v>
+      </c>
+      <c r="J63">
+        <f t="shared" si="5"/>
+        <v>8.6109577543918885</v>
+      </c>
+      <c r="K63">
+        <f t="shared" si="5"/>
+        <v>8.8119472733677942</v>
+      </c>
+      <c r="L63">
+        <f t="shared" si="5"/>
+        <v>8.8769417662830747</v>
+      </c>
+      <c r="M63">
+        <f t="shared" si="5"/>
+        <v>9.0797652001107316</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <drawing r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -1738,26 +4965,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="3" t="s">
+      <c r="A1" s="42" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="3"/>
-      <c r="C1" s="3"/>
-      <c r="D1" s="3"/>
-      <c r="E1" s="3"/>
-      <c r="F1" s="3"/>
-      <c r="G1" s="3"/>
+      <c r="B1" s="42"/>
+      <c r="C1" s="42"/>
+      <c r="D1" s="42"/>
+      <c r="E1" s="42"/>
+      <c r="F1" s="42"/>
+      <c r="G1" s="42"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="3" t="s">
+      <c r="A2" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="3"/>
-      <c r="C2" s="3"/>
-      <c r="D2" s="3"/>
-      <c r="E2" s="3"/>
-      <c r="F2" s="3"/>
-      <c r="G2" s="3"/>
+      <c r="B2" s="42"/>
+      <c r="C2" s="42"/>
+      <c r="D2" s="42"/>
+      <c r="E2" s="42"/>
+      <c r="F2" s="42"/>
+      <c r="G2" s="42"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -1769,14 +4996,14 @@
       <c r="C3" t="s">
         <v>67</v>
       </c>
-      <c r="D3" s="4">
+      <c r="D3" s="3">
         <f>B3*1000/(24*3600)</f>
         <v>18.287037037037038</v>
       </c>
-      <c r="E3" s="5" t="s">
+      <c r="E3" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F3" s="6">
+      <c r="F3" s="5">
         <f>B3*1000/24</f>
         <v>65833.333333333328</v>
       </c>
@@ -1794,14 +5021,14 @@
       <c r="C4" t="s">
         <v>67</v>
       </c>
-      <c r="D4" s="4">
+      <c r="D4" s="3">
         <f>B4*1000/(24*3600)</f>
         <v>2.9513888888888888</v>
       </c>
-      <c r="E4" s="5" t="s">
+      <c r="E4" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F4" s="6">
+      <c r="F4" s="5">
         <f>B4*1000/24</f>
         <v>10625</v>
       </c>
@@ -1829,15 +5056,15 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="3" t="s">
+      <c r="A6" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="3"/>
-      <c r="C6" s="3"/>
-      <c r="D6" s="3"/>
-      <c r="E6" s="3"/>
-      <c r="F6" s="3"/>
-      <c r="G6" s="3"/>
+      <c r="B6" s="42"/>
+      <c r="C6" s="42"/>
+      <c r="D6" s="42"/>
+      <c r="E6" s="42"/>
+      <c r="F6" s="42"/>
+      <c r="G6" s="42"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -1849,14 +5076,14 @@
       <c r="C7" t="s">
         <v>67</v>
       </c>
-      <c r="D7" s="4">
+      <c r="D7" s="3">
         <f>B7*1000/(24*3600)</f>
         <v>2.0370370370370372</v>
       </c>
-      <c r="E7" s="5" t="s">
+      <c r="E7" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F7" s="6">
+      <c r="F7" s="5">
         <f>B7*1000/24</f>
         <v>7333.333333333333</v>
       </c>
@@ -1874,14 +5101,14 @@
       <c r="C8" t="s">
         <v>67</v>
       </c>
-      <c r="D8" s="4">
+      <c r="D8" s="3">
         <f t="shared" ref="D8:D9" si="0">B8*1000/(24*3600)</f>
         <v>2.4652777777777777</v>
       </c>
-      <c r="E8" s="5" t="s">
+      <c r="E8" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F8" s="6">
+      <c r="F8" s="5">
         <f t="shared" ref="F8:F9" si="1">B8*1000/24</f>
         <v>8875</v>
       </c>
@@ -1899,14 +5126,14 @@
       <c r="C9" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="4">
+      <c r="D9" s="3">
         <f t="shared" si="0"/>
         <v>1.3657407407407407</v>
       </c>
-      <c r="E9" s="5" t="s">
+      <c r="E9" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="6">
+      <c r="F9" s="5">
         <f t="shared" si="1"/>
         <v>4916.666666666667</v>
       </c>
@@ -1915,22 +5142,22 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="3" t="s">
+      <c r="A11" s="42" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="3"/>
-      <c r="C11" s="3"/>
-      <c r="D11" s="3"/>
-      <c r="E11" s="3"/>
-      <c r="F11" s="3"/>
-      <c r="G11" s="3"/>
+      <c r="B11" s="42"/>
+      <c r="C11" s="42"/>
+      <c r="D11" s="42"/>
+      <c r="E11" s="42"/>
+      <c r="F11" s="42"/>
+      <c r="G11" s="42"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="3" t="s">
+      <c r="A12" s="42" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="3"/>
-      <c r="C12" s="3"/>
+      <c r="B12" s="42"/>
+      <c r="C12" s="42"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -1944,17 +5171,17 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="3" t="s">
+      <c r="A14" s="42" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="3"/>
-      <c r="C14" s="3"/>
+      <c r="B14" s="42"/>
+      <c r="C14" s="42"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="7">
+      <c r="B15" s="6">
         <f>1/B13</f>
         <v>2.5125628140703519E-2</v>
       </c>

</xml_diff>

<commit_message>
Compute values for sweep run of synfuels only baseline case
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/synfuels_model_numbers.xlsx
+++ b/use_cases/2022_05/data/synfuels_model_numbers.xlsx
@@ -8,18 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garrm\projects\FORCE\use_cases\2022_05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D8B42934-EE9E-48B8-91F4-EA5B7DB854D8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E37B663B-25E3-4037-BDC5-AC27B13A07B8}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="28680" yWindow="-120" windowWidth="38640" windowHeight="23640" activeTab="2" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
     <sheet name="HTSE" sheetId="2" r:id="rId2"/>
     <sheet name="FT" sheetId="7" r:id="rId3"/>
-    <sheet name="Capacity_Market" sheetId="3" r:id="rId4"/>
-    <sheet name="Transfer_rates" sheetId="4" r:id="rId5"/>
-    <sheet name="grid_sellall_test" sheetId="5" r:id="rId6"/>
-    <sheet name="grid_sellnothing_test" sheetId="6" r:id="rId7"/>
+    <sheet name="Syn_base" sheetId="8" r:id="rId4"/>
+    <sheet name="Capacity_Market" sheetId="3" r:id="rId5"/>
+    <sheet name="Transfer_rates" sheetId="4" r:id="rId6"/>
+    <sheet name="grid_sellall_test" sheetId="5" r:id="rId7"/>
+    <sheet name="grid_sellnothing_test" sheetId="6" r:id="rId8"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -41,7 +42,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="294" uniqueCount="171">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="176">
   <si>
     <t>Source</t>
   </si>
@@ -554,6 +555,21 @@
   </si>
   <si>
     <t>Log size factor</t>
+  </si>
+  <si>
+    <t>FT elec consumption</t>
+  </si>
+  <si>
+    <t>HTSE: elec to h2</t>
+  </si>
+  <si>
+    <t>kg/MWe</t>
+  </si>
+  <si>
+    <t>HTSE h2 prod</t>
+  </si>
+  <si>
+    <t>FT h2 capacity</t>
   </si>
 </sst>
 </file>
@@ -562,7 +578,7 @@
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
   <numFmts count="2">
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
-    <numFmt numFmtId="165" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
+    <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
   <fonts count="5" x14ac:knownFonts="1">
     <font>
@@ -830,12 +846,12 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="11" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="12" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="14" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
-    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
@@ -2342,10 +2358,10 @@
       </c>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="45" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="42"/>
+      <c r="B2" s="45"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -2652,8 +2668,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E35C99A-39AC-4C72-B859-1A7DCC98EEE1}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A41" workbookViewId="0">
-      <selection activeCell="T68" sqref="T68"/>
+    <sheetView topLeftCell="D41" workbookViewId="0">
+      <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -2981,7 +2997,7 @@
       <c r="A25" t="s">
         <v>133</v>
       </c>
-      <c r="B25" s="43">
+      <c r="B25" s="42">
         <v>11807922</v>
       </c>
       <c r="C25">
@@ -2990,39 +3006,39 @@
       <c r="D25">
         <v>0.65</v>
       </c>
-      <c r="E25" s="44">
+      <c r="E25" s="43">
         <f>$B25*POWER(E$24,$D25)</f>
         <v>4795506.4702437567</v>
       </c>
-      <c r="F25" s="44">
+      <c r="F25" s="43">
         <f>$B25*POWER(F$24,$D25)</f>
         <v>7524956.2358284583</v>
       </c>
-      <c r="G25" s="44">
+      <c r="G25" s="43">
         <f t="shared" ref="F25:M40" si="0">$B25*POWER(G$24,$D25)</f>
         <v>11807922</v>
       </c>
-      <c r="H25" s="44">
+      <c r="H25" s="43">
         <f t="shared" si="0"/>
         <v>13651016.264884572</v>
       </c>
-      <c r="I25" s="44">
+      <c r="I25" s="43">
         <f t="shared" si="0"/>
         <v>15368546.448911712</v>
       </c>
-      <c r="J25" s="44">
+      <c r="J25" s="43">
         <f t="shared" si="0"/>
         <v>18528615.660810392</v>
       </c>
-      <c r="K25" s="44">
+      <c r="K25" s="43">
         <f t="shared" si="0"/>
         <v>29074514.407025062</v>
       </c>
-      <c r="L25" s="44">
+      <c r="L25" s="43">
         <f t="shared" si="0"/>
         <v>33612744.821986459</v>
       </c>
-      <c r="M25" s="44">
+      <c r="M25" s="43">
         <f t="shared" si="0"/>
         <v>52744050.147983856</v>
       </c>
@@ -3031,7 +3047,7 @@
       <c r="A26" t="s">
         <v>134</v>
       </c>
-      <c r="B26" s="43">
+      <c r="B26" s="42">
         <v>17388504</v>
       </c>
       <c r="C26">
@@ -3040,39 +3056,39 @@
       <c r="D26">
         <v>0.8</v>
       </c>
-      <c r="E26" s="44">
+      <c r="E26" s="43">
         <f t="shared" ref="E26:M58" si="1">$B26*POWER(E$24,$D26)</f>
         <v>5736067.1461265292</v>
       </c>
-      <c r="F26" s="44">
+      <c r="F26" s="43">
         <f t="shared" si="0"/>
         <v>9987072.9703296833</v>
       </c>
-      <c r="G26" s="44">
+      <c r="G26" s="43">
         <f t="shared" si="0"/>
         <v>17388504</v>
       </c>
-      <c r="H26" s="44">
+      <c r="H26" s="43">
         <f t="shared" si="0"/>
         <v>20786924.085011322</v>
       </c>
-      <c r="I26" s="44">
+      <c r="I26" s="43">
         <f t="shared" si="0"/>
         <v>24051115.660847504</v>
       </c>
-      <c r="J26" s="44">
+      <c r="J26" s="43">
         <f t="shared" si="0"/>
         <v>30275143.904153816</v>
       </c>
-      <c r="K26" s="44">
+      <c r="K26" s="43">
         <f t="shared" si="0"/>
         <v>52712087.159264646</v>
       </c>
-      <c r="L26" s="44">
+      <c r="L26" s="43">
         <f t="shared" si="0"/>
         <v>63014170.40489132</v>
       </c>
-      <c r="M26" s="44">
+      <c r="M26" s="43">
         <f t="shared" si="0"/>
         <v>109714043.08323221</v>
       </c>
@@ -3081,7 +3097,7 @@
       <c r="A27" t="s">
         <v>135</v>
       </c>
-      <c r="B27" s="43">
+      <c r="B27" s="42">
         <v>2547995</v>
       </c>
       <c r="C27">
@@ -3090,39 +3106,39 @@
       <c r="D27">
         <v>0.6</v>
       </c>
-      <c r="E27" s="44">
+      <c r="E27" s="43">
         <f t="shared" si="1"/>
         <v>1109079.2412628538</v>
       </c>
-      <c r="F27" s="44">
+      <c r="F27" s="43">
         <f t="shared" si="0"/>
         <v>1681049.7795548902</v>
       </c>
-      <c r="G27" s="44">
+      <c r="G27" s="43">
         <f t="shared" si="0"/>
         <v>2547995</v>
       </c>
-      <c r="H27" s="44">
+      <c r="H27" s="43">
         <f t="shared" si="0"/>
         <v>2913027.4644639199</v>
       </c>
-      <c r="I27" s="44">
+      <c r="I27" s="43">
         <f t="shared" si="0"/>
         <v>3249775.2504720115</v>
       </c>
-      <c r="J27" s="44">
+      <c r="J27" s="43">
         <f t="shared" si="0"/>
         <v>3862038.2328856615</v>
       </c>
-      <c r="K27" s="44">
+      <c r="K27" s="43">
         <f t="shared" si="0"/>
         <v>5853755.3300813409</v>
       </c>
-      <c r="L27" s="44">
+      <c r="L27" s="43">
         <f t="shared" si="0"/>
         <v>6692379.7129817763</v>
       </c>
-      <c r="M27" s="44">
+      <c r="M27" s="43">
         <f t="shared" si="0"/>
         <v>10143750.800344583</v>
       </c>
@@ -3131,7 +3147,7 @@
       <c r="A28" t="s">
         <v>136</v>
       </c>
-      <c r="B28" s="43">
+      <c r="B28" s="42">
         <v>22972192</v>
       </c>
       <c r="C28">
@@ -3140,39 +3156,39 @@
       <c r="D28">
         <v>0.6</v>
       </c>
-      <c r="E28" s="44">
+      <c r="E28" s="43">
         <f t="shared" si="1"/>
         <v>9999227.3428733572</v>
       </c>
-      <c r="F28" s="44">
+      <c r="F28" s="43">
         <f t="shared" si="0"/>
         <v>15155994.535896897</v>
       </c>
-      <c r="G28" s="44">
+      <c r="G28" s="43">
         <f t="shared" si="0"/>
         <v>22972192</v>
       </c>
-      <c r="H28" s="44">
+      <c r="H28" s="43">
         <f t="shared" si="0"/>
         <v>26263248.638611279</v>
       </c>
-      <c r="I28" s="44">
+      <c r="I28" s="43">
         <f t="shared" si="0"/>
         <v>29299296.509879783</v>
       </c>
-      <c r="J28" s="44">
+      <c r="J28" s="43">
         <f t="shared" si="0"/>
         <v>34819331.983457632</v>
       </c>
-      <c r="K28" s="44">
+      <c r="K28" s="43">
         <f t="shared" si="0"/>
         <v>52776238.322152101</v>
       </c>
-      <c r="L28" s="44">
+      <c r="L28" s="43">
         <f t="shared" si="0"/>
         <v>60337101.016101778</v>
       </c>
-      <c r="M28" s="44">
+      <c r="M28" s="43">
         <f t="shared" si="0"/>
         <v>91453943.585316852</v>
       </c>
@@ -3181,7 +3197,7 @@
       <c r="A29" t="s">
         <v>137</v>
       </c>
-      <c r="B29" s="43">
+      <c r="B29" s="42">
         <v>6248204</v>
       </c>
       <c r="C29">
@@ -3190,39 +3206,39 @@
       <c r="D29">
         <v>0.6</v>
       </c>
-      <c r="E29" s="44">
+      <c r="E29" s="43">
         <f t="shared" si="1"/>
         <v>2719688.7558945478</v>
       </c>
-      <c r="F29" s="44">
+      <c r="F29" s="43">
         <f t="shared" si="0"/>
         <v>4122277.3030614201</v>
       </c>
-      <c r="G29" s="44">
+      <c r="G29" s="43">
         <f t="shared" si="0"/>
         <v>6248204</v>
       </c>
-      <c r="H29" s="44">
+      <c r="H29" s="43">
         <f t="shared" si="0"/>
         <v>7143338.1366813211</v>
       </c>
-      <c r="I29" s="44">
+      <c r="I29" s="43">
         <f t="shared" si="0"/>
         <v>7969112.4665080681</v>
       </c>
-      <c r="J29" s="44">
+      <c r="J29" s="43">
         <f t="shared" si="0"/>
         <v>9470506.3137365356</v>
       </c>
-      <c r="K29" s="44">
+      <c r="K29" s="43">
         <f t="shared" si="0"/>
         <v>14354603.312971789</v>
       </c>
-      <c r="L29" s="44">
+      <c r="L29" s="43">
         <f t="shared" si="0"/>
         <v>16411081.533586834</v>
       </c>
-      <c r="M29" s="44">
+      <c r="M29" s="43">
         <f t="shared" si="0"/>
         <v>24874548.15481044</v>
       </c>
@@ -3231,7 +3247,7 @@
       <c r="A30" t="s">
         <v>138</v>
       </c>
-      <c r="B30" s="43">
+      <c r="B30" s="42">
         <v>32995221</v>
       </c>
       <c r="C30">
@@ -3240,39 +3256,39 @@
       <c r="D30">
         <v>0.6</v>
       </c>
-      <c r="E30" s="44">
+      <c r="E30" s="43">
         <f t="shared" si="1"/>
         <v>14362004.113815052</v>
       </c>
-      <c r="F30" s="44">
+      <c r="F30" s="43">
         <f t="shared" si="0"/>
         <v>21768727.563599963</v>
       </c>
-      <c r="G30" s="44">
+      <c r="G30" s="43">
         <f t="shared" si="0"/>
         <v>32995221</v>
       </c>
-      <c r="H30" s="44">
+      <c r="H30" s="43">
         <f t="shared" si="0"/>
         <v>37722203.131896526</v>
       </c>
-      <c r="I30" s="44">
+      <c r="I30" s="43">
         <f t="shared" si="0"/>
         <v>42082913.266962603</v>
       </c>
-      <c r="J30" s="44">
+      <c r="J30" s="43">
         <f t="shared" si="0"/>
         <v>50011403.085371777</v>
       </c>
-      <c r="K30" s="44">
+      <c r="K30" s="43">
         <f t="shared" si="0"/>
         <v>75803112.170927256</v>
       </c>
-      <c r="L30" s="44">
+      <c r="L30" s="43">
         <f t="shared" si="0"/>
         <v>86662865.368947059</v>
       </c>
-      <c r="M30" s="44">
+      <c r="M30" s="43">
         <f t="shared" si="0"/>
         <v>131356340.74097335</v>
       </c>
@@ -3281,7 +3297,7 @@
       <c r="A31" t="s">
         <v>139</v>
       </c>
-      <c r="B31" s="43">
+      <c r="B31" s="42">
         <v>4186906</v>
       </c>
       <c r="C31">
@@ -3290,39 +3306,39 @@
       <c r="D31">
         <v>0.7</v>
       </c>
-      <c r="E31" s="44">
+      <c r="E31" s="43">
         <f t="shared" si="1"/>
         <v>1586540.6966554464</v>
       </c>
-      <c r="F31" s="44">
+      <c r="F31" s="43">
         <f t="shared" si="0"/>
         <v>2577342.9655501549</v>
       </c>
-      <c r="G31" s="44">
+      <c r="G31" s="43">
         <f t="shared" si="0"/>
         <v>4186906</v>
       </c>
-      <c r="H31" s="44">
+      <c r="H31" s="43">
         <f t="shared" si="0"/>
         <v>4894746.672099025</v>
       </c>
-      <c r="I31" s="44">
+      <c r="I31" s="43">
         <f t="shared" si="0"/>
         <v>5561053.740726185</v>
       </c>
-      <c r="J31" s="44">
+      <c r="J31" s="43">
         <f t="shared" si="0"/>
         <v>6801648.8636366008</v>
       </c>
-      <c r="K31" s="44">
+      <c r="K31" s="43">
         <f t="shared" si="0"/>
         <v>11049311.17732499</v>
       </c>
-      <c r="L31" s="44">
+      <c r="L31" s="43">
         <f t="shared" si="0"/>
         <v>12917313.910127921</v>
       </c>
-      <c r="M31" s="44">
+      <c r="M31" s="43">
         <f t="shared" si="0"/>
         <v>20984238.355974279</v>
       </c>
@@ -3331,7 +3347,7 @@
       <c r="A32" t="s">
         <v>140</v>
       </c>
-      <c r="B32" s="43">
+      <c r="B32" s="42">
         <v>807728</v>
       </c>
       <c r="C32">
@@ -3340,39 +3356,39 @@
       <c r="D32">
         <v>0.7</v>
       </c>
-      <c r="E32" s="44">
+      <c r="E32" s="43">
         <f t="shared" si="1"/>
         <v>306071.67770857771</v>
       </c>
-      <c r="F32" s="44">
+      <c r="F32" s="43">
         <f t="shared" si="0"/>
         <v>497214.90735113126</v>
       </c>
-      <c r="G32" s="44">
+      <c r="G32" s="43">
         <f t="shared" si="0"/>
         <v>807728</v>
       </c>
-      <c r="H32" s="44">
+      <c r="H32" s="43">
         <f t="shared" si="0"/>
         <v>944282.94782858784</v>
       </c>
-      <c r="I32" s="44">
+      <c r="I32" s="43">
         <f t="shared" si="0"/>
         <v>1072825.3311369494</v>
       </c>
-      <c r="J32" s="44">
+      <c r="J32" s="43">
         <f t="shared" si="0"/>
         <v>1312158.0072080588</v>
       </c>
-      <c r="K32" s="44">
+      <c r="K32" s="43">
         <f t="shared" si="0"/>
         <v>2131606.9715055367</v>
       </c>
-      <c r="L32" s="44">
+      <c r="L32" s="43">
         <f t="shared" si="0"/>
         <v>2491977.6393355392</v>
       </c>
-      <c r="M32" s="44">
+      <c r="M32" s="43">
         <f t="shared" si="0"/>
         <v>4048229.6184328939</v>
       </c>
@@ -3381,7 +3397,7 @@
       <c r="A33" t="s">
         <v>148</v>
       </c>
-      <c r="B33" s="43">
+      <c r="B33" s="42">
         <v>75501</v>
       </c>
       <c r="C33">
@@ -3390,39 +3406,39 @@
       <c r="D33">
         <v>0.7</v>
       </c>
-      <c r="E33" s="44">
+      <c r="E33" s="43">
         <f t="shared" si="1"/>
         <v>28609.529122025393</v>
       </c>
-      <c r="F33" s="44">
+      <c r="F33" s="43">
         <f t="shared" si="0"/>
         <v>46476.317175977267</v>
       </c>
-      <c r="G33" s="44">
+      <c r="G33" s="43">
         <f t="shared" si="0"/>
         <v>75501</v>
       </c>
-      <c r="H33" s="44">
+      <c r="H33" s="43">
         <f t="shared" si="0"/>
         <v>88265.24132381966</v>
       </c>
-      <c r="I33" s="44">
+      <c r="I33" s="43">
         <f t="shared" si="0"/>
         <v>100280.52181696167</v>
       </c>
-      <c r="J33" s="44">
+      <c r="J33" s="43">
         <f t="shared" si="0"/>
         <v>122651.73635458427</v>
       </c>
-      <c r="K33" s="44">
+      <c r="K33" s="43">
         <f t="shared" si="0"/>
         <v>199248.33354252856</v>
       </c>
-      <c r="L33" s="44">
+      <c r="L33" s="43">
         <f t="shared" si="0"/>
         <v>232933.3683461172</v>
       </c>
-      <c r="M33" s="44">
+      <c r="M33" s="43">
         <f t="shared" si="0"/>
         <v>378401.37326092686</v>
       </c>
@@ -3431,7 +3447,7 @@
       <c r="A34" t="s">
         <v>141</v>
       </c>
-      <c r="B34" s="43">
+      <c r="B34" s="42">
         <v>11461600</v>
       </c>
       <c r="C34">
@@ -3440,39 +3456,39 @@
       <c r="D34">
         <v>0.65</v>
       </c>
-      <c r="E34" s="44">
+      <c r="E34" s="43">
         <f t="shared" si="1"/>
         <v>4654856.0330383144</v>
       </c>
-      <c r="F34" s="44">
+      <c r="F34" s="43">
         <f t="shared" si="0"/>
         <v>7304252.0430412283</v>
       </c>
-      <c r="G34" s="44">
+      <c r="G34" s="43">
         <f t="shared" si="0"/>
         <v>11461600</v>
       </c>
-      <c r="H34" s="44">
+      <c r="H34" s="43">
         <f t="shared" si="0"/>
         <v>13250636.989438193</v>
       </c>
-      <c r="I34" s="44">
+      <c r="I34" s="43">
         <f t="shared" si="0"/>
         <v>14917792.646229072</v>
       </c>
-      <c r="J34" s="44">
+      <c r="J34" s="43">
         <f t="shared" si="0"/>
         <v>17985178.192906797</v>
       </c>
-      <c r="K34" s="44">
+      <c r="K34" s="43">
         <f t="shared" si="0"/>
         <v>28221769.615988184</v>
       </c>
-      <c r="L34" s="44">
+      <c r="L34" s="43">
         <f t="shared" si="0"/>
         <v>32626895.405616667</v>
       </c>
-      <c r="M34" s="44">
+      <c r="M34" s="43">
         <f t="shared" si="0"/>
         <v>51197086.5979748</v>
       </c>
@@ -3481,7 +3497,7 @@
       <c r="A35" t="s">
         <v>142</v>
       </c>
-      <c r="B35" s="43">
+      <c r="B35" s="42">
         <v>36681585</v>
       </c>
       <c r="C35">
@@ -3490,39 +3506,39 @@
       <c r="D35">
         <v>0.8</v>
       </c>
-      <c r="E35" s="44">
+      <c r="E35" s="43">
         <f t="shared" si="1"/>
         <v>12100410.396797085</v>
       </c>
-      <c r="F35" s="44">
+      <c r="F35" s="43">
         <f t="shared" si="0"/>
         <v>21068038.174091958</v>
       </c>
-      <c r="G35" s="44">
+      <c r="G35" s="43">
         <f t="shared" si="0"/>
         <v>36681585</v>
       </c>
-      <c r="H35" s="44">
+      <c r="H35" s="43">
         <f t="shared" si="0"/>
         <v>43850656.888763405</v>
       </c>
-      <c r="I35" s="44">
+      <c r="I35" s="43">
         <f t="shared" si="0"/>
         <v>50736569.601284206</v>
       </c>
-      <c r="J35" s="44">
+      <c r="J35" s="43">
         <f t="shared" si="0"/>
         <v>63866348.968689315</v>
       </c>
-      <c r="K35" s="44">
+      <c r="K35" s="43">
         <f t="shared" si="0"/>
         <v>111197772.14071864</v>
       </c>
-      <c r="L35" s="44">
+      <c r="L35" s="43">
         <f t="shared" si="0"/>
         <v>132930334.19732401</v>
       </c>
-      <c r="M35" s="44">
+      <c r="M35" s="43">
         <f t="shared" si="0"/>
         <v>231445154.62924495</v>
       </c>
@@ -3531,7 +3547,7 @@
       <c r="A36" t="s">
         <v>143</v>
       </c>
-      <c r="B36" s="43">
+      <c r="B36" s="42">
         <v>144155</v>
       </c>
       <c r="C36">
@@ -3540,39 +3556,39 @@
       <c r="D36">
         <v>0.6</v>
       </c>
-      <c r="E36" s="44">
+      <c r="E36" s="43">
         <f t="shared" si="1"/>
         <v>62747.108225976386</v>
       </c>
-      <c r="F36" s="44">
+      <c r="F36" s="43">
         <f t="shared" si="0"/>
         <v>95106.831438733279</v>
       </c>
-      <c r="G36" s="44">
+      <c r="G36" s="43">
         <f t="shared" si="0"/>
         <v>144155</v>
       </c>
-      <c r="H36" s="44">
+      <c r="H36" s="43">
         <f t="shared" si="0"/>
         <v>164807.02440145935</v>
       </c>
-      <c r="I36" s="44">
+      <c r="I36" s="43">
         <f t="shared" si="0"/>
         <v>183858.81888771086</v>
       </c>
-      <c r="J36" s="44">
+      <c r="J36" s="43">
         <f t="shared" si="0"/>
         <v>218498.12164530641</v>
       </c>
-      <c r="K36" s="44">
+      <c r="K36" s="43">
         <f t="shared" si="0"/>
         <v>331181.2227291952</v>
       </c>
-      <c r="L36" s="44">
+      <c r="L36" s="43">
         <f t="shared" si="0"/>
         <v>378627.11564382503</v>
       </c>
-      <c r="M36" s="44">
+      <c r="M36" s="43">
         <f t="shared" si="0"/>
         <v>573891.39171139395</v>
       </c>
@@ -3581,7 +3597,7 @@
       <c r="A37" t="s">
         <v>144</v>
       </c>
-      <c r="B37" s="43">
+      <c r="B37" s="42">
         <v>6595713</v>
       </c>
       <c r="C37">
@@ -3590,39 +3606,39 @@
       <c r="D37">
         <v>0.7</v>
       </c>
-      <c r="E37" s="44">
+      <c r="E37" s="43">
         <f t="shared" si="1"/>
         <v>2499307.8655119995</v>
       </c>
-      <c r="F37" s="44">
+      <c r="F37" s="43">
         <f t="shared" si="0"/>
         <v>4060137.6059882189</v>
       </c>
-      <c r="G37" s="44">
+      <c r="G37" s="43">
         <f t="shared" si="0"/>
         <v>6595713</v>
       </c>
-      <c r="H37" s="44">
+      <c r="H37" s="43">
         <f t="shared" si="0"/>
         <v>7710787.9319168562</v>
       </c>
-      <c r="I37" s="44">
+      <c r="I37" s="43">
         <f t="shared" si="0"/>
         <v>8760434.1849103682</v>
       </c>
-      <c r="J37" s="44">
+      <c r="J37" s="43">
         <f t="shared" si="0"/>
         <v>10714767.379855949</v>
       </c>
-      <c r="K37" s="44">
+      <c r="K37" s="43">
         <f t="shared" si="0"/>
         <v>17406190.961375237</v>
       </c>
-      <c r="L37" s="44">
+      <c r="L37" s="43">
         <f t="shared" si="0"/>
         <v>20348891.348912913</v>
       </c>
-      <c r="M37" s="44">
+      <c r="M37" s="43">
         <f t="shared" si="0"/>
         <v>33056871.522694372</v>
       </c>
@@ -3631,7 +3647,7 @@
       <c r="A38" t="s">
         <v>145</v>
       </c>
-      <c r="B38" s="43">
+      <c r="B38" s="42">
         <v>1626125</v>
       </c>
       <c r="C38">
@@ -3640,39 +3656,39 @@
       <c r="D38">
         <v>0.7</v>
       </c>
-      <c r="E38" s="44">
+      <c r="E38" s="43">
         <f t="shared" si="1"/>
         <v>616186.15042918036</v>
       </c>
-      <c r="F38" s="44">
+      <c r="F38" s="43">
         <f t="shared" si="0"/>
         <v>1000997.354575251</v>
       </c>
-      <c r="G38" s="44">
+      <c r="G38" s="43">
         <f t="shared" si="0"/>
         <v>1626125</v>
       </c>
-      <c r="H38" s="44">
+      <c r="H38" s="43">
         <f t="shared" si="0"/>
         <v>1901038.6027694501</v>
       </c>
-      <c r="I38" s="44">
+      <c r="I38" s="43">
         <f t="shared" si="0"/>
         <v>2159821.2413028539</v>
       </c>
-      <c r="J38" s="44">
+      <c r="J38" s="43">
         <f t="shared" si="0"/>
         <v>2641647.856049567</v>
       </c>
-      <c r="K38" s="44">
+      <c r="K38" s="43">
         <f t="shared" si="0"/>
         <v>4291369.6028111456</v>
       </c>
-      <c r="L38" s="44">
+      <c r="L38" s="43">
         <f t="shared" si="0"/>
         <v>5016870.9500778774</v>
       </c>
-      <c r="M38" s="44">
+      <c r="M38" s="43">
         <f t="shared" si="0"/>
         <v>8149930.9028214812</v>
       </c>
@@ -3681,7 +3697,7 @@
       <c r="A39" t="s">
         <v>146</v>
       </c>
-      <c r="B39" s="43">
+      <c r="B39" s="42">
         <v>980551</v>
       </c>
       <c r="C39">
@@ -3690,39 +3706,39 @@
       <c r="D39">
         <v>0.7</v>
       </c>
-      <c r="E39" s="44">
+      <c r="E39" s="43">
         <f t="shared" si="1"/>
         <v>371559.34875208436</v>
       </c>
-      <c r="F39" s="44">
+      <c r="F39" s="43">
         <f t="shared" si="0"/>
         <v>603599.94282488548</v>
       </c>
-      <c r="G39" s="44">
+      <c r="G39" s="43">
         <f t="shared" si="0"/>
         <v>980551</v>
       </c>
-      <c r="H39" s="44">
+      <c r="H39" s="43">
         <f t="shared" si="0"/>
         <v>1146323.5009511488</v>
       </c>
-      <c r="I39" s="44">
+      <c r="I39" s="43">
         <f t="shared" si="0"/>
         <v>1302369.0540276761</v>
       </c>
-      <c r="J39" s="44">
+      <c r="J39" s="43">
         <f t="shared" si="0"/>
         <v>1592909.7989990062</v>
       </c>
-      <c r="K39" s="44">
+      <c r="K39" s="43">
         <f t="shared" si="0"/>
         <v>2587689.6028325441</v>
       </c>
-      <c r="L39" s="44">
+      <c r="L39" s="43">
         <f t="shared" si="0"/>
         <v>3025165.8556198403</v>
       </c>
-      <c r="M39" s="44">
+      <c r="M39" s="43">
         <f t="shared" si="0"/>
         <v>4914396.4312045546</v>
       </c>
@@ -3731,7 +3747,7 @@
       <c r="A40" t="s">
         <v>147</v>
       </c>
-      <c r="B40" s="43">
+      <c r="B40" s="42">
         <v>123670</v>
       </c>
       <c r="C40">
@@ -3740,39 +3756,39 @@
       <c r="D40">
         <v>0.6</v>
       </c>
-      <c r="E40" s="44">
+      <c r="E40" s="43">
         <f t="shared" si="1"/>
         <v>53830.494081415833</v>
       </c>
-      <c r="F40" s="44">
+      <c r="F40" s="43">
         <f t="shared" si="0"/>
         <v>81591.771662641913</v>
       </c>
-      <c r="G40" s="44">
+      <c r="G40" s="43">
         <f t="shared" si="0"/>
         <v>123670</v>
       </c>
-      <c r="H40" s="44">
+      <c r="H40" s="43">
         <f t="shared" si="0"/>
         <v>141387.28942963114</v>
       </c>
-      <c r="I40" s="44">
+      <c r="I40" s="43">
         <f t="shared" si="0"/>
         <v>157731.74799239152</v>
       </c>
-      <c r="J40" s="44">
+      <c r="J40" s="43">
         <f t="shared" si="0"/>
         <v>187448.66778034091</v>
       </c>
-      <c r="K40" s="44">
+      <c r="K40" s="43">
         <f t="shared" si="0"/>
         <v>284119.05112496665</v>
       </c>
-      <c r="L40" s="44">
+      <c r="L40" s="43">
         <f t="shared" si="0"/>
         <v>324822.69357061386</v>
       </c>
-      <c r="M40" s="44">
+      <c r="M40" s="43">
         <f t="shared" si="0"/>
         <v>492339.1378235101</v>
       </c>
@@ -3781,7 +3797,7 @@
       <c r="A41" t="s">
         <v>149</v>
       </c>
-      <c r="B41" s="43">
+      <c r="B41" s="42">
         <v>718300</v>
       </c>
       <c r="C41">
@@ -3790,39 +3806,39 @@
       <c r="D41">
         <v>0.8</v>
       </c>
-      <c r="E41" s="44">
+      <c r="E41" s="43">
         <f t="shared" si="1"/>
         <v>236950.63307704253</v>
       </c>
-      <c r="F41" s="44">
+      <c r="F41" s="43">
         <f t="shared" si="1"/>
         <v>412555.01419718517</v>
       </c>
-      <c r="G41" s="44">
+      <c r="G41" s="43">
         <f t="shared" si="1"/>
         <v>718300</v>
       </c>
-      <c r="H41" s="44">
+      <c r="H41" s="43">
         <f t="shared" si="1"/>
         <v>858685.00074897939</v>
       </c>
-      <c r="I41" s="44">
+      <c r="I41" s="43">
         <f t="shared" si="1"/>
         <v>993525.16922598751</v>
       </c>
-      <c r="J41" s="44">
+      <c r="J41" s="43">
         <f t="shared" si="1"/>
         <v>1250632.939231212</v>
       </c>
-      <c r="K41" s="44">
+      <c r="K41" s="43">
         <f t="shared" si="1"/>
         <v>2177478.4194488376</v>
       </c>
-      <c r="L41" s="44">
+      <c r="L41" s="43">
         <f t="shared" si="1"/>
         <v>2603046.1620984436</v>
       </c>
-      <c r="M41" s="44">
+      <c r="M41" s="43">
         <f t="shared" si="1"/>
         <v>4532166.6054012291</v>
       </c>
@@ -3831,7 +3847,7 @@
       <c r="A42" t="s">
         <v>150</v>
       </c>
-      <c r="B42" s="43">
+      <c r="B42" s="42">
         <v>7495642</v>
       </c>
       <c r="C42">
@@ -3840,39 +3856,39 @@
       <c r="D42">
         <v>0.6</v>
       </c>
-      <c r="E42" s="44">
+      <c r="E42" s="43">
         <f t="shared" si="1"/>
         <v>3262667.6826830432</v>
       </c>
-      <c r="F42" s="44">
+      <c r="F42" s="43">
         <f t="shared" si="1"/>
         <v>4945279.4576607794</v>
       </c>
-      <c r="G42" s="44">
+      <c r="G42" s="43">
         <f t="shared" si="1"/>
         <v>7495642</v>
       </c>
-      <c r="H42" s="44">
+      <c r="H42" s="43">
         <f t="shared" si="1"/>
         <v>8569487.3850966208</v>
       </c>
-      <c r="I42" s="44">
+      <c r="I42" s="43">
         <f t="shared" si="1"/>
         <v>9560125.4547197036</v>
       </c>
-      <c r="J42" s="44">
+      <c r="J42" s="43">
         <f t="shared" si="1"/>
         <v>11361268.756031133</v>
       </c>
-      <c r="K42" s="44">
+      <c r="K42" s="43">
         <f t="shared" si="1"/>
         <v>17220463.270093374</v>
       </c>
-      <c r="L42" s="44">
+      <c r="L42" s="43">
         <f t="shared" si="1"/>
         <v>19687512.124856662</v>
       </c>
-      <c r="M42" s="44">
+      <c r="M42" s="43">
         <f t="shared" si="1"/>
         <v>29840688.281019572</v>
       </c>
@@ -3881,7 +3897,7 @@
       <c r="A43" t="s">
         <v>151</v>
       </c>
-      <c r="B43" s="43">
+      <c r="B43" s="42">
         <v>969104</v>
       </c>
       <c r="C43">
@@ -3890,39 +3906,39 @@
       <c r="D43">
         <v>0.7</v>
       </c>
-      <c r="E43" s="44">
+      <c r="E43" s="43">
         <f t="shared" si="1"/>
         <v>367221.74686787324</v>
       </c>
-      <c r="F43" s="44">
+      <c r="F43" s="43">
         <f t="shared" si="1"/>
         <v>596553.48777510587</v>
       </c>
-      <c r="G43" s="44">
+      <c r="G43" s="43">
         <f t="shared" si="1"/>
         <v>969104</v>
       </c>
-      <c r="H43" s="44">
+      <c r="H43" s="43">
         <f t="shared" si="1"/>
         <v>1132941.2647233671</v>
       </c>
-      <c r="I43" s="44">
+      <c r="I43" s="43">
         <f t="shared" si="1"/>
         <v>1287165.1344340448</v>
       </c>
-      <c r="J43" s="44">
+      <c r="J43" s="43">
         <f t="shared" si="1"/>
         <v>1574314.0926368264</v>
       </c>
-      <c r="K43" s="44">
+      <c r="K43" s="43">
         <f t="shared" si="1"/>
         <v>2557480.7887233095</v>
       </c>
-      <c r="L43" s="44">
+      <c r="L43" s="43">
         <f t="shared" si="1"/>
         <v>2989849.9224870605</v>
       </c>
-      <c r="M43" s="44">
+      <c r="M43" s="43">
         <f t="shared" si="1"/>
         <v>4857025.5285712406</v>
       </c>
@@ -3931,7 +3947,7 @@
       <c r="A44" t="s">
         <v>152</v>
       </c>
-      <c r="B44" s="43">
+      <c r="B44" s="42">
         <v>29456</v>
       </c>
       <c r="C44">
@@ -3940,39 +3956,39 @@
       <c r="D44">
         <v>0.7</v>
       </c>
-      <c r="E44" s="44">
+      <c r="E44" s="43">
         <f t="shared" si="1"/>
         <v>11161.736795782572</v>
       </c>
-      <c r="F44" s="44">
+      <c r="F44" s="43">
         <f t="shared" si="1"/>
         <v>18132.294919743927</v>
       </c>
-      <c r="G44" s="44">
+      <c r="G44" s="43">
         <f t="shared" si="1"/>
         <v>29456</v>
       </c>
-      <c r="H44" s="44">
+      <c r="H44" s="43">
         <f t="shared" si="1"/>
         <v>34435.847848828918</v>
       </c>
-      <c r="I44" s="44">
+      <c r="I44" s="43">
         <f t="shared" si="1"/>
         <v>39123.495723770851</v>
       </c>
-      <c r="J44" s="44">
+      <c r="J44" s="43">
         <f t="shared" si="1"/>
         <v>47851.413174138543</v>
       </c>
-      <c r="K44" s="44">
+      <c r="K44" s="43">
         <f t="shared" si="1"/>
         <v>77734.850039452736</v>
       </c>
-      <c r="L44" s="44">
+      <c r="L44" s="43">
         <f t="shared" si="1"/>
         <v>90876.747301403011</v>
       </c>
-      <c r="M44" s="44">
+      <c r="M44" s="43">
         <f t="shared" si="1"/>
         <v>147629.71153724933</v>
       </c>
@@ -3981,7 +3997,7 @@
       <c r="A45" t="s">
         <v>153</v>
       </c>
-      <c r="B45" s="43">
+      <c r="B45" s="42">
         <v>21715</v>
       </c>
       <c r="C45">
@@ -3990,39 +4006,39 @@
       <c r="D45">
         <v>0.6</v>
       </c>
-      <c r="E45" s="44">
+      <c r="E45" s="43">
         <f t="shared" si="1"/>
         <v>9452.0027409876675</v>
       </c>
-      <c r="F45" s="44">
+      <c r="F45" s="43">
         <f t="shared" si="1"/>
         <v>14326.557141216699</v>
       </c>
-      <c r="G45" s="44">
+      <c r="G45" s="43">
         <f t="shared" si="1"/>
         <v>21715</v>
       </c>
-      <c r="H45" s="44">
+      <c r="H45" s="43">
         <f t="shared" si="1"/>
         <v>24825.948006504732</v>
       </c>
-      <c r="I45" s="44">
+      <c r="I45" s="43">
         <f t="shared" si="1"/>
         <v>27695.843031089047</v>
       </c>
-      <c r="J45" s="44">
+      <c r="J45" s="43">
         <f t="shared" si="1"/>
         <v>32913.785241773294</v>
       </c>
-      <c r="K45" s="44">
+      <c r="K45" s="43">
         <f t="shared" si="1"/>
         <v>49887.969557521232</v>
       </c>
-      <c r="L45" s="44">
+      <c r="L45" s="43">
         <f t="shared" si="1"/>
         <v>57035.051272627803</v>
       </c>
-      <c r="M45" s="44">
+      <c r="M45" s="43">
         <f t="shared" si="1"/>
         <v>86448.97208569193</v>
       </c>
@@ -4031,7 +4047,7 @@
       <c r="A46" t="s">
         <v>154</v>
       </c>
-      <c r="B46" s="43">
+      <c r="B46" s="42">
         <v>50244</v>
       </c>
       <c r="C46">
@@ -4040,39 +4056,39 @@
       <c r="D46">
         <v>0.7</v>
       </c>
-      <c r="E46" s="44">
+      <c r="E46" s="43">
         <f t="shared" si="1"/>
         <v>19038.915791937114</v>
       </c>
-      <c r="F46" s="44">
+      <c r="F46" s="43">
         <f t="shared" si="1"/>
         <v>30928.809952050986</v>
       </c>
-      <c r="G46" s="44">
+      <c r="G46" s="43">
         <f t="shared" si="1"/>
         <v>50244</v>
       </c>
-      <c r="H46" s="44">
+      <c r="H46" s="43">
         <f t="shared" si="1"/>
         <v>58738.27876549973</v>
       </c>
-      <c r="I46" s="44">
+      <c r="I46" s="43">
         <f t="shared" si="1"/>
         <v>66734.143099712877</v>
       </c>
-      <c r="J46" s="44">
+      <c r="J46" s="43">
         <f t="shared" si="1"/>
         <v>81621.618805045393</v>
       </c>
-      <c r="K46" s="44">
+      <c r="K46" s="43">
         <f t="shared" si="1"/>
         <v>132594.7109377466</v>
       </c>
-      <c r="L46" s="44">
+      <c r="L46" s="43">
         <f t="shared" si="1"/>
         <v>155011.24699252081</v>
       </c>
-      <c r="M46" s="44">
+      <c r="M46" s="43">
         <f t="shared" si="1"/>
         <v>251816.5136636867</v>
       </c>
@@ -4081,7 +4097,7 @@
       <c r="A47" t="s">
         <v>155</v>
       </c>
-      <c r="B47" s="43">
+      <c r="B47" s="42">
         <v>33067253</v>
       </c>
       <c r="C47">
@@ -4090,39 +4106,39 @@
       <c r="D47">
         <v>0.65</v>
       </c>
-      <c r="E47" s="44">
+      <c r="E47" s="43">
         <f t="shared" si="1"/>
         <v>13429477.745083958</v>
       </c>
-      <c r="F47" s="44">
+      <c r="F47" s="43">
         <f t="shared" si="1"/>
         <v>21073109.363702379</v>
       </c>
-      <c r="G47" s="44">
+      <c r="G47" s="43">
         <f t="shared" si="1"/>
         <v>33067253</v>
       </c>
-      <c r="H47" s="44">
+      <c r="H47" s="43">
         <f t="shared" si="1"/>
         <v>38228708.534664541</v>
       </c>
-      <c r="I47" s="44">
+      <c r="I47" s="43">
         <f t="shared" si="1"/>
         <v>43038530.714245498</v>
       </c>
-      <c r="J47" s="44">
+      <c r="J47" s="43">
         <f t="shared" si="1"/>
         <v>51888081.729857251</v>
       </c>
-      <c r="K47" s="44">
+      <c r="K47" s="43">
         <f t="shared" si="1"/>
         <v>81421127.591225848</v>
       </c>
-      <c r="L47" s="44">
+      <c r="L47" s="43">
         <f t="shared" si="1"/>
         <v>94130121.883686736</v>
       </c>
-      <c r="M47" s="44">
+      <c r="M47" s="43">
         <f t="shared" si="1"/>
         <v>147705993.52604714</v>
       </c>
@@ -4131,7 +4147,7 @@
       <c r="A48" t="s">
         <v>156</v>
       </c>
-      <c r="B48" s="43">
+      <c r="B48" s="42">
         <v>411911</v>
       </c>
       <c r="C48">
@@ -4140,39 +4156,39 @@
       <c r="D48">
         <v>0.65</v>
       </c>
-      <c r="E48" s="44">
+      <c r="E48" s="43">
         <f t="shared" si="1"/>
         <v>167287.84841774666</v>
       </c>
-      <c r="F48" s="44">
+      <c r="F48" s="43">
         <f t="shared" si="1"/>
         <v>262502.77127985231</v>
       </c>
-      <c r="G48" s="44">
+      <c r="G48" s="43">
         <f t="shared" si="1"/>
         <v>411911</v>
       </c>
-      <c r="H48" s="44">
+      <c r="H48" s="43">
         <f t="shared" si="1"/>
         <v>476206.03868190094</v>
       </c>
-      <c r="I48" s="44">
+      <c r="I48" s="43">
         <f t="shared" si="1"/>
         <v>536120.86329141329</v>
       </c>
-      <c r="J48" s="44">
+      <c r="J48" s="43">
         <f t="shared" si="1"/>
         <v>646357.64069749706</v>
       </c>
-      <c r="K48" s="44">
+      <c r="K48" s="43">
         <f t="shared" si="1"/>
         <v>1014243.8528906356</v>
       </c>
-      <c r="L48" s="44">
+      <c r="L48" s="43">
         <f t="shared" si="1"/>
         <v>1172556.808248671</v>
       </c>
-      <c r="M48" s="44">
+      <c r="M48" s="43">
         <f t="shared" si="1"/>
         <v>1839938.8512649538</v>
       </c>
@@ -4181,7 +4197,7 @@
       <c r="A49" t="s">
         <v>157</v>
       </c>
-      <c r="B49" s="43">
+      <c r="B49" s="42">
         <v>585966</v>
       </c>
       <c r="C49">
@@ -4190,39 +4206,39 @@
       <c r="D49">
         <v>0.65</v>
       </c>
-      <c r="E49" s="44">
+      <c r="E49" s="43">
         <f t="shared" si="1"/>
         <v>237976.14384163893</v>
       </c>
-      <c r="F49" s="44">
+      <c r="F49" s="43">
         <f t="shared" si="1"/>
         <v>373424.5962738794</v>
       </c>
-      <c r="G49" s="44">
+      <c r="G49" s="43">
         <f t="shared" si="1"/>
         <v>585966</v>
       </c>
-      <c r="H49" s="44">
+      <c r="H49" s="43">
         <f t="shared" si="1"/>
         <v>677429.22054103622</v>
       </c>
-      <c r="I49" s="44">
+      <c r="I49" s="43">
         <f t="shared" si="1"/>
         <v>762661.34621172119</v>
       </c>
-      <c r="J49" s="44">
+      <c r="J49" s="43">
         <f t="shared" si="1"/>
         <v>919479.21101633494</v>
       </c>
-      <c r="K49" s="44">
+      <c r="K49" s="43">
         <f t="shared" si="1"/>
         <v>1442817.5346201344</v>
       </c>
-      <c r="L49" s="44">
+      <c r="L49" s="43">
         <f t="shared" si="1"/>
         <v>1668026.4006113959</v>
       </c>
-      <c r="M49" s="44">
+      <c r="M49" s="43">
         <f t="shared" si="1"/>
         <v>2617413.9775833129</v>
       </c>
@@ -4231,7 +4247,7 @@
       <c r="A50" t="s">
         <v>158</v>
       </c>
-      <c r="B50" s="43">
+      <c r="B50" s="42">
         <v>326304</v>
       </c>
       <c r="C50">
@@ -4240,39 +4256,39 @@
       <c r="D50">
         <v>0.65</v>
       </c>
-      <c r="E50" s="44">
+      <c r="E50" s="43">
         <f t="shared" si="1"/>
         <v>132520.60297031252</v>
       </c>
-      <c r="F50" s="44">
+      <c r="F50" s="43">
         <f t="shared" si="1"/>
         <v>207947.11546839227</v>
       </c>
-      <c r="G50" s="44">
+      <c r="G50" s="43">
         <f t="shared" si="1"/>
         <v>326304</v>
       </c>
-      <c r="H50" s="44">
+      <c r="H50" s="43">
         <f t="shared" si="1"/>
         <v>377236.67308243527</v>
       </c>
-      <c r="I50" s="44">
+      <c r="I50" s="43">
         <f t="shared" si="1"/>
         <v>424699.46705827554</v>
       </c>
-      <c r="J50" s="44">
+      <c r="J50" s="43">
         <f t="shared" si="1"/>
         <v>512025.85896020272</v>
       </c>
-      <c r="K50" s="44">
+      <c r="K50" s="43">
         <f t="shared" si="1"/>
         <v>803454.69330419914</v>
       </c>
-      <c r="L50" s="44">
+      <c r="L50" s="43">
         <f t="shared" si="1"/>
         <v>928865.6451485256</v>
       </c>
-      <c r="M50" s="44">
+      <c r="M50" s="43">
         <f t="shared" si="1"/>
         <v>1457546.4285322789</v>
       </c>
@@ -4281,7 +4297,7 @@
       <c r="A51" t="s">
         <v>166</v>
       </c>
-      <c r="B51" s="43">
+      <c r="B51" s="42">
         <v>178050</v>
       </c>
       <c r="C51">
@@ -4290,39 +4306,39 @@
       <c r="D51">
         <v>0.65</v>
       </c>
-      <c r="E51" s="44">
+      <c r="E51" s="43">
         <f t="shared" si="1"/>
         <v>72310.76958561386</v>
       </c>
-      <c r="F51" s="44">
+      <c r="F51" s="43">
         <f t="shared" si="1"/>
         <v>113467.75984709732</v>
       </c>
-      <c r="G51" s="44">
+      <c r="G51" s="43">
         <f t="shared" si="1"/>
         <v>178050</v>
       </c>
-      <c r="H51" s="44">
+      <c r="H51" s="43">
         <f t="shared" si="1"/>
         <v>205841.75996104124</v>
       </c>
-      <c r="I51" s="44">
+      <c r="I51" s="43">
         <f t="shared" si="1"/>
         <v>231740.15675482361</v>
       </c>
-      <c r="J51" s="44">
+      <c r="J51" s="43">
         <f t="shared" si="1"/>
         <v>279390.39726103295</v>
       </c>
-      <c r="K51" s="44">
+      <c r="K51" s="43">
         <f t="shared" si="1"/>
         <v>438410.52559212467</v>
       </c>
-      <c r="L51" s="44">
+      <c r="L51" s="43">
         <f t="shared" si="1"/>
         <v>506841.86561824247</v>
       </c>
-      <c r="M51" s="44">
+      <c r="M51" s="43">
         <f t="shared" si="1"/>
         <v>795320.13582478999</v>
       </c>
@@ -4331,7 +4347,7 @@
       <c r="A52" t="s">
         <v>159</v>
       </c>
-      <c r="B52" s="43">
+      <c r="B52" s="42">
         <v>223100</v>
       </c>
       <c r="C52">
@@ -4340,39 +4356,39 @@
       <c r="D52">
         <v>0.7</v>
       </c>
-      <c r="E52" s="44">
+      <c r="E52" s="43">
         <f t="shared" si="1"/>
         <v>84539.091497117464</v>
       </c>
-      <c r="F52" s="44">
+      <c r="F52" s="43">
         <f t="shared" si="1"/>
         <v>137334.15930862541</v>
       </c>
-      <c r="G52" s="44">
+      <c r="G52" s="43">
         <f t="shared" si="1"/>
         <v>223100</v>
       </c>
-      <c r="H52" s="44">
+      <c r="H52" s="43">
         <f t="shared" si="1"/>
         <v>260817.4108865335</v>
       </c>
-      <c r="I52" s="44">
+      <c r="I52" s="43">
         <f t="shared" si="1"/>
         <v>296321.69663135783</v>
       </c>
-      <c r="J52" s="44">
+      <c r="J52" s="43">
         <f t="shared" si="1"/>
         <v>362427.01925415226</v>
       </c>
-      <c r="K52" s="44">
+      <c r="K52" s="43">
         <f t="shared" si="1"/>
         <v>588764.42978686537</v>
       </c>
-      <c r="L52" s="44">
+      <c r="L52" s="43">
         <f t="shared" si="1"/>
         <v>688301.27386417065</v>
       </c>
-      <c r="M52" s="44">
+      <c r="M52" s="43">
         <f t="shared" si="1"/>
         <v>1118148.7182224444</v>
       </c>
@@ -4381,7 +4397,7 @@
       <c r="A53" t="s">
         <v>160</v>
       </c>
-      <c r="B53" s="43">
+      <c r="B53" s="42">
         <v>27883640</v>
       </c>
       <c r="C53">
@@ -4390,39 +4406,39 @@
       <c r="D53">
         <v>0.6</v>
       </c>
-      <c r="E53" s="44">
+      <c r="E53" s="43">
         <f t="shared" si="1"/>
         <v>12137059.254373169</v>
       </c>
-      <c r="F53" s="44">
+      <c r="F53" s="43">
         <f t="shared" si="1"/>
         <v>18396341.780571751</v>
       </c>
-      <c r="G53" s="44">
+      <c r="G53" s="43">
         <f t="shared" si="1"/>
         <v>27883640</v>
       </c>
-      <c r="H53" s="44">
+      <c r="H53" s="43">
         <f t="shared" si="1"/>
         <v>31878323.595307186</v>
       </c>
-      <c r="I53" s="44">
+      <c r="I53" s="43">
         <f t="shared" si="1"/>
         <v>35563477.622629322</v>
       </c>
-      <c r="J53" s="44">
+      <c r="J53" s="43">
         <f t="shared" si="1"/>
         <v>42263695.082611993</v>
       </c>
-      <c r="K53" s="44">
+      <c r="K53" s="43">
         <f t="shared" si="1"/>
         <v>64059782.798659056</v>
       </c>
-      <c r="L53" s="44">
+      <c r="L53" s="43">
         <f t="shared" si="1"/>
         <v>73237155.74798505</v>
       </c>
-      <c r="M53" s="44">
+      <c r="M53" s="43">
         <f t="shared" si="1"/>
         <v>111006770.25132319</v>
       </c>
@@ -4431,7 +4447,7 @@
       <c r="A54" t="s">
         <v>161</v>
       </c>
-      <c r="B54" s="43">
+      <c r="B54" s="42">
         <v>11065762</v>
       </c>
       <c r="C54">
@@ -4440,39 +4456,39 @@
       <c r="D54">
         <v>0.6</v>
       </c>
-      <c r="E54" s="44">
+      <c r="E54" s="43">
         <f t="shared" si="1"/>
         <v>4816652.6712004226</v>
       </c>
-      <c r="F54" s="44">
+      <c r="F54" s="43">
         <f t="shared" si="1"/>
         <v>7300680.2488650419</v>
       </c>
-      <c r="G54" s="44">
+      <c r="G54" s="43">
         <f t="shared" si="1"/>
         <v>11065762</v>
       </c>
-      <c r="H54" s="44">
+      <c r="H54" s="43">
         <f t="shared" si="1"/>
         <v>12651072.165063588</v>
       </c>
-      <c r="I54" s="44">
+      <c r="I54" s="43">
         <f t="shared" si="1"/>
         <v>14113543.972893851</v>
       </c>
-      <c r="J54" s="44">
+      <c r="J54" s="43">
         <f t="shared" si="1"/>
         <v>16772558.784461234</v>
       </c>
-      <c r="K54" s="44">
+      <c r="K54" s="43">
         <f t="shared" si="1"/>
         <v>25422445.212377403</v>
       </c>
-      <c r="L54" s="44">
+      <c r="L54" s="43">
         <f t="shared" si="1"/>
         <v>29064531.569914639</v>
       </c>
-      <c r="M54" s="44">
+      <c r="M54" s="43">
         <f t="shared" si="1"/>
         <v>44053591.998384088</v>
       </c>
@@ -4481,7 +4497,7 @@
       <c r="A55" t="s">
         <v>162</v>
       </c>
-      <c r="B55" s="43">
+      <c r="B55" s="42">
         <v>6015366</v>
       </c>
       <c r="C55">
@@ -4490,39 +4506,39 @@
       <c r="D55">
         <v>0.6</v>
       </c>
-      <c r="E55" s="44">
+      <c r="E55" s="43">
         <f t="shared" si="1"/>
         <v>2618340.1298661763</v>
       </c>
-      <c r="F55" s="44">
+      <c r="F55" s="43">
         <f t="shared" si="1"/>
         <v>3968661.5115971509</v>
       </c>
-      <c r="G55" s="44">
+      <c r="G55" s="43">
         <f t="shared" si="1"/>
         <v>6015366</v>
       </c>
-      <c r="H55" s="44">
+      <c r="H55" s="43">
         <f t="shared" si="1"/>
         <v>6877143.152479684</v>
       </c>
-      <c r="I55" s="44">
+      <c r="I55" s="43">
         <f t="shared" si="1"/>
         <v>7672145.1766313603</v>
       </c>
-      <c r="J55" s="44">
+      <c r="J55" s="43">
         <f t="shared" si="1"/>
         <v>9117589.8998233862</v>
       </c>
-      <c r="K55" s="44">
+      <c r="K55" s="43">
         <f t="shared" si="1"/>
         <v>13819682.057810189</v>
       </c>
-      <c r="L55" s="44">
+      <c r="L55" s="43">
         <f t="shared" si="1"/>
         <v>15799526.05266507</v>
       </c>
-      <c r="M55" s="44">
+      <c r="M55" s="43">
         <f t="shared" si="1"/>
         <v>23947603.381037086</v>
       </c>
@@ -4531,7 +4547,7 @@
       <c r="A56" t="s">
         <v>165</v>
       </c>
-      <c r="B56" s="43">
+      <c r="B56" s="42">
         <v>1779507</v>
       </c>
       <c r="C56">
@@ -4540,39 +4556,39 @@
       <c r="D56">
         <v>0.6</v>
       </c>
-      <c r="E56" s="44">
+      <c r="E56" s="43">
         <f t="shared" si="1"/>
         <v>774575.410619698</v>
       </c>
-      <c r="F56" s="44">
+      <c r="F56" s="43">
         <f t="shared" si="1"/>
         <v>1174036.7818878703</v>
       </c>
-      <c r="G56" s="44">
+      <c r="G56" s="43">
         <f t="shared" si="1"/>
         <v>1779507</v>
       </c>
-      <c r="H56" s="44">
+      <c r="H56" s="43">
         <f t="shared" si="1"/>
         <v>2034443.8526001018</v>
       </c>
-      <c r="I56" s="44">
+      <c r="I56" s="43">
         <f t="shared" si="1"/>
         <v>2269626.8268350991</v>
       </c>
-      <c r="J56" s="44">
+      <c r="J56" s="43">
         <f t="shared" si="1"/>
         <v>2697228.2401212188</v>
       </c>
-      <c r="K56" s="44">
+      <c r="K56" s="43">
         <f t="shared" si="1"/>
         <v>4088233.5272114179</v>
       </c>
-      <c r="L56" s="44">
+      <c r="L56" s="43">
         <f t="shared" si="1"/>
         <v>4673924.6136311339</v>
       </c>
-      <c r="M56" s="44">
+      <c r="M56" s="43">
         <f t="shared" si="1"/>
         <v>7084344.9675014224</v>
       </c>
@@ -4581,7 +4597,7 @@
       <c r="A57" t="s">
         <v>163</v>
       </c>
-      <c r="B57" s="43">
+      <c r="B57" s="42">
         <v>2929758</v>
       </c>
       <c r="C57">
@@ -4590,39 +4606,39 @@
       <c r="D57">
         <v>0.6</v>
       </c>
-      <c r="E57" s="44">
+      <c r="E57" s="43">
         <f t="shared" si="1"/>
         <v>1275251.238610663</v>
       </c>
-      <c r="F57" s="44">
+      <c r="F57" s="43">
         <f t="shared" si="1"/>
         <v>1932919.4288250864</v>
       </c>
-      <c r="G57" s="44">
+      <c r="G57" s="43">
         <f t="shared" si="1"/>
         <v>2929758</v>
       </c>
-      <c r="H57" s="44">
+      <c r="H57" s="43">
         <f t="shared" si="1"/>
         <v>3349482.8358112499</v>
       </c>
-      <c r="I57" s="44">
+      <c r="I57" s="43">
         <f t="shared" si="1"/>
         <v>3736685.1341044153</v>
       </c>
-      <c r="J57" s="44">
+      <c r="J57" s="43">
         <f t="shared" si="1"/>
         <v>4440682.7364663705</v>
       </c>
-      <c r="K57" s="44">
+      <c r="K57" s="43">
         <f t="shared" si="1"/>
         <v>6730816.3902788069</v>
       </c>
-      <c r="L57" s="44">
+      <c r="L57" s="43">
         <f t="shared" si="1"/>
         <v>7695090.8471743716</v>
       </c>
-      <c r="M57" s="44">
+      <c r="M57" s="43">
         <f t="shared" si="1"/>
         <v>11663576.67786473</v>
       </c>
@@ -4631,7 +4647,7 @@
       <c r="A58" t="s">
         <v>164</v>
       </c>
-      <c r="B58" s="43">
+      <c r="B58" s="42">
         <v>7405996</v>
       </c>
       <c r="C58">
@@ -4640,39 +4656,39 @@
       <c r="D58">
         <v>0.65</v>
       </c>
-      <c r="E58" s="44">
+      <c r="E58" s="43">
         <f t="shared" si="1"/>
         <v>3007768.9992023474</v>
       </c>
-      <c r="F58" s="44">
+      <c r="F58" s="43">
         <f t="shared" si="1"/>
         <v>4719695.4538419731</v>
       </c>
-      <c r="G58" s="44">
+      <c r="G58" s="43">
         <f t="shared" si="1"/>
         <v>7405996</v>
       </c>
-      <c r="H58" s="44">
+      <c r="H58" s="43">
         <f t="shared" si="1"/>
         <v>8561995.2311397456</v>
       </c>
-      <c r="I58" s="44">
+      <c r="I58" s="43">
         <f t="shared" si="1"/>
         <v>9639239.9548755772</v>
       </c>
-      <c r="J58" s="44">
+      <c r="J58" s="43">
         <f t="shared" si="1"/>
         <v>11621253.38137389</v>
       </c>
-      <c r="K58" s="44">
+      <c r="K58" s="43">
         <f t="shared" si="1"/>
         <v>18235701.201309595</v>
       </c>
-      <c r="L58" s="44">
+      <c r="L58" s="43">
         <f t="shared" si="1"/>
         <v>21082105.191807028</v>
       </c>
-      <c r="M58" s="44">
+      <c r="M58" s="43">
         <f t="shared" si="1"/>
         <v>33081368.967356648</v>
       </c>
@@ -4681,39 +4697,39 @@
       <c r="D60" t="s">
         <v>168</v>
       </c>
-      <c r="E60" s="45">
+      <c r="E60" s="44">
         <f>E24</f>
         <v>0.25</v>
       </c>
-      <c r="F60" s="45">
+      <c r="F60" s="44">
         <f t="shared" ref="F60:M60" si="2">F24</f>
         <v>0.5</v>
       </c>
-      <c r="G60" s="45">
+      <c r="G60" s="44">
         <f t="shared" si="2"/>
         <v>1</v>
       </c>
-      <c r="H60" s="45">
+      <c r="H60" s="44">
         <f t="shared" si="2"/>
         <v>1.25</v>
       </c>
-      <c r="I60" s="45">
+      <c r="I60" s="44">
         <f t="shared" si="2"/>
         <v>1.5</v>
       </c>
-      <c r="J60" s="45">
+      <c r="J60" s="44">
         <f t="shared" si="2"/>
         <v>2</v>
       </c>
-      <c r="K60" s="45">
+      <c r="K60" s="44">
         <f t="shared" si="2"/>
         <v>4</v>
       </c>
-      <c r="L60" s="45">
+      <c r="L60" s="44">
         <f t="shared" si="2"/>
         <v>5</v>
       </c>
-      <c r="M60" s="45">
+      <c r="M60" s="44">
         <f t="shared" si="2"/>
         <v>10</v>
       </c>
@@ -4722,39 +4738,39 @@
       <c r="D61" t="s">
         <v>112</v>
       </c>
-      <c r="E61" s="44">
+      <c r="E61" s="43">
         <f>SUM(E25:E58)</f>
         <v>103661944.99376373</v>
       </c>
-      <c r="F61" s="44">
+      <c r="F61" s="43">
         <f t="shared" ref="F61:M61" si="3">SUM(F25:F58)</f>
         <v>163252732.89508671</v>
       </c>
-      <c r="G61" s="44">
-        <f t="shared" si="3"/>
+      <c r="G61" s="43">
+        <f>SUM(G25:G58)</f>
         <v>257800646</v>
       </c>
-      <c r="H61" s="44">
+      <c r="H61" s="43">
         <f t="shared" si="3"/>
         <v>298830505.00587934</v>
       </c>
-      <c r="I61" s="44">
+      <c r="I61" s="43">
         <f t="shared" si="3"/>
         <v>337232658.66429305</v>
       </c>
-      <c r="J61" s="44">
+      <c r="J61" s="43">
         <f t="shared" si="3"/>
         <v>408279669.36056608</v>
       </c>
-      <c r="K61" s="44">
+      <c r="K61" s="43">
         <f t="shared" si="3"/>
         <v>648555689.20624173</v>
       </c>
-      <c r="L61" s="44">
+      <c r="L61" s="43">
         <f t="shared" si="3"/>
         <v>753254554.49843431</v>
       </c>
-      <c r="M61" s="44">
+      <c r="M61" s="43">
         <f t="shared" si="3"/>
         <v>1201614609.967025</v>
       </c>
@@ -4763,39 +4779,39 @@
       <c r="D62" t="s">
         <v>170</v>
       </c>
-      <c r="E62" s="45">
+      <c r="E62" s="44">
         <f>LOG(E60)</f>
         <v>-0.6020599913279624</v>
       </c>
-      <c r="F62" s="45">
+      <c r="F62" s="44">
         <f t="shared" ref="F62:M62" si="4">LOG(F60)</f>
         <v>-0.3010299956639812</v>
       </c>
-      <c r="G62" s="45">
+      <c r="G62" s="44">
         <f t="shared" si="4"/>
         <v>0</v>
       </c>
-      <c r="H62" s="45">
+      <c r="H62" s="44">
         <f t="shared" si="4"/>
         <v>9.691001300805642E-2</v>
       </c>
-      <c r="I62" s="45">
+      <c r="I62" s="44">
         <f t="shared" si="4"/>
         <v>0.17609125905568124</v>
       </c>
-      <c r="J62" s="45">
+      <c r="J62" s="44">
         <f t="shared" si="4"/>
         <v>0.3010299956639812</v>
       </c>
-      <c r="K62" s="45">
+      <c r="K62" s="44">
         <f t="shared" si="4"/>
         <v>0.6020599913279624</v>
       </c>
-      <c r="L62" s="45">
+      <c r="L62" s="44">
         <f t="shared" si="4"/>
         <v>0.69897000433601886</v>
       </c>
-      <c r="M62" s="45">
+      <c r="M62" s="44">
         <f t="shared" si="4"/>
         <v>1</v>
       </c>
@@ -4848,6 +4864,111 @@
 </file>
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E40FBC7-515F-444A-AA65-63C61A66544C}">
+  <dimension ref="A1:D6"/>
+  <sheetViews>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="K12" sqref="K12"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <cols>
+    <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>84</v>
+      </c>
+      <c r="B1">
+        <v>50</v>
+      </c>
+      <c r="C1">
+        <v>300</v>
+      </c>
+      <c r="D1">
+        <v>1000</v>
+      </c>
+    </row>
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>17</v>
+      </c>
+      <c r="B2">
+        <f>-B1-$B3</f>
+        <v>-35.1</v>
+      </c>
+      <c r="C2">
+        <f t="shared" ref="C2:D2" si="0">-C1-$B3</f>
+        <v>-285.10000000000002</v>
+      </c>
+      <c r="D2">
+        <f t="shared" si="0"/>
+        <v>-985.1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>171</v>
+      </c>
+      <c r="B3">
+        <v>-14.9</v>
+      </c>
+    </row>
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
+        <v>172</v>
+      </c>
+      <c r="B4">
+        <v>25.13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>173</v>
+      </c>
+    </row>
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>174</v>
+      </c>
+      <c r="B5">
+        <f>ABS(B2)*$B4</f>
+        <v>882.06299999999999</v>
+      </c>
+      <c r="C5">
+        <f t="shared" ref="C5:D5" si="1">ABS(C2)*$B4</f>
+        <v>7164.5630000000001</v>
+      </c>
+      <c r="D5">
+        <f t="shared" si="1"/>
+        <v>24755.562999999998</v>
+      </c>
+    </row>
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+      <c r="A6" t="s">
+        <v>175</v>
+      </c>
+      <c r="B6">
+        <f>-B5</f>
+        <v>-882.06299999999999</v>
+      </c>
+      <c r="C6">
+        <f t="shared" ref="C6:D6" si="2">-C5</f>
+        <v>-7164.5630000000001</v>
+      </c>
+      <c r="D6">
+        <f t="shared" si="2"/>
+        <v>-24755.562999999998</v>
+      </c>
+    </row>
+  </sheetData>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -4951,7 +5072,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -4965,26 +5086,26 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A1" s="42" t="s">
+      <c r="A1" s="45" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="42"/>
-      <c r="C1" s="42"/>
-      <c r="D1" s="42"/>
-      <c r="E1" s="42"/>
-      <c r="F1" s="42"/>
-      <c r="G1" s="42"/>
+      <c r="B1" s="45"/>
+      <c r="C1" s="45"/>
+      <c r="D1" s="45"/>
+      <c r="E1" s="45"/>
+      <c r="F1" s="45"/>
+      <c r="G1" s="45"/>
     </row>
     <row r="2" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A2" s="42" t="s">
+      <c r="A2" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="42"/>
-      <c r="C2" s="42"/>
-      <c r="D2" s="42"/>
-      <c r="E2" s="42"/>
-      <c r="F2" s="42"/>
-      <c r="G2" s="42"/>
+      <c r="B2" s="45"/>
+      <c r="C2" s="45"/>
+      <c r="D2" s="45"/>
+      <c r="E2" s="45"/>
+      <c r="F2" s="45"/>
+      <c r="G2" s="45"/>
     </row>
     <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
@@ -5056,15 +5177,15 @@
       <c r="H5" s="2"/>
     </row>
     <row r="6" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A6" s="42" t="s">
+      <c r="A6" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B6" s="42"/>
-      <c r="C6" s="42"/>
-      <c r="D6" s="42"/>
-      <c r="E6" s="42"/>
-      <c r="F6" s="42"/>
-      <c r="G6" s="42"/>
+      <c r="B6" s="45"/>
+      <c r="C6" s="45"/>
+      <c r="D6" s="45"/>
+      <c r="E6" s="45"/>
+      <c r="F6" s="45"/>
+      <c r="G6" s="45"/>
     </row>
     <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
@@ -5142,22 +5263,22 @@
       </c>
     </row>
     <row r="11" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A11" s="42" t="s">
+      <c r="A11" s="45" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="42"/>
-      <c r="C11" s="42"/>
-      <c r="D11" s="42"/>
-      <c r="E11" s="42"/>
-      <c r="F11" s="42"/>
-      <c r="G11" s="42"/>
+      <c r="B11" s="45"/>
+      <c r="C11" s="45"/>
+      <c r="D11" s="45"/>
+      <c r="E11" s="45"/>
+      <c r="F11" s="45"/>
+      <c r="G11" s="45"/>
     </row>
     <row r="12" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A12" s="42" t="s">
+      <c r="A12" s="45" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="42"/>
-      <c r="C12" s="42"/>
+      <c r="B12" s="45"/>
+      <c r="C12" s="45"/>
     </row>
     <row r="13" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
@@ -5171,11 +5292,11 @@
       </c>
     </row>
     <row r="14" spans="1:8" x14ac:dyDescent="0.35">
-      <c r="A14" s="42" t="s">
+      <c r="A14" s="45" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="42"/>
-      <c r="C14" s="42"/>
+      <c r="B14" s="45"/>
+      <c r="C14" s="45"/>
     </row>
     <row r="15" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
@@ -5203,7 +5324,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD4092A-9167-4B1E-A144-D4BB7A88B529}">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -5457,7 +5578,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8827ECA-5F74-4389-B5A8-A15818A92C9F}">
   <dimension ref="A1:E42"/>
   <sheetViews>

</xml_diff>

<commit_message>
Calculate cashflows and transfer rates for combined FT and HTSE component
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/synfuels_model_numbers.xlsx
+++ b/use_cases/2022_05/data/synfuels_model_numbers.xlsx
@@ -1,26 +1,27 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garrm\projects\FORCE\use_cases\2022_05\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/projects/FORCE/use_cases/2022_05/data/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FCE4C4CA-C971-4B15-88C9-3483D082D055}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8373BB-AADB-5743-BADF-39C03BB54623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" activeTab="3" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="0" yWindow="500" windowWidth="43500" windowHeight="26140" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
     <sheet name="HTSE" sheetId="2" r:id="rId2"/>
     <sheet name="FT" sheetId="7" r:id="rId3"/>
     <sheet name="Syn_base" sheetId="8" r:id="rId4"/>
-    <sheet name="Capacity_Market" sheetId="3" r:id="rId5"/>
-    <sheet name="Transfer_rates" sheetId="4" r:id="rId6"/>
-    <sheet name="grid_sellall_test" sheetId="5" r:id="rId7"/>
-    <sheet name="grid_sellnothing_test" sheetId="6" r:id="rId8"/>
+    <sheet name="FT_HTSE_combined" sheetId="9" r:id="rId5"/>
+    <sheet name="Capacity_Market" sheetId="3" r:id="rId6"/>
+    <sheet name="Transfer_rates" sheetId="4" r:id="rId7"/>
+    <sheet name="grid_sellall_test" sheetId="5" r:id="rId8"/>
+    <sheet name="grid_sellnothing_test" sheetId="6" r:id="rId9"/>
   </sheets>
   <calcPr calcId="191029"/>
   <extLst>
@@ -42,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="301" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="222">
   <si>
     <t>Source</t>
   </si>
@@ -570,17 +571,156 @@
   </si>
   <si>
     <t>FT h2 capacity</t>
+  </si>
+  <si>
+    <t>electricity</t>
+  </si>
+  <si>
+    <t>Cashflows</t>
+  </si>
+  <si>
+    <t>Capacity</t>
+  </si>
+  <si>
+    <t>HTSE capacity (MWe)</t>
+  </si>
+  <si>
+    <t>electricity (Mwe)</t>
+  </si>
+  <si>
+    <t>All cashflows will be calculated based on it</t>
+  </si>
+  <si>
+    <t>Name</t>
+  </si>
+  <si>
+    <t>Driver</t>
+  </si>
+  <si>
+    <t>Repeating?</t>
+  </si>
+  <si>
+    <t>htse_capex</t>
+  </si>
+  <si>
+    <t>htse_noak_capex Function</t>
+  </si>
+  <si>
+    <t>None</t>
+  </si>
+  <si>
+    <t>htse_fom</t>
+  </si>
+  <si>
+    <t>htse_capacity</t>
+  </si>
+  <si>
+    <t>$/MW-ac-year</t>
+  </si>
+  <si>
+    <t>year</t>
+  </si>
+  <si>
+    <t>yes</t>
+  </si>
+  <si>
+    <t>htse_vom</t>
+  </si>
+  <si>
+    <t>electricity (activity)</t>
+  </si>
+  <si>
+    <t>$/MWh-ac</t>
+  </si>
+  <si>
+    <t>hour</t>
+  </si>
+  <si>
+    <t>elec_cap_market</t>
+  </si>
+  <si>
+    <t>$/MWe-year</t>
+  </si>
+  <si>
+    <t>ft_capex</t>
+  </si>
+  <si>
+    <t>scaling factor</t>
+  </si>
+  <si>
+    <t>$/2020</t>
+  </si>
+  <si>
+    <t>none</t>
+  </si>
+  <si>
+    <t>no</t>
+  </si>
+  <si>
+    <t>depreciate</t>
+  </si>
+  <si>
+    <t>ft_fom</t>
+  </si>
+  <si>
+    <t>$/year (2020)</t>
+  </si>
+  <si>
+    <t>ft_vom</t>
+  </si>
+  <si>
+    <t>h2</t>
+  </si>
+  <si>
+    <t>$/kg-h2</t>
+  </si>
+  <si>
+    <t>co2_shipping</t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Current transfer rates</t>
+  </si>
+  <si>
+    <t>Resource</t>
+  </si>
+  <si>
+    <t>naphtha</t>
+  </si>
+  <si>
+    <t>jet_fuel</t>
+  </si>
+  <si>
+    <t>diesel</t>
+  </si>
+  <si>
+    <t>Combined HTSE+FT</t>
+  </si>
+  <si>
+    <t>Mwe</t>
+  </si>
+  <si>
+    <t>kg</t>
+  </si>
+  <si>
+    <t>FT (capacity expressed in kg-H2)</t>
+  </si>
+  <si>
+    <t>Just need to redefine this</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <numFmts count="2">
+  <numFmts count="3">
+    <numFmt numFmtId="6" formatCode="&quot;$&quot;#,##0_);[Red]\(&quot;$&quot;#,##0\)"/>
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="5" x14ac:knownFonts="1">
+  <fonts count="6" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -617,8 +757,15 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <sz val="12"/>
+      <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="3">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -630,8 +777,13 @@
         <fgColor rgb="FFC6EFCE"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFC7CE"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="15">
+  <borders count="18">
     <border>
       <left/>
       <right/>
@@ -787,13 +939,45 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="medium">
+        <color indexed="64"/>
+      </left>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="medium">
+        <color indexed="64"/>
+      </right>
+      <top style="medium">
+        <color indexed="64"/>
+      </top>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="3">
+  <cellStyleXfs count="4">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="46">
+  <cellXfs count="54">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -852,8 +1036,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="2" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="3">
+  <cellStyles count="4">
+    <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -2340,13 +2539,13 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="8.7265625" style="1"/>
-    <col min="2" max="2" width="85.7265625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6640625" style="1"/>
+    <col min="2" max="2" width="85.6640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2357,7 +2556,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
         <v>2</v>
       </c>
@@ -2375,7 +2574,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2395,7 +2594,7 @@
         <v>49.222000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2415,7 +2614,7 @@
         <v>49.24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -2435,7 +2634,7 @@
         <v>49.220999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -2458,7 +2657,7 @@
         <v>49.220999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2469,7 +2668,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2497,14 +2696,14 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.36328125" customWidth="1"/>
-    <col min="3" max="3" width="12.08984375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.33203125" customWidth="1"/>
+    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2512,7 +2711,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
@@ -2523,7 +2722,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
@@ -2534,7 +2733,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" s="22"/>
       <c r="B4" s="16">
         <f>1/B3</f>
@@ -2544,7 +2743,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" s="22" t="s">
         <v>30</v>
       </c>
@@ -2555,7 +2754,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" s="22" t="s">
         <v>36</v>
       </c>
@@ -2566,7 +2765,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A7" s="22" t="s">
         <v>37</v>
       </c>
@@ -2577,7 +2776,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" s="22" t="s">
         <v>32</v>
       </c>
@@ -2588,7 +2787,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>35</v>
       </c>
@@ -2599,7 +2798,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>38</v>
       </c>
@@ -2610,7 +2809,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" s="22" t="s">
         <v>40</v>
       </c>
@@ -2621,7 +2820,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
         <v>42</v>
       </c>
@@ -2632,7 +2831,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
         <v>44</v>
       </c>
@@ -2643,7 +2842,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A14" s="40" t="s">
         <v>46</v>
       </c>
@@ -2654,7 +2853,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A16" s="7" t="s">
         <v>97</v>
       </c>
@@ -2668,22 +2867,22 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8E35C99A-39AC-4C72-B859-1A7DCC98EEE1}">
   <dimension ref="A1:M63"/>
   <sheetViews>
-    <sheetView topLeftCell="D41" workbookViewId="0">
+    <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="B66" sqref="B66"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.81640625" customWidth="1"/>
-    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.54296875" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.90625" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="13.08984375" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.83203125" customWidth="1"/>
+    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="1" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2691,7 +2890,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
@@ -2705,7 +2904,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
       <c r="A3" s="20" t="s">
         <v>102</v>
       </c>
@@ -2719,7 +2918,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A4" s="22" t="s">
         <v>103</v>
       </c>
@@ -2734,7 +2933,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A5" s="22"/>
       <c r="B5" s="11" t="s">
         <v>109</v>
@@ -2747,7 +2946,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A6" s="22"/>
       <c r="B6" s="11" t="s">
         <v>107</v>
@@ -2760,7 +2959,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A7" s="22"/>
       <c r="B7" s="11" t="s">
         <v>114</v>
@@ -2772,7 +2971,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A8" s="22"/>
       <c r="B8" s="11" t="s">
         <v>108</v>
@@ -2785,7 +2984,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A9" s="22" t="s">
         <v>113</v>
       </c>
@@ -2798,7 +2997,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A10" s="22" t="s">
         <v>104</v>
       </c>
@@ -2813,7 +3012,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A11" s="24" t="s">
         <v>112</v>
       </c>
@@ -2828,7 +3027,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A12" s="26" t="s">
         <v>115</v>
       </c>
@@ -2842,7 +3041,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A13" s="28" t="s">
         <v>118</v>
       </c>
@@ -2857,7 +3056,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
       <c r="A14" s="28" t="s">
         <v>119</v>
       </c>
@@ -2872,7 +3071,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A15" s="28" t="s">
         <v>122</v>
       </c>
@@ -2884,7 +3083,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A16" s="28" t="s">
         <v>123</v>
       </c>
@@ -2897,7 +3096,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A17" s="26" t="s">
         <v>124</v>
       </c>
@@ -2909,7 +3108,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A18" s="38" t="s">
         <v>125</v>
       </c>
@@ -2922,7 +3121,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+    <row r="19" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A19" s="30" t="s">
         <v>126</v>
       </c>
@@ -2936,7 +3135,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>127</v>
       </c>
@@ -2947,12 +3146,12 @@
         <v>167</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E23" t="s">
         <v>168</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -2993,7 +3192,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>133</v>
       </c>
@@ -3043,7 +3242,7 @@
         <v>52744050.147983856</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A26" t="s">
         <v>134</v>
       </c>
@@ -3093,7 +3292,7 @@
         <v>109714043.08323221</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A27" t="s">
         <v>135</v>
       </c>
@@ -3143,7 +3342,7 @@
         <v>10143750.800344583</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A28" t="s">
         <v>136</v>
       </c>
@@ -3193,7 +3392,7 @@
         <v>91453943.585316852</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A29" t="s">
         <v>137</v>
       </c>
@@ -3243,7 +3442,7 @@
         <v>24874548.15481044</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A30" t="s">
         <v>138</v>
       </c>
@@ -3293,7 +3492,7 @@
         <v>131356340.74097335</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A31" t="s">
         <v>139</v>
       </c>
@@ -3343,7 +3542,7 @@
         <v>20984238.355974279</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>140</v>
       </c>
@@ -3393,7 +3592,7 @@
         <v>4048229.6184328939</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>148</v>
       </c>
@@ -3443,7 +3642,7 @@
         <v>378401.37326092686</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>141</v>
       </c>
@@ -3493,7 +3692,7 @@
         <v>51197086.5979748</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>142</v>
       </c>
@@ -3543,7 +3742,7 @@
         <v>231445154.62924495</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>143</v>
       </c>
@@ -3593,7 +3792,7 @@
         <v>573891.39171139395</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>144</v>
       </c>
@@ -3643,7 +3842,7 @@
         <v>33056871.522694372</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>145</v>
       </c>
@@ -3693,7 +3892,7 @@
         <v>8149930.9028214812</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>146</v>
       </c>
@@ -3743,7 +3942,7 @@
         <v>4914396.4312045546</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A40" t="s">
         <v>147</v>
       </c>
@@ -3793,7 +3992,7 @@
         <v>492339.1378235101</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A41" t="s">
         <v>149</v>
       </c>
@@ -3843,7 +4042,7 @@
         <v>4532166.6054012291</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A42" t="s">
         <v>150</v>
       </c>
@@ -3893,7 +4092,7 @@
         <v>29840688.281019572</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A43" t="s">
         <v>151</v>
       </c>
@@ -3943,7 +4142,7 @@
         <v>4857025.5285712406</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
         <v>152</v>
       </c>
@@ -3993,7 +4192,7 @@
         <v>147629.71153724933</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A45" t="s">
         <v>153</v>
       </c>
@@ -4043,7 +4242,7 @@
         <v>86448.97208569193</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
         <v>154</v>
       </c>
@@ -4093,7 +4292,7 @@
         <v>251816.5136636867</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
         <v>155</v>
       </c>
@@ -4143,7 +4342,7 @@
         <v>147705993.52604714</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A48" t="s">
         <v>156</v>
       </c>
@@ -4193,7 +4392,7 @@
         <v>1839938.8512649538</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A49" t="s">
         <v>157</v>
       </c>
@@ -4243,7 +4442,7 @@
         <v>2617413.9775833129</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A50" t="s">
         <v>158</v>
       </c>
@@ -4293,7 +4492,7 @@
         <v>1457546.4285322789</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A51" t="s">
         <v>166</v>
       </c>
@@ -4343,7 +4542,7 @@
         <v>795320.13582478999</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A52" t="s">
         <v>159</v>
       </c>
@@ -4393,7 +4592,7 @@
         <v>1118148.7182224444</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A53" t="s">
         <v>160</v>
       </c>
@@ -4443,7 +4642,7 @@
         <v>111006770.25132319</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
         <v>161</v>
       </c>
@@ -4493,7 +4692,7 @@
         <v>44053591.998384088</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A55" t="s">
         <v>162</v>
       </c>
@@ -4543,7 +4742,7 @@
         <v>23947603.381037086</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A56" t="s">
         <v>165</v>
       </c>
@@ -4593,7 +4792,7 @@
         <v>7084344.9675014224</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A57" t="s">
         <v>163</v>
       </c>
@@ -4643,7 +4842,7 @@
         <v>11663576.67786473</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
         <v>164</v>
       </c>
@@ -4693,7 +4892,7 @@
         <v>33081368.967356648</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D60" t="s">
         <v>168</v>
       </c>
@@ -4734,7 +4933,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D61" t="s">
         <v>112</v>
       </c>
@@ -4775,7 +4974,7 @@
         <v>1201614609.967025</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D62" t="s">
         <v>170</v>
       </c>
@@ -4816,7 +5015,7 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
       <c r="D63" t="s">
         <v>169</v>
       </c>
@@ -4867,19 +5066,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E40FBC7-515F-444A-AA65-63C61A66544C}">
   <dimension ref="A1:D6"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
       <selection activeCell="K12" sqref="K12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.453125" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.453125" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.453125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>84</v>
       </c>
@@ -4893,7 +5092,7 @@
         <v>1000</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>17</v>
       </c>
@@ -4910,7 +5109,7 @@
         <v>-985.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>171</v>
       </c>
@@ -4918,7 +5117,7 @@
         <v>-14.9</v>
       </c>
     </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>172</v>
       </c>
@@ -4929,7 +5128,7 @@
         <v>173</v>
       </c>
     </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>174</v>
       </c>
@@ -4946,7 +5145,7 @@
         <v>24755.562999999998</v>
       </c>
     </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>175</v>
       </c>
@@ -4969,6 +5168,465 @@
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9120567B-0376-BC4D-A254-A4551F910A7D}">
+  <dimension ref="A1:I27"/>
+  <sheetViews>
+    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
+      <selection activeCell="K41" sqref="K41"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A1" t="s">
+        <v>62</v>
+      </c>
+      <c r="B1" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A2" t="s">
+        <v>178</v>
+      </c>
+      <c r="B2" t="s">
+        <v>179</v>
+      </c>
+      <c r="C2" t="s">
+        <v>181</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="A4" t="s">
+        <v>177</v>
+      </c>
+      <c r="B4" s="46" t="s">
+        <v>17</v>
+      </c>
+      <c r="C4" s="47"/>
+      <c r="D4" s="47"/>
+      <c r="E4" s="47"/>
+      <c r="F4" s="47"/>
+      <c r="G4" s="47"/>
+      <c r="H4" s="48"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B5" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C5" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D5" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E5" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F5" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G5" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="H5" s="23"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B6" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C6" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D6" s="12">
+        <v>1</v>
+      </c>
+      <c r="E6" s="12"/>
+      <c r="F6" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H6" s="23"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B7" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C7" s="12"/>
+      <c r="D7" s="12">
+        <v>20</v>
+      </c>
+      <c r="E7" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F7" s="12"/>
+      <c r="G7" s="12"/>
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B8" s="22" t="s">
+        <v>188</v>
+      </c>
+      <c r="C8" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="D8" s="12">
+        <v>-30320</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>190</v>
+      </c>
+      <c r="F8" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="G8" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B9" s="22" t="s">
+        <v>193</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>194</v>
+      </c>
+      <c r="D9" s="12">
+        <v>-3.1680000000000001</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>195</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>196</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B10" s="40" t="s">
+        <v>197</v>
+      </c>
+      <c r="C10" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="D10" s="31">
+        <v>-27933.45</v>
+      </c>
+      <c r="E10" s="31" t="s">
+        <v>198</v>
+      </c>
+      <c r="F10" s="31" t="s">
+        <v>191</v>
+      </c>
+      <c r="G10" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="H10" s="41"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B11" s="46" t="s">
+        <v>220</v>
+      </c>
+      <c r="C11" s="47"/>
+      <c r="D11" s="47"/>
+      <c r="E11" s="47"/>
+      <c r="F11" s="47"/>
+      <c r="G11" s="47"/>
+      <c r="H11" s="48"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B12" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C12" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D12" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E12" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F12" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G12" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="H12" s="23" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B13" s="22" t="s">
+        <v>199</v>
+      </c>
+      <c r="C13" s="12">
+        <v>1</v>
+      </c>
+      <c r="D13" s="12">
+        <v>-350734933</v>
+      </c>
+      <c r="E13" s="51" t="s">
+        <v>201</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>202</v>
+      </c>
+      <c r="G13" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="H13" s="23">
+        <v>0.66420000000000001</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B14" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C14" s="12"/>
+      <c r="D14" s="12">
+        <v>20</v>
+      </c>
+      <c r="E14" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F14" s="12"/>
+      <c r="G14" s="12"/>
+      <c r="H14" s="23"/>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B15" s="22" t="s">
+        <v>205</v>
+      </c>
+      <c r="C15" s="12">
+        <v>1</v>
+      </c>
+      <c r="D15" s="12">
+        <v>-27412351</v>
+      </c>
+      <c r="E15" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F15" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="G15" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
+      <c r="B16" s="22" t="s">
+        <v>207</v>
+      </c>
+      <c r="C16" s="12">
+        <v>1</v>
+      </c>
+      <c r="D16" s="12">
+        <v>-9636868</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>206</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="H16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B17" s="52" t="s">
+        <v>210</v>
+      </c>
+      <c r="C17" s="31" t="s">
+        <v>208</v>
+      </c>
+      <c r="D17" s="31">
+        <v>0.13100999999999999</v>
+      </c>
+      <c r="E17" s="31" t="s">
+        <v>209</v>
+      </c>
+      <c r="F17" s="31" t="s">
+        <v>196</v>
+      </c>
+      <c r="G17" s="31" t="s">
+        <v>192</v>
+      </c>
+      <c r="H17" s="41"/>
+      <c r="I17" s="53" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="19" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
+    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A20" s="46" t="s">
+        <v>212</v>
+      </c>
+      <c r="B20" s="47"/>
+      <c r="C20" s="47"/>
+      <c r="D20" s="48"/>
+      <c r="G20" s="46" t="s">
+        <v>217</v>
+      </c>
+      <c r="H20" s="48"/>
+    </row>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A21" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B21" s="12" t="s">
+        <v>213</v>
+      </c>
+      <c r="C21" s="12" t="s">
+        <v>211</v>
+      </c>
+      <c r="D21" s="23" t="s">
+        <v>28</v>
+      </c>
+      <c r="G21" s="22" t="s">
+        <v>213</v>
+      </c>
+      <c r="H21" s="23" t="s">
+        <v>211</v>
+      </c>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A22" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B22" s="12" t="s">
+        <v>176</v>
+      </c>
+      <c r="C22" s="12">
+        <v>-1</v>
+      </c>
+      <c r="D22" s="23" t="s">
+        <v>218</v>
+      </c>
+      <c r="G22" s="22" t="s">
+        <v>176</v>
+      </c>
+      <c r="H22" s="49">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A23" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B23" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C23" s="12">
+        <v>25.13</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="H23" s="49">
+        <f>(C25/ABS(C$24))*(C$23)</f>
+        <v>17.377632075471695</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A24" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>208</v>
+      </c>
+      <c r="C24" s="12">
+        <v>-1.06</v>
+      </c>
+      <c r="D24" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>215</v>
+      </c>
+      <c r="H24" s="49">
+        <f>(C26/ABS(C$24))*(C$23)</f>
+        <v>21.052301886792449</v>
+      </c>
+    </row>
+    <row r="25" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A25" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B25" s="12" t="s">
+        <v>214</v>
+      </c>
+      <c r="C25" s="12">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="D25" s="23" t="s">
+        <v>219</v>
+      </c>
+      <c r="G25" s="40" t="s">
+        <v>216</v>
+      </c>
+      <c r="H25" s="50">
+        <f>(C27/ABS(C$24))*(C$23)</f>
+        <v>11.664113207547167</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="A26" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B26" s="12" t="s">
+        <v>215</v>
+      </c>
+      <c r="C26" s="12">
+        <v>0.88800000000000001</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>219</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A27" s="40" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="31" t="s">
+        <v>216</v>
+      </c>
+      <c r="C27" s="31">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="D27" s="41" t="s">
+        <v>219</v>
+      </c>
+    </row>
+  </sheetData>
+  <mergeCells count="4">
+    <mergeCell ref="B11:H11"/>
+    <mergeCell ref="B4:H4"/>
+    <mergeCell ref="A20:D20"/>
+    <mergeCell ref="G20:H20"/>
+  </mergeCells>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
   <dimension ref="A1:C11"/>
   <sheetViews>
@@ -4976,17 +5634,17 @@
       <selection activeCell="E33" sqref="E33"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A2" t="s">
         <v>48</v>
       </c>
@@ -4997,7 +5655,7 @@
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>55</v>
       </c>
@@ -5008,7 +5666,7 @@
         <v>1.395</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>54</v>
       </c>
@@ -5019,7 +5677,7 @@
         <v>1.395</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>53</v>
       </c>
@@ -5030,7 +5688,7 @@
         <v>1.395</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
         <v>52</v>
       </c>
@@ -5041,17 +5699,17 @@
         <v>1.395</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>50</v>
       </c>
@@ -5059,7 +5717,7 @@
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>59</v>
       </c>
@@ -5072,7 +5730,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
   <dimension ref="A1:H15"/>
   <sheetViews>
@@ -5080,12 +5738,12 @@
       <selection activeCell="G19" sqref="G19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A1" s="45" t="s">
         <v>61</v>
       </c>
@@ -5096,7 +5754,7 @@
       <c r="F1" s="45"/>
       <c r="G1" s="45"/>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A2" s="45" t="s">
         <v>62</v>
       </c>
@@ -5107,7 +5765,7 @@
       <c r="F2" s="45"/>
       <c r="G2" s="45"/>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>63</v>
       </c>
@@ -5132,7 +5790,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>64</v>
       </c>
@@ -5157,7 +5815,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>65</v>
       </c>
@@ -5176,7 +5834,7 @@
       <c r="F5" s="2"/>
       <c r="H5" s="2"/>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A6" s="45" t="s">
         <v>68</v>
       </c>
@@ -5187,7 +5845,7 @@
       <c r="F6" s="45"/>
       <c r="G6" s="45"/>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>69</v>
       </c>
@@ -5212,7 +5870,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>70</v>
       </c>
@@ -5237,7 +5895,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>71</v>
       </c>
@@ -5262,7 +5920,7 @@
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A11" s="45" t="s">
         <v>17</v>
       </c>
@@ -5273,14 +5931,14 @@
       <c r="F11" s="45"/>
       <c r="G11" s="45"/>
     </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A12" s="45" t="s">
         <v>62</v>
       </c>
       <c r="B12" s="45"/>
       <c r="C12" s="45"/>
     </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>65</v>
       </c>
@@ -5291,14 +5949,14 @@
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A14" s="45" t="s">
         <v>68</v>
       </c>
       <c r="B14" s="45"/>
       <c r="C14" s="45"/>
     </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>64</v>
       </c>
@@ -5324,7 +5982,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9CD4092A-9167-4B1E-A144-D4BB7A88B529}">
   <dimension ref="A1:E22"/>
   <sheetViews>
@@ -5332,13 +5990,13 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="32.90625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.83203125" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -5349,7 +6007,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>0.5</v>
       </c>
@@ -5357,7 +6015,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -5368,7 +6026,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -5379,7 +6037,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -5390,12 +6048,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -5412,7 +6070,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -5429,7 +6087,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -5446,7 +6104,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -5463,7 +6121,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -5480,7 +6138,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -5497,17 +6155,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -5521,12 +6179,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -5540,7 +6198,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -5554,12 +6212,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -5578,7 +6236,7 @@
 </worksheet>
 </file>
 
-<file path=xl/worksheets/sheet8.xml><?xml version="1.0" encoding="utf-8"?>
+<file path=xl/worksheets/sheet9.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8827ECA-5F74-4389-B5A8-A15818A92C9F}">
   <dimension ref="A1:E42"/>
   <sheetViews>
@@ -5586,14 +6244,14 @@
       <selection activeCell="B50" sqref="B50"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="31.90625" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -5604,7 +6262,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
       <c r="B2">
         <v>0</v>
       </c>
@@ -5612,7 +6270,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -5623,7 +6281,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -5634,7 +6292,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -5645,12 +6303,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -5667,7 +6325,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -5684,7 +6342,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -5701,7 +6359,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -5718,7 +6376,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -5735,7 +6393,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -5752,17 +6410,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -5776,7 +6434,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -5790,7 +6448,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -5804,7 +6462,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -5818,12 +6476,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -5840,7 +6498,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
       <c r="E42" t="s">
         <v>94</v>
       </c>

</xml_diff>

<commit_message>
Add comments and references for future users
</commit_message>
<xml_diff>
--- a/use_cases/2022_05/data/synfuels_model_numbers.xlsx
+++ b/use_cases/2022_05/data/synfuels_model_numbers.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="10611"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25225"/>
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="/Users/garrm/projects/FORCE/use_cases/2022_05/data/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\garrm\projects\FORCE\use_cases\2022_05\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BD8373BB-AADB-5743-BADF-39C03BB54623}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{257D98F4-FF1F-4C66-ADBC-B12F9A065227}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="500" windowWidth="43500" windowHeight="26140" activeTab="4" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
+    <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10420" firstSheet="4" activeTab="8" xr2:uid="{3CE7F202-39F9-48AF-B0C7-575379157397}"/>
   </bookViews>
   <sheets>
     <sheet name="MACRS" sheetId="1" r:id="rId1"/>
@@ -43,7 +43,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="393" uniqueCount="222">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="410" uniqueCount="234">
   <si>
     <t>Source</t>
   </si>
@@ -441,9 +441,6 @@
     <t>Scaling exponent</t>
   </si>
   <si>
-    <t>Source: Performance and Cost Analysis of Liquid Fuel Production from H2 and CO2 Based on the Fischer-Tropsch Process</t>
-  </si>
-  <si>
     <t>CO2 compressor 1</t>
   </si>
   <si>
@@ -546,9 +543,6 @@
     <t>Diesel distillation</t>
   </si>
   <si>
-    <t>Assumption: Every component size increases in the same way as the whole process</t>
-  </si>
-  <si>
     <t>Size factor</t>
   </si>
   <si>
@@ -585,9 +579,6 @@
     <t>HTSE capacity (MWe)</t>
   </si>
   <si>
-    <t>electricity (Mwe)</t>
-  </si>
-  <si>
     <t>All cashflows will be calculated based on it</t>
   </si>
   <si>
@@ -709,6 +700,51 @@
   </si>
   <si>
     <t>Just need to redefine this</t>
+  </si>
+  <si>
+    <t xml:space="preserve"> Nuclear refinery dedicated to synthetic fuel production, not connected to the grid</t>
+  </si>
+  <si>
+    <t>Synfuel baseline case</t>
+  </si>
+  <si>
+    <t>Performance and Cost Analysis of Liquid Fuel Production from H2 and CO2 Based on the Fischer-Tropsch Process</t>
+  </si>
+  <si>
+    <t>Assumption</t>
+  </si>
+  <si>
+    <t xml:space="preserve">: </t>
+  </si>
+  <si>
+    <t>Every component size increases in the same way as the whole process</t>
+  </si>
+  <si>
+    <t>Electricity (MWe)</t>
+  </si>
+  <si>
+    <t>Comment</t>
+  </si>
+  <si>
+    <t>Case without h2 storage, HTSE and FT combined into 1 component</t>
+  </si>
+  <si>
+    <t>Acronyms</t>
+  </si>
+  <si>
+    <t>Equations</t>
+  </si>
+  <si>
+    <t>Average</t>
+  </si>
+  <si>
+    <t>Used to compute a negative cashflow for the capacity of the NPP not sold on the capacity market</t>
+  </si>
+  <si>
+    <t>FT ANL report</t>
+  </si>
+  <si>
+    <t>Dan Wendt report</t>
   </si>
 </sst>
 </file>
@@ -720,7 +756,7 @@
     <numFmt numFmtId="44" formatCode="_(&quot;$&quot;* #,##0.00_);_(&quot;$&quot;* \(#,##0.00\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
     <numFmt numFmtId="164" formatCode="_(&quot;$&quot;* #,##0_);_(&quot;$&quot;* \(#,##0\);_(&quot;$&quot;* &quot;-&quot;??_);_(@_)"/>
   </numFmts>
-  <fonts count="6" x14ac:knownFonts="1">
+  <fonts count="7" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -760,6 +796,14 @@
     <font>
       <sz val="12"/>
       <color rgb="FF9C0006"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <u/>
+      <sz val="11"/>
+      <color theme="10"/>
       <name val="Calibri"/>
       <family val="2"/>
       <scheme val="minor"/>
@@ -971,13 +1015,14 @@
       <diagonal/>
     </border>
   </borders>
-  <cellStyleXfs count="4">
+  <cellStyleXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="44" fontId="1" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="2" fillId="2" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" applyNumberFormat="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="54">
+  <cellXfs count="61">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="11" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
@@ -1033,6 +1078,11 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="1" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="2" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="2" applyBorder="1"/>
+    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="3" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
@@ -1045,16 +1095,23 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="9" xfId="2" applyBorder="1"/>
-    <xf numFmtId="0" fontId="2" fillId="2" borderId="14" xfId="2" applyBorder="1"/>
-    <xf numFmtId="6" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="5" fillId="3" borderId="12" xfId="3" applyBorder="1"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="15" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="16" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="17" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="9" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="4"/>
   </cellXfs>
-  <cellStyles count="4">
+  <cellStyles count="5">
     <cellStyle name="Bad" xfId="3" builtinId="27"/>
     <cellStyle name="Currency" xfId="1" builtinId="4"/>
     <cellStyle name="Good" xfId="2" builtinId="26"/>
+    <cellStyle name="Hyperlink" xfId="4" builtinId="8"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
   <dxfs count="0"/>
@@ -2539,13 +2596,13 @@
       <selection activeCell="H15" sqref="H15"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="8.6640625" style="1"/>
-    <col min="2" max="2" width="85.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="8.6328125" style="1"/>
+    <col min="2" max="2" width="85.6328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" s="1" t="s">
         <v>11</v>
       </c>
@@ -2556,11 +2613,11 @@
         <v>10</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" s="50" t="s">
         <v>2</v>
       </c>
-      <c r="B2" s="45"/>
+      <c r="B2" s="50"/>
       <c r="C2" t="s">
         <v>4</v>
       </c>
@@ -2574,7 +2631,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A3" s="1" t="s">
         <v>5</v>
       </c>
@@ -2594,7 +2651,7 @@
         <v>49.222000000000001</v>
       </c>
     </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A4" s="1" t="s">
         <v>6</v>
       </c>
@@ -2614,7 +2671,7 @@
         <v>49.24</v>
       </c>
     </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A5" s="1" t="s">
         <v>20</v>
       </c>
@@ -2634,7 +2691,7 @@
         <v>49.220999999999997</v>
       </c>
     </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A6" s="1" t="s">
         <v>12</v>
       </c>
@@ -2657,7 +2714,7 @@
         <v>49.220999999999997</v>
       </c>
     </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A7" s="1" t="s">
         <v>8</v>
       </c>
@@ -2668,7 +2725,7 @@
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" s="1" t="s">
         <v>22</v>
       </c>
@@ -2696,14 +2753,14 @@
       <selection activeCell="H35" sqref="H35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="29" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="15.33203125" customWidth="1"/>
-    <col min="3" max="3" width="12.1640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.36328125" customWidth="1"/>
+    <col min="3" max="3" width="12.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2711,7 +2768,7 @@
         <v>24</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
@@ -2722,7 +2779,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A3" s="22" t="s">
         <v>25</v>
       </c>
@@ -2733,7 +2790,7 @@
         <v>29</v>
       </c>
     </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A4" s="22"/>
       <c r="B4" s="16">
         <f>1/B3</f>
@@ -2743,7 +2800,7 @@
         <v>98</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" s="22" t="s">
         <v>30</v>
       </c>
@@ -2754,7 +2811,7 @@
         <v>31</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" s="22" t="s">
         <v>36</v>
       </c>
@@ -2765,7 +2822,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="7" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A7" s="22" t="s">
         <v>37</v>
       </c>
@@ -2776,7 +2833,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" s="22" t="s">
         <v>32</v>
       </c>
@@ -2787,7 +2844,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>35</v>
       </c>
@@ -2798,7 +2855,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>38</v>
       </c>
@@ -2809,7 +2866,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A11" s="22" t="s">
         <v>40</v>
       </c>
@@ -2820,7 +2877,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A12" s="22" t="s">
         <v>42</v>
       </c>
@@ -2831,7 +2888,7 @@
         <v>43</v>
       </c>
     </row>
-    <row r="13" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A13" s="22" t="s">
         <v>44</v>
       </c>
@@ -2842,7 +2899,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="14" spans="1:3" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:3" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A14" s="40" t="s">
         <v>46</v>
       </c>
@@ -2853,7 +2910,7 @@
         <v>39</v>
       </c>
     </row>
-    <row r="16" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A16" s="7" t="s">
         <v>97</v>
       </c>
@@ -2868,21 +2925,21 @@
   <dimension ref="A1:M63"/>
   <sheetViews>
     <sheetView topLeftCell="A19" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="B66" sqref="B66"/>
+      <selection activeCell="B23" sqref="B23"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="27" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="34.83203125" customWidth="1"/>
-    <col min="3" max="3" width="15.6640625" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="15.5" bestFit="1" customWidth="1"/>
-    <col min="5" max="5" width="14.83203125" bestFit="1" customWidth="1"/>
-    <col min="6" max="12" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="13" max="13" width="14.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="34.81640625" customWidth="1"/>
+    <col min="3" max="3" width="15.6328125" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="15.453125" bestFit="1" customWidth="1"/>
+    <col min="5" max="5" width="14.81640625" bestFit="1" customWidth="1"/>
+    <col min="6" max="12" width="13.1796875" bestFit="1" customWidth="1"/>
+    <col min="13" max="13" width="14.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" ht="49" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:4" ht="44" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A1" t="s">
         <v>0</v>
       </c>
@@ -2890,7 +2947,7 @@
         <v>99</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="17" t="s">
         <v>26</v>
       </c>
@@ -2904,7 +2961,7 @@
         <v>28</v>
       </c>
     </row>
-    <row r="3" spans="1:4" ht="32" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:4" ht="29" x14ac:dyDescent="0.35">
       <c r="A3" s="20" t="s">
         <v>102</v>
       </c>
@@ -2918,7 +2975,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="4" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A4" s="22" t="s">
         <v>103</v>
       </c>
@@ -2933,7 +2990,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="5" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A5" s="22"/>
       <c r="B5" s="11" t="s">
         <v>109</v>
@@ -2946,7 +3003,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="6" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A6" s="22"/>
       <c r="B6" s="11" t="s">
         <v>107</v>
@@ -2959,7 +3016,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="7" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A7" s="22"/>
       <c r="B7" s="11" t="s">
         <v>114</v>
@@ -2971,7 +3028,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="8" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A8" s="22"/>
       <c r="B8" s="11" t="s">
         <v>108</v>
@@ -2984,7 +3041,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="9" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A9" s="22" t="s">
         <v>113</v>
       </c>
@@ -2997,7 +3054,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="10" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A10" s="22" t="s">
         <v>104</v>
       </c>
@@ -3012,7 +3069,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="11" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A11" s="24" t="s">
         <v>112</v>
       </c>
@@ -3027,7 +3084,7 @@
         <v>106</v>
       </c>
     </row>
-    <row r="12" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A12" s="26" t="s">
         <v>115</v>
       </c>
@@ -3041,7 +3098,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="13" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A13" s="28" t="s">
         <v>118</v>
       </c>
@@ -3056,7 +3113,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="14" spans="1:4" ht="16" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A14" s="28" t="s">
         <v>119</v>
       </c>
@@ -3071,7 +3128,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="15" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A15" s="28" t="s">
         <v>122</v>
       </c>
@@ -3083,7 +3140,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="16" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A16" s="28" t="s">
         <v>123</v>
       </c>
@@ -3096,7 +3153,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A17" s="26" t="s">
         <v>124</v>
       </c>
@@ -3108,7 +3165,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A18" s="38" t="s">
         <v>125</v>
       </c>
@@ -3121,7 +3178,7 @@
         <v>117</v>
       </c>
     </row>
-    <row r="19" spans="1:13" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A19" s="30" t="s">
         <v>126</v>
       </c>
@@ -3135,23 +3192,36 @@
         <v>39</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A20" s="28" t="s">
+        <v>0</v>
+      </c>
+      <c r="B20" t="s">
+        <v>221</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.35">
+      <c r="A21" t="s">
+        <v>222</v>
+      </c>
+      <c r="B21" t="s">
+        <v>224</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>127</v>
       </c>
-      <c r="B22" t="s">
-        <v>132</v>
-      </c>
       <c r="C22" t="s">
-        <v>167</v>
-      </c>
-    </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+        <v>223</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.35">
       <c r="E23" t="s">
-        <v>168</v>
-      </c>
-    </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+        <v>166</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A24" t="s">
         <v>128</v>
       </c>
@@ -3192,9 +3262,9 @@
         <v>10</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A25" t="s">
-        <v>133</v>
+        <v>132</v>
       </c>
       <c r="B25" s="42">
         <v>11807922</v>
@@ -3242,9 +3312,9 @@
         <v>52744050.147983856</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A26" t="s">
-        <v>134</v>
+        <v>133</v>
       </c>
       <c r="B26" s="42">
         <v>17388504</v>
@@ -3292,9 +3362,9 @@
         <v>109714043.08323221</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A27" t="s">
-        <v>135</v>
+        <v>134</v>
       </c>
       <c r="B27" s="42">
         <v>2547995</v>
@@ -3342,9 +3412,9 @@
         <v>10143750.800344583</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A28" t="s">
-        <v>136</v>
+        <v>135</v>
       </c>
       <c r="B28" s="42">
         <v>22972192</v>
@@ -3392,9 +3462,9 @@
         <v>91453943.585316852</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A29" t="s">
-        <v>137</v>
+        <v>136</v>
       </c>
       <c r="B29" s="42">
         <v>6248204</v>
@@ -3442,9 +3512,9 @@
         <v>24874548.15481044</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A30" t="s">
-        <v>138</v>
+        <v>137</v>
       </c>
       <c r="B30" s="42">
         <v>32995221</v>
@@ -3492,9 +3562,9 @@
         <v>131356340.74097335</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A31" t="s">
-        <v>139</v>
+        <v>138</v>
       </c>
       <c r="B31" s="42">
         <v>4186906</v>
@@ -3542,9 +3612,9 @@
         <v>20984238.355974279</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A32" t="s">
-        <v>140</v>
+        <v>139</v>
       </c>
       <c r="B32" s="42">
         <v>807728</v>
@@ -3592,9 +3662,9 @@
         <v>4048229.6184328939</v>
       </c>
     </row>
-    <row r="33" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A33" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="B33" s="42">
         <v>75501</v>
@@ -3642,9 +3712,9 @@
         <v>378401.37326092686</v>
       </c>
     </row>
-    <row r="34" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A34" t="s">
-        <v>141</v>
+        <v>140</v>
       </c>
       <c r="B34" s="42">
         <v>11461600</v>
@@ -3692,9 +3762,9 @@
         <v>51197086.5979748</v>
       </c>
     </row>
-    <row r="35" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A35" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B35" s="42">
         <v>36681585</v>
@@ -3742,9 +3812,9 @@
         <v>231445154.62924495</v>
       </c>
     </row>
-    <row r="36" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A36" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="B36" s="42">
         <v>144155</v>
@@ -3792,9 +3862,9 @@
         <v>573891.39171139395</v>
       </c>
     </row>
-    <row r="37" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A37" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="B37" s="42">
         <v>6595713</v>
@@ -3842,9 +3912,9 @@
         <v>33056871.522694372</v>
       </c>
     </row>
-    <row r="38" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A38" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="B38" s="42">
         <v>1626125</v>
@@ -3892,9 +3962,9 @@
         <v>8149930.9028214812</v>
       </c>
     </row>
-    <row r="39" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A39" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="B39" s="42">
         <v>980551</v>
@@ -3942,9 +4012,9 @@
         <v>4914396.4312045546</v>
       </c>
     </row>
-    <row r="40" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A40" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="B40" s="42">
         <v>123670</v>
@@ -3992,9 +4062,9 @@
         <v>492339.1378235101</v>
       </c>
     </row>
-    <row r="41" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A41" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="B41" s="42">
         <v>718300</v>
@@ -4042,9 +4112,9 @@
         <v>4532166.6054012291</v>
       </c>
     </row>
-    <row r="42" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A42" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="B42" s="42">
         <v>7495642</v>
@@ -4092,9 +4162,9 @@
         <v>29840688.281019572</v>
       </c>
     </row>
-    <row r="43" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A43" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="B43" s="42">
         <v>969104</v>
@@ -4142,9 +4212,9 @@
         <v>4857025.5285712406</v>
       </c>
     </row>
-    <row r="44" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A44" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="B44" s="42">
         <v>29456</v>
@@ -4192,9 +4262,9 @@
         <v>147629.71153724933</v>
       </c>
     </row>
-    <row r="45" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="45" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A45" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="B45" s="42">
         <v>21715</v>
@@ -4242,9 +4312,9 @@
         <v>86448.97208569193</v>
       </c>
     </row>
-    <row r="46" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="46" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A46" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="B46" s="42">
         <v>50244</v>
@@ -4292,9 +4362,9 @@
         <v>251816.5136636867</v>
       </c>
     </row>
-    <row r="47" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A47" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="B47" s="42">
         <v>33067253</v>
@@ -4342,9 +4412,9 @@
         <v>147705993.52604714</v>
       </c>
     </row>
-    <row r="48" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="48" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A48" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B48" s="42">
         <v>411911</v>
@@ -4392,9 +4462,9 @@
         <v>1839938.8512649538</v>
       </c>
     </row>
-    <row r="49" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A49" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B49" s="42">
         <v>585966</v>
@@ -4442,9 +4512,9 @@
         <v>2617413.9775833129</v>
       </c>
     </row>
-    <row r="50" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A50" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B50" s="42">
         <v>326304</v>
@@ -4492,9 +4562,9 @@
         <v>1457546.4285322789</v>
       </c>
     </row>
-    <row r="51" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A51" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B51" s="42">
         <v>178050</v>
@@ -4542,9 +4612,9 @@
         <v>795320.13582478999</v>
       </c>
     </row>
-    <row r="52" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A52" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B52" s="42">
         <v>223100</v>
@@ -4592,9 +4662,9 @@
         <v>1118148.7182224444</v>
       </c>
     </row>
-    <row r="53" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A53" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B53" s="42">
         <v>27883640</v>
@@ -4642,9 +4712,9 @@
         <v>111006770.25132319</v>
       </c>
     </row>
-    <row r="54" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A54" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B54" s="42">
         <v>11065762</v>
@@ -4692,9 +4762,9 @@
         <v>44053591.998384088</v>
       </c>
     </row>
-    <row r="55" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A55" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B55" s="42">
         <v>6015366</v>
@@ -4742,9 +4812,9 @@
         <v>23947603.381037086</v>
       </c>
     </row>
-    <row r="56" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A56" t="s">
-        <v>165</v>
+        <v>164</v>
       </c>
       <c r="B56" s="42">
         <v>1779507</v>
@@ -4792,9 +4862,9 @@
         <v>7084344.9675014224</v>
       </c>
     </row>
-    <row r="57" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A57" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B57" s="42">
         <v>2929758</v>
@@ -4842,9 +4912,9 @@
         <v>11663576.67786473</v>
       </c>
     </row>
-    <row r="58" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:13" x14ac:dyDescent="0.35">
       <c r="A58" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B58" s="42">
         <v>7405996</v>
@@ -4892,9 +4962,9 @@
         <v>33081368.967356648</v>
       </c>
     </row>
-    <row r="60" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D60" t="s">
-        <v>168</v>
+        <v>166</v>
       </c>
       <c r="E60" s="44">
         <f>E24</f>
@@ -4933,7 +5003,7 @@
         <v>10</v>
       </c>
     </row>
-    <row r="61" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="61" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D61" t="s">
         <v>112</v>
       </c>
@@ -4974,9 +5044,9 @@
         <v>1201614609.967025</v>
       </c>
     </row>
-    <row r="62" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="62" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D62" t="s">
-        <v>170</v>
+        <v>168</v>
       </c>
       <c r="E62" s="44">
         <f>LOG(E60)</f>
@@ -5015,9 +5085,9 @@
         <v>1</v>
       </c>
     </row>
-    <row r="63" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="63" spans="1:13" x14ac:dyDescent="0.35">
       <c r="D63" t="s">
-        <v>169</v>
+        <v>167</v>
       </c>
       <c r="E63">
         <f>LOG(E61)</f>
@@ -5064,563 +5134,590 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2E40FBC7-515F-444A-AA65-63C61A66544C}">
-  <dimension ref="A1:D6"/>
+  <dimension ref="A1:F7"/>
   <sheetViews>
     <sheetView zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K12" sqref="K12"/>
+      <selection activeCell="F6" sqref="F6"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
     <col min="1" max="1" width="18" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="8.5" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="9.5" bestFit="1" customWidth="1"/>
-    <col min="4" max="4" width="10.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="8.7265625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="9.81640625" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.81640625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A1" t="s">
+    <row r="1" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A1" s="54" t="s">
+        <v>220</v>
+      </c>
+      <c r="B1" s="50" t="s">
+        <v>219</v>
+      </c>
+      <c r="C1" s="50"/>
+      <c r="D1" s="50"/>
+      <c r="E1" s="50"/>
+      <c r="F1" s="54"/>
+    </row>
+    <row r="2" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A2" s="55" t="s">
         <v>84</v>
       </c>
-      <c r="B1">
+      <c r="B2" s="56">
         <v>50</v>
       </c>
-      <c r="C1">
+      <c r="C2" s="56">
         <v>300</v>
       </c>
-      <c r="D1">
+      <c r="D2" s="57">
         <v>1000</v>
       </c>
     </row>
-    <row r="2" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A3" s="22" t="s">
         <v>17</v>
       </c>
-      <c r="B2">
-        <f>-B1-$B3</f>
+      <c r="B3" s="12">
+        <f>-B2-$B4</f>
         <v>-35.1</v>
       </c>
-      <c r="C2">
-        <f t="shared" ref="C2:D2" si="0">-C1-$B3</f>
+      <c r="C3" s="12">
+        <f t="shared" ref="C3:D3" si="0">-C2-$B4</f>
         <v>-285.10000000000002</v>
       </c>
-      <c r="D2">
+      <c r="D3" s="23">
         <f t="shared" si="0"/>
         <v>-985.1</v>
       </c>
     </row>
-    <row r="3" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A4" s="22" t="s">
+        <v>169</v>
+      </c>
+      <c r="B4" s="58">
+        <v>-14.9</v>
+      </c>
+      <c r="C4" s="58"/>
+      <c r="D4" s="59"/>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A5" s="22" t="s">
+        <v>170</v>
+      </c>
+      <c r="B5" s="12">
+        <v>25.13</v>
+      </c>
+      <c r="C5" s="12" t="s">
         <v>171</v>
       </c>
-      <c r="B3">
-        <v>-14.9</v>
-      </c>
-    </row>
-    <row r="4" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
+      <c r="D5" s="23"/>
+    </row>
+    <row r="6" spans="1:6" x14ac:dyDescent="0.35">
+      <c r="A6" s="22" t="s">
         <v>172</v>
       </c>
-      <c r="B4">
-        <v>25.13</v>
-      </c>
-      <c r="C4" t="s">
+      <c r="B6" s="12">
+        <f>ABS(B3)*$B5</f>
+        <v>882.06299999999999</v>
+      </c>
+      <c r="C6" s="12">
+        <f t="shared" ref="C6:D6" si="1">ABS(C3)*$B5</f>
+        <v>7164.5630000000001</v>
+      </c>
+      <c r="D6" s="23">
+        <f t="shared" si="1"/>
+        <v>24755.562999999998</v>
+      </c>
+    </row>
+    <row r="7" spans="1:6" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A7" s="40" t="s">
         <v>173</v>
       </c>
-    </row>
-    <row r="5" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>174</v>
-      </c>
-      <c r="B5">
-        <f>ABS(B2)*$B4</f>
-        <v>882.06299999999999</v>
-      </c>
-      <c r="C5">
-        <f t="shared" ref="C5:D5" si="1">ABS(C2)*$B4</f>
-        <v>7164.5630000000001</v>
-      </c>
-      <c r="D5">
-        <f t="shared" si="1"/>
-        <v>24755.562999999998</v>
-      </c>
-    </row>
-    <row r="6" spans="1:4" x14ac:dyDescent="0.2">
-      <c r="A6" t="s">
-        <v>175</v>
-      </c>
-      <c r="B6">
-        <f>-B5</f>
+      <c r="B7" s="31">
+        <f>-B6</f>
         <v>-882.06299999999999</v>
       </c>
-      <c r="C6">
-        <f t="shared" ref="C6:D6" si="2">-C5</f>
+      <c r="C7" s="31">
+        <f t="shared" ref="C7:D7" si="2">-C6</f>
         <v>-7164.5630000000001</v>
       </c>
-      <c r="D6">
+      <c r="D7" s="41">
         <f t="shared" si="2"/>
         <v>-24755.562999999998</v>
       </c>
     </row>
   </sheetData>
+  <mergeCells count="2">
+    <mergeCell ref="B1:E1"/>
+    <mergeCell ref="B4:D4"/>
+  </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
 </file>
 
 <file path=xl/worksheets/sheet5.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{9120567B-0376-BC4D-A254-A4551F910A7D}">
-  <dimension ref="A1:I27"/>
+  <dimension ref="A1:I28"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="130" zoomScaleNormal="130" workbookViewId="0">
-      <selection activeCell="K41" sqref="K41"/>
+    <sheetView zoomScale="90" zoomScaleNormal="90" workbookViewId="0">
+      <selection activeCell="B1" sqref="B1"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="10.90625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="2" max="2" width="17" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="33.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="18.90625" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="33.453125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>62</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>225</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>176</v>
+      </c>
+      <c r="B3" t="s">
+        <v>177</v>
+      </c>
+      <c r="C3" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" t="s">
+        <v>175</v>
+      </c>
+      <c r="B5" s="51" t="s">
+        <v>17</v>
+      </c>
+      <c r="C5" s="52"/>
+      <c r="D5" s="52"/>
+      <c r="E5" s="52"/>
+      <c r="F5" s="52"/>
+      <c r="G5" s="52"/>
+      <c r="H5" s="53"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B6" s="22" t="s">
+        <v>179</v>
+      </c>
+      <c r="C6" s="12" t="s">
         <v>180</v>
       </c>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
-        <v>178</v>
-      </c>
-      <c r="B2" t="s">
+      <c r="D6" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E6" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F6" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G6" s="12" t="s">
+        <v>181</v>
+      </c>
+      <c r="H6" s="23"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B7" s="22" t="s">
+        <v>182</v>
+      </c>
+      <c r="C7" s="12" t="s">
+        <v>183</v>
+      </c>
+      <c r="D7" s="12">
+        <v>1</v>
+      </c>
+      <c r="E7" s="12"/>
+      <c r="F7" s="12" t="s">
+        <v>184</v>
+      </c>
+      <c r="G7" s="12" t="s">
+        <v>34</v>
+      </c>
+      <c r="H7" s="23"/>
+    </row>
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B8" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C8" s="12"/>
+      <c r="D8" s="12">
+        <v>20</v>
+      </c>
+      <c r="E8" s="12" t="s">
+        <v>39</v>
+      </c>
+      <c r="F8" s="12"/>
+      <c r="G8" s="12"/>
+      <c r="H8" s="23"/>
+    </row>
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B9" s="22" t="s">
+        <v>185</v>
+      </c>
+      <c r="C9" s="12" t="s">
+        <v>186</v>
+      </c>
+      <c r="D9" s="12">
+        <v>-30320</v>
+      </c>
+      <c r="E9" s="12" t="s">
+        <v>187</v>
+      </c>
+      <c r="F9" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G9" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H9" s="23"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B10" s="22" t="s">
+        <v>190</v>
+      </c>
+      <c r="C10" s="12" t="s">
+        <v>191</v>
+      </c>
+      <c r="D10" s="12">
+        <v>-3.1680000000000001</v>
+      </c>
+      <c r="E10" s="12" t="s">
+        <v>192</v>
+      </c>
+      <c r="F10" s="12" t="s">
+        <v>193</v>
+      </c>
+      <c r="G10" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H10" s="23"/>
+    </row>
+    <row r="11" spans="1:8" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B11" s="40" t="s">
+        <v>194</v>
+      </c>
+      <c r="C11" s="31" t="s">
+        <v>186</v>
+      </c>
+      <c r="D11" s="31">
+        <v>-27933.45</v>
+      </c>
+      <c r="E11" s="31" t="s">
+        <v>195</v>
+      </c>
+      <c r="F11" s="31" t="s">
+        <v>188</v>
+      </c>
+      <c r="G11" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="H11" s="41"/>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B12" s="51" t="s">
+        <v>217</v>
+      </c>
+      <c r="C12" s="52"/>
+      <c r="D12" s="52"/>
+      <c r="E12" s="52"/>
+      <c r="F12" s="52"/>
+      <c r="G12" s="52"/>
+      <c r="H12" s="53"/>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B13" s="22" t="s">
         <v>179</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C13" s="12" t="s">
+        <v>180</v>
+      </c>
+      <c r="D13" s="12" t="s">
+        <v>27</v>
+      </c>
+      <c r="E13" s="12" t="s">
+        <v>28</v>
+      </c>
+      <c r="F13" s="12" t="s">
+        <v>48</v>
+      </c>
+      <c r="G13" s="12" t="s">
         <v>181</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>177</v>
-      </c>
-      <c r="B4" s="46" t="s">
-        <v>17</v>
-      </c>
-      <c r="C4" s="47"/>
-      <c r="D4" s="47"/>
-      <c r="E4" s="47"/>
-      <c r="F4" s="47"/>
-      <c r="G4" s="47"/>
-      <c r="H4" s="48"/>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B5" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="C5" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="D5" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E5" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F5" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G5" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="H5" s="23"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B6" s="22" t="s">
-        <v>185</v>
-      </c>
-      <c r="C6" s="12" t="s">
-        <v>186</v>
-      </c>
-      <c r="D6" s="12">
+      <c r="H13" s="23" t="s">
+        <v>197</v>
+      </c>
+    </row>
+    <row r="14" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B14" s="22" t="s">
+        <v>196</v>
+      </c>
+      <c r="C14" s="12">
         <v>1</v>
       </c>
-      <c r="E6" s="12"/>
-      <c r="F6" s="12" t="s">
-        <v>187</v>
-      </c>
-      <c r="G6" s="12" t="s">
-        <v>34</v>
-      </c>
-      <c r="H6" s="23"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B7" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="C7" s="12"/>
-      <c r="D7" s="12">
+      <c r="D14" s="12">
+        <v>-350734933</v>
+      </c>
+      <c r="E14" s="47" t="s">
+        <v>198</v>
+      </c>
+      <c r="F14" s="12" t="s">
+        <v>199</v>
+      </c>
+      <c r="G14" s="12" t="s">
+        <v>200</v>
+      </c>
+      <c r="H14" s="23">
+        <v>0.66420000000000001</v>
+      </c>
+    </row>
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B15" s="22" t="s">
+        <v>201</v>
+      </c>
+      <c r="C15" s="12"/>
+      <c r="D15" s="12">
         <v>20</v>
       </c>
-      <c r="E7" s="12" t="s">
+      <c r="E15" s="12" t="s">
         <v>39</v>
       </c>
-      <c r="F7" s="12"/>
-      <c r="G7" s="12"/>
-      <c r="H7" s="23"/>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B8" s="22" t="s">
-        <v>188</v>
-      </c>
-      <c r="C8" s="12" t="s">
-        <v>189</v>
-      </c>
-      <c r="D8" s="12">
-        <v>-30320</v>
-      </c>
-      <c r="E8" s="12" t="s">
-        <v>190</v>
-      </c>
-      <c r="F8" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="G8" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="H8" s="23"/>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B9" s="22" t="s">
-        <v>193</v>
-      </c>
-      <c r="C9" s="12" t="s">
-        <v>194</v>
-      </c>
-      <c r="D9" s="12">
-        <v>-3.1680000000000001</v>
-      </c>
-      <c r="E9" s="12" t="s">
-        <v>195</v>
-      </c>
-      <c r="F9" s="12" t="s">
-        <v>196</v>
-      </c>
-      <c r="G9" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="H9" s="23"/>
-    </row>
-    <row r="10" spans="1:8" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B10" s="40" t="s">
-        <v>197</v>
-      </c>
-      <c r="C10" s="31" t="s">
-        <v>189</v>
-      </c>
-      <c r="D10" s="31">
-        <v>-27933.45</v>
-      </c>
-      <c r="E10" s="31" t="s">
-        <v>198</v>
-      </c>
-      <c r="F10" s="31" t="s">
-        <v>191</v>
-      </c>
-      <c r="G10" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="H10" s="41"/>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B11" s="46" t="s">
-        <v>220</v>
-      </c>
-      <c r="C11" s="47"/>
-      <c r="D11" s="47"/>
-      <c r="E11" s="47"/>
-      <c r="F11" s="47"/>
-      <c r="G11" s="47"/>
-      <c r="H11" s="48"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B12" s="22" t="s">
-        <v>182</v>
-      </c>
-      <c r="C12" s="12" t="s">
-        <v>183</v>
-      </c>
-      <c r="D12" s="12" t="s">
-        <v>27</v>
-      </c>
-      <c r="E12" s="12" t="s">
-        <v>28</v>
-      </c>
-      <c r="F12" s="12" t="s">
-        <v>48</v>
-      </c>
-      <c r="G12" s="12" t="s">
-        <v>184</v>
-      </c>
-      <c r="H12" s="23" t="s">
-        <v>200</v>
-      </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B13" s="22" t="s">
-        <v>199</v>
-      </c>
-      <c r="C13" s="12">
-        <v>1</v>
-      </c>
-      <c r="D13" s="12">
-        <v>-350734933</v>
-      </c>
-      <c r="E13" s="51" t="s">
-        <v>201</v>
-      </c>
-      <c r="F13" s="12" t="s">
+      <c r="F15" s="12"/>
+      <c r="G15" s="12"/>
+      <c r="H15" s="23"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B16" s="22" t="s">
         <v>202</v>
-      </c>
-      <c r="G13" s="12" t="s">
-        <v>203</v>
-      </c>
-      <c r="H13" s="23">
-        <v>0.66420000000000001</v>
-      </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B14" s="22" t="s">
-        <v>204</v>
-      </c>
-      <c r="C14" s="12"/>
-      <c r="D14" s="12">
-        <v>20</v>
-      </c>
-      <c r="E14" s="12" t="s">
-        <v>39</v>
-      </c>
-      <c r="F14" s="12"/>
-      <c r="G14" s="12"/>
-      <c r="H14" s="23"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B15" s="22" t="s">
-        <v>205</v>
-      </c>
-      <c r="C15" s="12">
-        <v>1</v>
-      </c>
-      <c r="D15" s="12">
-        <v>-27412351</v>
-      </c>
-      <c r="E15" s="12" t="s">
-        <v>206</v>
-      </c>
-      <c r="F15" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="G15" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="H15" s="23"/>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="B16" s="22" t="s">
-        <v>207</v>
       </c>
       <c r="C16" s="12">
         <v>1</v>
       </c>
       <c r="D16" s="12">
+        <v>-27412351</v>
+      </c>
+      <c r="E16" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="F16" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G16" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H16" s="23"/>
+    </row>
+    <row r="17" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="B17" s="22" t="s">
+        <v>204</v>
+      </c>
+      <c r="C17" s="12">
+        <v>1</v>
+      </c>
+      <c r="D17" s="12">
         <v>-9636868</v>
       </c>
-      <c r="E16" s="12" t="s">
+      <c r="E17" s="12" t="s">
+        <v>203</v>
+      </c>
+      <c r="F17" s="12" t="s">
+        <v>188</v>
+      </c>
+      <c r="G17" s="12" t="s">
+        <v>189</v>
+      </c>
+      <c r="H17" s="23"/>
+    </row>
+    <row r="18" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="B18" s="48" t="s">
+        <v>207</v>
+      </c>
+      <c r="C18" s="31" t="s">
+        <v>205</v>
+      </c>
+      <c r="D18" s="31">
+        <v>0.13100999999999999</v>
+      </c>
+      <c r="E18" s="31" t="s">
         <v>206</v>
       </c>
-      <c r="F16" s="12" t="s">
-        <v>191</v>
-      </c>
-      <c r="G16" s="12" t="s">
-        <v>192</v>
-      </c>
-      <c r="H16" s="23"/>
-    </row>
-    <row r="17" spans="1:9" ht="17" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="B17" s="52" t="s">
+      <c r="F18" s="31" t="s">
+        <v>193</v>
+      </c>
+      <c r="G18" s="31" t="s">
+        <v>189</v>
+      </c>
+      <c r="H18" s="41"/>
+      <c r="I18" s="49" t="s">
+        <v>218</v>
+      </c>
+    </row>
+    <row r="20" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4"/>
+    <row r="21" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A21" s="51" t="s">
+        <v>209</v>
+      </c>
+      <c r="B21" s="52"/>
+      <c r="C21" s="52"/>
+      <c r="D21" s="53"/>
+      <c r="G21" s="51" t="s">
+        <v>214</v>
+      </c>
+      <c r="H21" s="53"/>
+    </row>
+    <row r="22" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A22" s="22" t="s">
+        <v>14</v>
+      </c>
+      <c r="B22" s="12" t="s">
         <v>210</v>
       </c>
-      <c r="C17" s="31" t="s">
+      <c r="C22" s="12" t="s">
         <v>208</v>
       </c>
-      <c r="D17" s="31">
-        <v>0.13100999999999999</v>
-      </c>
-      <c r="E17" s="31" t="s">
-        <v>209</v>
-      </c>
-      <c r="F17" s="31" t="s">
-        <v>196</v>
-      </c>
-      <c r="G17" s="31" t="s">
-        <v>192</v>
-      </c>
-      <c r="H17" s="41"/>
-      <c r="I17" s="53" t="s">
-        <v>221</v>
-      </c>
-    </row>
-    <row r="19" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25"/>
-    <row r="20" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A20" s="46" t="s">
-        <v>212</v>
-      </c>
-      <c r="B20" s="47"/>
-      <c r="C20" s="47"/>
-      <c r="D20" s="48"/>
-      <c r="G20" s="46" t="s">
-        <v>217</v>
-      </c>
-      <c r="H20" s="48"/>
-    </row>
-    <row r="21" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A21" s="22" t="s">
-        <v>14</v>
-      </c>
-      <c r="B21" s="12" t="s">
-        <v>213</v>
-      </c>
-      <c r="C21" s="12" t="s">
-        <v>211</v>
-      </c>
-      <c r="D21" s="23" t="s">
+      <c r="D22" s="23" t="s">
         <v>28</v>
       </c>
-      <c r="G21" s="22" t="s">
-        <v>213</v>
-      </c>
-      <c r="H21" s="23" t="s">
-        <v>211</v>
-      </c>
-    </row>
-    <row r="22" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A22" s="22" t="s">
-        <v>17</v>
-      </c>
-      <c r="B22" s="12" t="s">
-        <v>176</v>
-      </c>
-      <c r="C22" s="12">
-        <v>-1</v>
-      </c>
-      <c r="D22" s="23" t="s">
-        <v>218</v>
-      </c>
       <c r="G22" s="22" t="s">
-        <v>176</v>
-      </c>
-      <c r="H22" s="49">
-        <v>-1</v>
-      </c>
-    </row>
-    <row r="23" spans="1:9" x14ac:dyDescent="0.2">
+        <v>210</v>
+      </c>
+      <c r="H22" s="23" t="s">
+        <v>208</v>
+      </c>
+    </row>
+    <row r="23" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A23" s="22" t="s">
         <v>17</v>
       </c>
       <c r="B23" s="12" t="s">
-        <v>208</v>
+        <v>174</v>
       </c>
       <c r="C23" s="12">
+        <v>-1</v>
+      </c>
+      <c r="D23" s="23" t="s">
+        <v>215</v>
+      </c>
+      <c r="G23" s="22" t="s">
+        <v>174</v>
+      </c>
+      <c r="H23" s="45">
+        <v>-1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A24" s="22" t="s">
+        <v>17</v>
+      </c>
+      <c r="B24" s="12" t="s">
+        <v>205</v>
+      </c>
+      <c r="C24" s="12">
         <v>25.13</v>
       </c>
-      <c r="D23" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="G23" s="22" t="s">
-        <v>214</v>
-      </c>
-      <c r="H23" s="49">
-        <f>(C25/ABS(C$24))*(C$23)</f>
+      <c r="D24" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G24" s="22" t="s">
+        <v>211</v>
+      </c>
+      <c r="H24" s="45">
+        <f>(C26/ABS(C$25))*(C$24)</f>
         <v>17.377632075471695</v>
       </c>
     </row>
-    <row r="24" spans="1:9" x14ac:dyDescent="0.2">
-      <c r="A24" s="22" t="s">
-        <v>15</v>
-      </c>
-      <c r="B24" s="12" t="s">
-        <v>208</v>
-      </c>
-      <c r="C24" s="12">
-        <v>-1.06</v>
-      </c>
-      <c r="D24" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="G24" s="22" t="s">
-        <v>215</v>
-      </c>
-      <c r="H24" s="49">
-        <f>(C26/ABS(C$24))*(C$23)</f>
-        <v>21.052301886792449</v>
-      </c>
-    </row>
-    <row r="25" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:9" x14ac:dyDescent="0.35">
       <c r="A25" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B25" s="12" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="C25" s="12">
-        <v>0.73299999999999998</v>
+        <v>-1.06</v>
       </c>
       <c r="D25" s="23" t="s">
-        <v>219</v>
-      </c>
-      <c r="G25" s="40" t="s">
         <v>216</v>
       </c>
-      <c r="H25" s="50">
-        <f>(C27/ABS(C$24))*(C$23)</f>
-        <v>11.664113207547167</v>
-      </c>
-    </row>
-    <row r="26" spans="1:9" x14ac:dyDescent="0.2">
+      <c r="G25" s="22" t="s">
+        <v>212</v>
+      </c>
+      <c r="H25" s="45">
+        <f>(C27/ABS(C$25))*(C$24)</f>
+        <v>21.052301886792449</v>
+      </c>
+    </row>
+    <row r="26" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
       <c r="A26" s="22" t="s">
         <v>15</v>
       </c>
       <c r="B26" s="12" t="s">
-        <v>215</v>
+        <v>211</v>
       </c>
       <c r="C26" s="12">
+        <v>0.73299999999999998</v>
+      </c>
+      <c r="D26" s="23" t="s">
+        <v>216</v>
+      </c>
+      <c r="G26" s="40" t="s">
+        <v>213</v>
+      </c>
+      <c r="H26" s="46">
+        <f>(C28/ABS(C$25))*(C$24)</f>
+        <v>11.664113207547167</v>
+      </c>
+    </row>
+    <row r="27" spans="1:9" x14ac:dyDescent="0.35">
+      <c r="A27" s="22" t="s">
+        <v>15</v>
+      </c>
+      <c r="B27" s="12" t="s">
+        <v>212</v>
+      </c>
+      <c r="C27" s="12">
         <v>0.88800000000000001</v>
       </c>
-      <c r="D26" s="23" t="s">
-        <v>219</v>
-      </c>
-    </row>
-    <row r="27" spans="1:9" ht="16" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A27" s="40" t="s">
+      <c r="D27" s="23" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="28" spans="1:9" ht="15" thickBot="1" x14ac:dyDescent="0.4">
+      <c r="A28" s="40" t="s">
         <v>15</v>
       </c>
-      <c r="B27" s="31" t="s">
+      <c r="B28" s="31" t="s">
+        <v>213</v>
+      </c>
+      <c r="C28" s="31">
+        <v>0.49199999999999999</v>
+      </c>
+      <c r="D28" s="41" t="s">
         <v>216</v>
-      </c>
-      <c r="C27" s="31">
-        <v>0.49199999999999999</v>
-      </c>
-      <c r="D27" s="41" t="s">
-        <v>219</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="4">
-    <mergeCell ref="B11:H11"/>
-    <mergeCell ref="B4:H4"/>
-    <mergeCell ref="A20:D20"/>
-    <mergeCell ref="G20:H20"/>
+    <mergeCell ref="B12:H12"/>
+    <mergeCell ref="B5:H5"/>
+    <mergeCell ref="A21:D21"/>
+    <mergeCell ref="G21:H21"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
 </worksheet>
@@ -5628,100 +5725,128 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8FC147DE-C2D1-4559-861B-2B8673B56208}">
-  <dimension ref="A1:C11"/>
+  <dimension ref="A1:C15"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="E33" sqref="E33"/>
+      <selection activeCell="B2" sqref="B2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="30.1640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="30.1796875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="33.1796875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
+        <v>226</v>
+      </c>
+      <c r="B1" t="s">
+        <v>231</v>
+      </c>
+    </row>
+    <row r="2" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
         <v>47</v>
       </c>
     </row>
-    <row r="2" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A2" t="s">
+    <row r="3" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
         <v>48</v>
       </c>
-      <c r="B2" t="s">
+      <c r="B3" t="s">
         <v>49</v>
       </c>
-      <c r="C2" t="s">
+      <c r="C3" t="s">
         <v>51</v>
       </c>
     </row>
-    <row r="3" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+    <row r="4" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A4" t="s">
         <v>55</v>
       </c>
-      <c r="B3">
+      <c r="B4">
         <v>164.77</v>
-      </c>
-      <c r="C3">
-        <v>1.395</v>
-      </c>
-    </row>
-    <row r="4" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>54</v>
-      </c>
-      <c r="B4">
-        <v>100</v>
       </c>
       <c r="C4">
         <v>1.395</v>
       </c>
     </row>
-    <row r="5" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
-        <v>53</v>
+        <v>54</v>
       </c>
       <c r="B5">
-        <v>76.53</v>
+        <v>100</v>
       </c>
       <c r="C5">
         <v>1.395</v>
       </c>
     </row>
-    <row r="6" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="6" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A6" t="s">
-        <v>52</v>
+        <v>53</v>
       </c>
       <c r="B6">
-        <v>140</v>
+        <v>76.53</v>
       </c>
       <c r="C6">
         <v>1.395</v>
       </c>
     </row>
-    <row r="8" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
+        <v>52</v>
+      </c>
+      <c r="B7">
+        <v>140</v>
+      </c>
+      <c r="C7">
+        <v>1.395</v>
+      </c>
+    </row>
+    <row r="8" spans="1:3" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
+        <v>230</v>
+      </c>
+      <c r="B8">
+        <f>AVERAGE(B4:B7)</f>
+        <v>120.32499999999999</v>
+      </c>
+    </row>
+    <row r="10" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A10" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="11" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="9" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A9" t="s">
+    <row r="12" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
         <v>57</v>
       </c>
     </row>
-    <row r="10" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A10" t="s">
+    <row r="13" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
+        <v>228</v>
+      </c>
+    </row>
+    <row r="14" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A14" t="s">
         <v>50</v>
       </c>
-      <c r="B10" t="s">
+      <c r="B14" t="s">
         <v>58</v>
       </c>
     </row>
-    <row r="11" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A11" t="s">
+    <row r="15" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A15" t="s">
         <v>59</v>
       </c>
-      <c r="B11" t="s">
+      <c r="B15" t="s">
         <v>60</v>
       </c>
     </row>
@@ -5732,253 +5857,283 @@
 
 <file path=xl/worksheets/sheet7.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{926ACCEB-6613-41C3-AB8E-7E632C9D30FD}">
-  <dimension ref="A1:H15"/>
+  <dimension ref="A1:H19"/>
   <sheetViews>
-    <sheetView zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
-      <selection activeCell="G19" sqref="G19"/>
+    <sheetView topLeftCell="A4" zoomScale="120" zoomScaleNormal="120" workbookViewId="0">
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="4" max="4" width="10.33203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="9.54296875" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="12.1796875" bestFit="1" customWidth="1"/>
+    <col min="4" max="4" width="10.36328125" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A1" s="45" t="s">
+    <row r="1" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A1" t="s">
+        <v>11</v>
+      </c>
+    </row>
+    <row r="2" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A2" t="s">
+        <v>15</v>
+      </c>
+      <c r="B2" s="60" t="s">
+        <v>232</v>
+      </c>
+    </row>
+    <row r="3" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A3" t="s">
+        <v>17</v>
+      </c>
+      <c r="B3" s="60" t="s">
+        <v>233</v>
+      </c>
+    </row>
+    <row r="4" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="B4" s="60"/>
+    </row>
+    <row r="5" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A5" s="50" t="s">
         <v>61</v>
       </c>
-      <c r="B1" s="45"/>
-      <c r="C1" s="45"/>
-      <c r="D1" s="45"/>
-      <c r="E1" s="45"/>
-      <c r="F1" s="45"/>
-      <c r="G1" s="45"/>
-    </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A2" s="45" t="s">
+      <c r="B5" s="50"/>
+      <c r="C5" s="50"/>
+      <c r="D5" s="50"/>
+      <c r="E5" s="50"/>
+      <c r="F5" s="50"/>
+      <c r="G5" s="50"/>
+    </row>
+    <row r="6" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A6" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="B2" s="45"/>
-      <c r="C2" s="45"/>
-      <c r="D2" s="45"/>
-      <c r="E2" s="45"/>
-      <c r="F2" s="45"/>
-      <c r="G2" s="45"/>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A3" t="s">
+      <c r="B6" s="50"/>
+      <c r="C6" s="50"/>
+      <c r="D6" s="50"/>
+      <c r="E6" s="50"/>
+      <c r="F6" s="50"/>
+      <c r="G6" s="50"/>
+    </row>
+    <row r="7" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A7" t="s">
         <v>63</v>
       </c>
-      <c r="B3">
+      <c r="B7">
         <v>1580</v>
-      </c>
-      <c r="C3" t="s">
-        <v>67</v>
-      </c>
-      <c r="D3" s="3">
-        <f>B3*1000/(24*3600)</f>
-        <v>18.287037037037038</v>
-      </c>
-      <c r="E3" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F3" s="5">
-        <f>B3*1000/24</f>
-        <v>65833.333333333328</v>
-      </c>
-      <c r="G3" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A4" t="s">
-        <v>64</v>
-      </c>
-      <c r="B4">
-        <v>255</v>
-      </c>
-      <c r="C4" t="s">
-        <v>67</v>
-      </c>
-      <c r="D4" s="3">
-        <f>B4*1000/(24*3600)</f>
-        <v>2.9513888888888888</v>
-      </c>
-      <c r="E4" s="4" t="s">
-        <v>72</v>
-      </c>
-      <c r="F4" s="5">
-        <f>B4*1000/24</f>
-        <v>10625</v>
-      </c>
-      <c r="G4" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A5" t="s">
-        <v>65</v>
-      </c>
-      <c r="B5">
-        <v>14.9</v>
-      </c>
-      <c r="C5" t="s">
-        <v>66</v>
-      </c>
-      <c r="D5" s="2" t="s">
-        <v>95</v>
-      </c>
-      <c r="E5" t="s">
-        <v>96</v>
-      </c>
-      <c r="F5" s="2"/>
-      <c r="H5" s="2"/>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A6" s="45" t="s">
-        <v>68</v>
-      </c>
-      <c r="B6" s="45"/>
-      <c r="C6" s="45"/>
-      <c r="D6" s="45"/>
-      <c r="E6" s="45"/>
-      <c r="F6" s="45"/>
-      <c r="G6" s="45"/>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A7" t="s">
-        <v>69</v>
-      </c>
-      <c r="B7">
-        <v>176</v>
       </c>
       <c r="C7" t="s">
         <v>67</v>
       </c>
       <c r="D7" s="3">
         <f>B7*1000/(24*3600)</f>
-        <v>2.0370370370370372</v>
+        <v>18.287037037037038</v>
       </c>
       <c r="E7" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F7" s="5">
         <f>B7*1000/24</f>
-        <v>7333.333333333333</v>
+        <v>65833.333333333328</v>
       </c>
       <c r="G7" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
-        <v>70</v>
+        <v>64</v>
       </c>
       <c r="B8">
-        <v>213</v>
+        <v>255</v>
       </c>
       <c r="C8" t="s">
         <v>67</v>
       </c>
       <c r="D8" s="3">
-        <f t="shared" ref="D8:D9" si="0">B8*1000/(24*3600)</f>
-        <v>2.4652777777777777</v>
+        <f>B8*1000/(24*3600)</f>
+        <v>2.9513888888888888</v>
       </c>
       <c r="E8" s="4" t="s">
         <v>72</v>
       </c>
       <c r="F8" s="5">
-        <f t="shared" ref="F8:F9" si="1">B8*1000/24</f>
-        <v>8875</v>
+        <f>B8*1000/24</f>
+        <v>10625</v>
       </c>
       <c r="G8" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:8" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
+        <v>65</v>
+      </c>
+      <c r="B9">
+        <v>14.9</v>
+      </c>
+      <c r="C9" t="s">
+        <v>66</v>
+      </c>
+      <c r="D9" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="E9" t="s">
+        <v>96</v>
+      </c>
+      <c r="F9" s="2"/>
+      <c r="H9" s="2"/>
+    </row>
+    <row r="10" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A10" s="50" t="s">
+        <v>68</v>
+      </c>
+      <c r="B10" s="50"/>
+      <c r="C10" s="50"/>
+      <c r="D10" s="50"/>
+      <c r="E10" s="50"/>
+      <c r="F10" s="50"/>
+      <c r="G10" s="50"/>
+    </row>
+    <row r="11" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A11" t="s">
+        <v>69</v>
+      </c>
+      <c r="B11">
+        <v>176</v>
+      </c>
+      <c r="C11" t="s">
+        <v>67</v>
+      </c>
+      <c r="D11" s="3">
+        <f>B11*1000/(24*3600)</f>
+        <v>2.0370370370370372</v>
+      </c>
+      <c r="E11" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F11" s="5">
+        <f>B11*1000/24</f>
+        <v>7333.333333333333</v>
+      </c>
+      <c r="G11" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="12" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A12" t="s">
+        <v>70</v>
+      </c>
+      <c r="B12">
+        <v>213</v>
+      </c>
+      <c r="C12" t="s">
+        <v>67</v>
+      </c>
+      <c r="D12" s="3">
+        <f t="shared" ref="D12:D13" si="0">B12*1000/(24*3600)</f>
+        <v>2.4652777777777777</v>
+      </c>
+      <c r="E12" s="4" t="s">
+        <v>72</v>
+      </c>
+      <c r="F12" s="5">
+        <f t="shared" ref="F12:F13" si="1">B12*1000/24</f>
+        <v>8875</v>
+      </c>
+      <c r="G12" t="s">
+        <v>75</v>
+      </c>
+    </row>
+    <row r="13" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A13" t="s">
         <v>71</v>
       </c>
-      <c r="B9">
+      <c r="B13">
         <v>118</v>
       </c>
-      <c r="C9" t="s">
+      <c r="C13" t="s">
         <v>67</v>
       </c>
-      <c r="D9" s="3">
+      <c r="D13" s="3">
         <f t="shared" si="0"/>
         <v>1.3657407407407407</v>
       </c>
-      <c r="E9" s="4" t="s">
+      <c r="E13" s="4" t="s">
         <v>72</v>
       </c>
-      <c r="F9" s="5">
+      <c r="F13" s="5">
         <f t="shared" si="1"/>
         <v>4916.666666666667</v>
       </c>
-      <c r="G9" t="s">
+      <c r="G13" t="s">
         <v>75</v>
       </c>
     </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A11" s="45" t="s">
+    <row r="15" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A15" s="50" t="s">
         <v>17</v>
       </c>
-      <c r="B11" s="45"/>
-      <c r="C11" s="45"/>
-      <c r="D11" s="45"/>
-      <c r="E11" s="45"/>
-      <c r="F11" s="45"/>
-      <c r="G11" s="45"/>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A12" s="45" t="s">
+      <c r="B15" s="50"/>
+      <c r="C15" s="50"/>
+      <c r="D15" s="50"/>
+      <c r="E15" s="50"/>
+      <c r="F15" s="50"/>
+      <c r="G15" s="50"/>
+    </row>
+    <row r="16" spans="1:8" x14ac:dyDescent="0.35">
+      <c r="A16" s="50" t="s">
         <v>62</v>
       </c>
-      <c r="B12" s="45"/>
-      <c r="C12" s="45"/>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A13" t="s">
+      <c r="B16" s="50"/>
+      <c r="C16" s="50"/>
+    </row>
+    <row r="17" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A17" t="s">
         <v>65</v>
       </c>
-      <c r="B13">
+      <c r="B17">
         <v>39.799999999999997</v>
       </c>
-      <c r="C13" t="s">
+      <c r="C17" t="s">
         <v>74</v>
       </c>
     </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A14" s="45" t="s">
+    <row r="18" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A18" s="50" t="s">
         <v>68</v>
       </c>
-      <c r="B14" s="45"/>
-      <c r="C14" s="45"/>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.2">
-      <c r="A15" t="s">
+      <c r="B18" s="50"/>
+      <c r="C18" s="50"/>
+    </row>
+    <row r="19" spans="1:3" x14ac:dyDescent="0.35">
+      <c r="A19" t="s">
         <v>64</v>
       </c>
-      <c r="B15" s="6">
-        <f>1/B13</f>
+      <c r="B19" s="6">
+        <f>1/B17</f>
         <v>2.5125628140703519E-2</v>
       </c>
-      <c r="C15" t="s">
+      <c r="C19" t="s">
         <v>76</v>
       </c>
     </row>
   </sheetData>
   <mergeCells count="6">
-    <mergeCell ref="A12:C12"/>
-    <mergeCell ref="A14:C14"/>
-    <mergeCell ref="A2:G2"/>
+    <mergeCell ref="A16:C16"/>
+    <mergeCell ref="A18:C18"/>
     <mergeCell ref="A6:G6"/>
-    <mergeCell ref="A1:G1"/>
-    <mergeCell ref="A11:G11"/>
+    <mergeCell ref="A10:G10"/>
+    <mergeCell ref="A5:G5"/>
+    <mergeCell ref="A15:G15"/>
   </mergeCells>
+  <hyperlinks>
+    <hyperlink ref="B2" r:id="rId1" xr:uid="{D47EE4A2-649A-42B4-8738-DF2E48262124}"/>
+    <hyperlink ref="B3" r:id="rId2" xr:uid="{49708E60-D8BD-48F2-8030-EEB685223FB9}"/>
+  </hyperlinks>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup orientation="portrait" r:id="rId1"/>
+  <pageSetup orientation="portrait" r:id="rId3"/>
 </worksheet>
 </file>
 
@@ -5990,13 +6145,13 @@
       <selection activeCell="A35" sqref="A35"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="32.83203125" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="32.81640625" bestFit="1" customWidth="1"/>
     <col min="2" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -6007,7 +6162,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>0.5</v>
       </c>
@@ -6015,7 +6170,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -6026,7 +6181,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -6037,7 +6192,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -6048,12 +6203,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -6070,7 +6225,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -6087,7 +6242,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -6104,7 +6259,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -6121,7 +6276,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -6138,7 +6293,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -6155,17 +6310,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>89</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -6179,12 +6334,12 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>84</v>
       </c>
     </row>
-    <row r="19" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -6198,7 +6353,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -6212,12 +6367,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:4" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -6240,18 +6395,18 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{A8827ECA-5F74-4389-B5A8-A15818A92C9F}">
   <dimension ref="A1:E42"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="B50" sqref="B50"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="G8" sqref="G8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultColWidth="8.83203125" defaultRowHeight="15" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultColWidth="8.81640625" defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
   <cols>
-    <col min="1" max="1" width="31.83203125" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="16.6640625" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="31.81640625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="16.6328125" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="9" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A1" t="s">
         <v>77</v>
       </c>
@@ -6262,7 +6417,7 @@
         <v>78</v>
       </c>
     </row>
-    <row r="2" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:5" x14ac:dyDescent="0.35">
       <c r="B2">
         <v>0</v>
       </c>
@@ -6270,7 +6425,7 @@
         <v>79</v>
       </c>
     </row>
-    <row r="3" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A3" t="s">
         <v>69</v>
       </c>
@@ -6281,7 +6436,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="4" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A4" t="s">
         <v>70</v>
       </c>
@@ -6292,7 +6447,7 @@
         <v>81</v>
       </c>
     </row>
-    <row r="5" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="5" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A5" t="s">
         <v>71</v>
       </c>
@@ -6303,12 +6458,12 @@
         <v>81</v>
       </c>
     </row>
-    <row r="7" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="7" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A7" t="s">
         <v>80</v>
       </c>
     </row>
-    <row r="8" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A8" t="s">
         <v>14</v>
       </c>
@@ -6325,7 +6480,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="9" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A9" t="s">
         <v>84</v>
       </c>
@@ -6342,7 +6497,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="10" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A10" t="s">
         <v>17</v>
       </c>
@@ -6359,7 +6514,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="11" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A11" t="s">
         <v>15</v>
       </c>
@@ -6376,7 +6531,7 @@
         <v>64</v>
       </c>
     </row>
-    <row r="12" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A12" t="s">
         <v>87</v>
       </c>
@@ -6393,7 +6548,7 @@
         <v>63</v>
       </c>
     </row>
-    <row r="13" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A13" t="s">
         <v>16</v>
       </c>
@@ -6410,17 +6565,17 @@
         <v>64</v>
       </c>
     </row>
-    <row r="15" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A15" t="s">
         <v>92</v>
       </c>
     </row>
-    <row r="16" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A16" t="s">
         <v>90</v>
       </c>
     </row>
-    <row r="17" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A17" t="s">
         <v>14</v>
       </c>
@@ -6434,7 +6589,7 @@
         <v>85</v>
       </c>
     </row>
-    <row r="18" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A18" t="s">
         <v>84</v>
       </c>
@@ -6448,7 +6603,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="19" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A19" t="s">
         <v>17</v>
       </c>
@@ -6462,7 +6617,7 @@
         <v>86</v>
       </c>
     </row>
-    <row r="20" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A20" t="s">
         <v>15</v>
       </c>
@@ -6476,12 +6631,12 @@
         <v>64</v>
       </c>
     </row>
-    <row r="21" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A21" t="s">
         <v>87</v>
       </c>
     </row>
-    <row r="22" spans="1:5" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:5" x14ac:dyDescent="0.35">
       <c r="A22" t="s">
         <v>16</v>
       </c>
@@ -6498,7 +6653,7 @@
         <v>93</v>
       </c>
     </row>
-    <row r="42" spans="5:5" x14ac:dyDescent="0.2">
+    <row r="42" spans="5:5" x14ac:dyDescent="0.35">
       <c r="E42" t="s">
         <v>94</v>
       </c>

</xml_diff>